<commit_message>
Updated sheets based on Davide's comments
Updated:
templates\template_input.xlsx
and
applications\demo\data\national\demo_input.xlsx
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A2F1B839-CF8D-7848-983D-22BA07ADD3F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="961" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21135" windowWidth="19200" windowHeight="11760" tabRatio="961"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -74,7 +68,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$39</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$31</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,12 +78,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,12 +136,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="216">
   <si>
     <t>year</t>
   </si>
@@ -565,12 +559,6 @@
     <t>Total WRA</t>
   </si>
   <si>
-    <t>Percentage of deaths in baseline year attributable to cause</t>
-  </si>
-  <si>
-    <t>Percentage of children in each category in baseline year</t>
-  </si>
-  <si>
     <t>Wasting (weight-for-height)</t>
   </si>
   <si>
@@ -601,9 +589,6 @@
     <t>SAM   (WHZ-score &lt; -3)</t>
   </si>
   <si>
-    <t>Percentage of births in category</t>
-  </si>
-  <si>
     <t>Birth age and order</t>
   </si>
   <si>
@@ -637,9 +622,6 @@
     <t>Percentage of anaemia that is iron deficient</t>
   </si>
   <si>
-    <t>Percentage of population in each category in baseline year</t>
-  </si>
-  <si>
     <t>Birth outcome distribution</t>
   </si>
   <si>
@@ -788,9 +770,6 @@
   </si>
   <si>
     <t>saturation coverage of target population</t>
-  </si>
-  <si>
-    <t>baseline coverage</t>
   </si>
   <si>
     <t>Unit costs by delivery modality and target population</t>
@@ -853,7 +832,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1836,7 +1815,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2027,6 +2006,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -2753,8 +2735,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 2" xfId="725"/>
+    <cellStyle name="Normal 3" xfId="726"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -2813,7 +2795,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2870,7 +2852,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2927,7 +2909,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2984,7 +2966,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3041,7 +3023,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3098,7 +3080,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3155,7 +3137,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3212,7 +3194,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3269,7 +3251,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3326,7 +3308,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3383,7 +3365,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3440,7 +3422,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3497,7 +3479,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3554,7 +3536,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3611,7 +3593,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3668,7 +3650,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3725,7 +3707,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3782,7 +3764,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3831,7 +3813,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4194,70 +4176,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B2" s="62"/>
       <c r="C2" s="62"/>
     </row>
-    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C3" s="96">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C4" s="97">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="62"/>
       <c r="C5" s="62"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>117</v>
       </c>
@@ -4265,7 +4247,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>118</v>
       </c>
@@ -4273,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>116</v>
       </c>
@@ -4281,7 +4263,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4289,7 +4271,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4297,7 +4279,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4305,17 +4287,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
         <v>105</v>
       </c>
@@ -4323,7 +4305,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>106</v>
       </c>
@@ -4331,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>107</v>
       </c>
@@ -4339,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>108</v>
       </c>
@@ -4347,7 +4329,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
         <v>109</v>
       </c>
@@ -4356,15 +4338,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>112</v>
       </c>
@@ -4372,7 +4354,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>113</v>
       </c>
@@ -4380,7 +4362,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="27" t="s">
         <v>114</v>
       </c>
@@ -4388,7 +4370,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>115</v>
       </c>
@@ -4396,20 +4378,20 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="64" t="s">
         <v>103</v>
       </c>
@@ -4417,7 +4399,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19" t="s">
         <v>102</v>
       </c>
@@ -4427,7 +4409,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="19" t="s">
         <v>101</v>
       </c>
@@ -4437,15 +4419,15 @@
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C32" s="25">
         <v>4.01</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
         <v>100</v>
       </c>
@@ -4453,7 +4435,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="64" t="s">
         <v>104</v>
       </c>
@@ -4461,16 +4443,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="20"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D36" s="20"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="19" t="s">
         <v>9</v>
       </c>
@@ -4479,7 +4461,7 @@
       </c>
       <c r="D37" s="20"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
         <v>11</v>
       </c>
@@ -4488,7 +4470,7 @@
       </c>
       <c r="D38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>12</v>
       </c>
@@ -4498,7 +4480,7 @@
       <c r="D39" s="20"/>
       <c r="E39" s="21"/>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="19" t="s">
         <v>26</v>
       </c>
@@ -4509,62 +4491,62 @@
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="20"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
         <v>73</v>
       </c>
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C43" s="7">
         <v>1.66</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C44" s="7">
         <v>1.66</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C45" s="7">
         <v>5.64</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C46" s="7">
         <v>5.43</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C47" s="7">
         <v>1.91</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="9" t="s">
         <v>122</v>
       </c>
@@ -4572,31 +4554,31 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C51" s="24">
         <v>0.42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="19" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C52" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="19" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C53" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
     </row>
   </sheetData>
@@ -4606,40 +4588,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56" style="74" customWidth="1"/>
     <col min="2" max="2" width="20" style="57" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="56" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="56" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="56"/>
+    <col min="3" max="3" width="20.42578125" style="56" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="56" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="83" t="s">
-        <v>201</v>
+      <c r="B1" s="98" t="str">
+        <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
+        <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
         <v>29</v>
       </c>
@@ -4653,7 +4636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
         <v>97</v>
       </c>
@@ -4668,7 +4651,7 @@
       </c>
       <c r="E3" s="65"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="74" t="s">
         <v>61</v>
       </c>
@@ -4684,7 +4667,7 @@
       </c>
       <c r="E4" s="65"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
         <v>68</v>
       </c>
@@ -4700,7 +4683,7 @@
       </c>
       <c r="E5" s="80"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
         <v>63</v>
       </c>
@@ -4715,9 +4698,9 @@
       </c>
       <c r="E6" s="79"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="93" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B7" s="75">
         <v>0</v>
@@ -4729,9 +4712,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B8" s="75">
         <v>0</v>
@@ -4743,9 +4726,9 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B9" s="75">
         <v>0</v>
@@ -4757,9 +4740,9 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="93" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B10" s="75">
         <v>0</v>
@@ -4771,9 +4754,9 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B11" s="75">
         <v>0</v>
@@ -4785,9 +4768,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B12" s="75">
         <v>0</v>
@@ -4799,7 +4782,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
         <v>57</v>
       </c>
@@ -4814,7 +4797,7 @@
       </c>
       <c r="E13" s="65"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
         <v>47</v>
       </c>
@@ -4829,9 +4812,9 @@
       </c>
       <c r="E14" s="65"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="74" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B15" s="75">
         <v>0</v>
@@ -4844,9 +4827,9 @@
         <v>10.49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="74" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B16" s="75">
         <v>0</v>
@@ -4859,7 +4842,7 @@
       </c>
       <c r="E16" s="65"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="74" t="s">
         <v>34</v>
       </c>
@@ -4874,7 +4857,7 @@
       </c>
       <c r="E17" s="65"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
         <v>99</v>
       </c>
@@ -4889,7 +4872,7 @@
       </c>
       <c r="E18" s="65"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
         <v>98</v>
       </c>
@@ -4904,9 +4887,9 @@
       </c>
       <c r="E19" s="78"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="74" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B20" s="75">
         <v>0.1</v>
@@ -4919,7 +4902,7 @@
       </c>
       <c r="E20" s="65"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
         <v>59</v>
       </c>
@@ -4934,7 +4917,7 @@
       </c>
       <c r="E21" s="65"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
         <v>95</v>
       </c>
@@ -4948,7 +4931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
         <v>58</v>
       </c>
@@ -4962,7 +4945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
         <v>67</v>
       </c>
@@ -4977,7 +4960,7 @@
         <v>10.015195269175592</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
         <v>28</v>
       </c>
@@ -4991,7 +4974,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
         <v>94</v>
       </c>
@@ -5005,7 +4988,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="74" t="s">
         <v>93</v>
       </c>
@@ -5019,7 +5002,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="74" t="s">
         <v>92</v>
       </c>
@@ -5033,7 +5016,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="74" t="s">
         <v>90</v>
       </c>
@@ -5047,7 +5030,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="74" t="s">
         <v>91</v>
       </c>
@@ -5062,7 +5045,7 @@
       </c>
       <c r="F30" s="56"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="74" t="s">
         <v>96</v>
       </c>
@@ -5076,7 +5059,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="74" t="s">
         <v>60</v>
       </c>
@@ -5090,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="57"/>
     </row>
   </sheetData>
@@ -5103,7 +5086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5113,32 +5096,32 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="84" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="84"/>
+    <col min="1" max="1" width="18.7109375" style="84" customWidth="1"/>
+    <col min="2" max="16384" width="10.85546875" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B1" s="88" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C1" s="88" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D1" s="88" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>32</v>
@@ -5154,7 +5137,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="86"/>
       <c r="B3" s="86" t="s">
         <v>1</v>
@@ -5171,7 +5154,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="86"/>
       <c r="B4" s="86" t="s">
         <v>2</v>
@@ -5188,7 +5171,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="86" t="s">
         <v>3</v>
@@ -5205,7 +5188,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
       <c r="B6" s="86" t="s">
         <v>4</v>
@@ -5222,7 +5205,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="85"/>
     </row>
   </sheetData>
@@ -5231,7 +5214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5241,83 +5224,83 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" style="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="56" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="56" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="56"/>
+    <col min="2" max="2" width="47.85546875" style="56" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="56" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B2" s="70" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="70"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B3" s="70" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="70"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="74" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="70"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5" s="70"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
     </row>
   </sheetData>
@@ -5328,7 +5311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5338,85 +5321,85 @@
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="56" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="56"/>
+    <col min="1" max="1" width="30.140625" style="56" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="70" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="70" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="70" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="70" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="70" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="70" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="70"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="70"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="70"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="70"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="70"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="70"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="70"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="70"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="70"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="70"/>
     </row>
   </sheetData>
@@ -5426,7 +5409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5436,9 +5419,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5458,7 +5441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -5483,7 +5466,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -5508,7 +5491,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5540,7 +5523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5550,19 +5533,19 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5609,7 +5592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5660,9 +5643,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="54">
         <v>1</v>
@@ -5704,9 +5687,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="54">
         <v>0</v>
@@ -5750,9 +5733,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C5" s="54">
         <v>0</v>
@@ -5797,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="52" t="s">
         <v>95</v>
       </c>
@@ -5841,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
@@ -5887,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>67</v>
       </c>
@@ -5935,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
@@ -5979,7 +5962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="52" t="s">
         <v>96</v>
       </c>
@@ -6023,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>60</v>
       </c>
@@ -6067,10 +6050,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="52"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -6121,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="14" t="s">
         <v>97</v>
@@ -6166,10 +6149,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C15" s="55">
         <v>0</v>
@@ -6215,10 +6198,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C16" s="55">
         <v>0</v>
@@ -6264,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="52" t="s">
         <v>57</v>
       </c>
@@ -6312,7 +6295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>99</v>
       </c>
@@ -6356,7 +6339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>98</v>
       </c>
@@ -6400,7 +6383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="52" t="s">
         <v>59</v>
       </c>
@@ -6448,10 +6431,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="52"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="91" t="s">
         <v>37</v>
       </c>
@@ -6498,9 +6481,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="93" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C23" s="55">
         <v>0</v>
@@ -6546,9 +6529,9 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="93" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C24" s="55">
         <v>0</v>
@@ -6594,9 +6577,9 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="93" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C25" s="55">
         <v>0</v>
@@ -6642,9 +6625,9 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="93" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C26" s="55">
         <v>0</v>
@@ -6687,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="14"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -6697,7 +6680,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
@@ -6755,7 +6738,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="14" t="s">
         <v>64</v>
       </c>
@@ -6810,7 +6793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>62</v>
       </c>
@@ -6865,7 +6848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>47</v>
       </c>
@@ -6909,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
         <v>34</v>
       </c>
@@ -6966,7 +6949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="52" t="s">
         <v>94</v>
       </c>
@@ -7010,7 +6993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="52" t="s">
         <v>93</v>
@@ -7055,7 +7038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="52" t="s">
         <v>92</v>
       </c>
@@ -7099,7 +7082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="52" t="s">
         <v>90</v>
       </c>
@@ -7143,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="52" t="s">
         <v>91</v>
       </c>
@@ -7187,7 +7170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="52"/>
     </row>
   </sheetData>
@@ -7200,45 +7183,45 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="56" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="56"/>
-    <col min="5" max="5" width="17.5" style="56" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="56"/>
+    <col min="1" max="1" width="33.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="56" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="56"/>
+    <col min="5" max="5" width="17.42578125" style="56" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E1" s="61" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B2" s="59">
         <v>0.9</v>
@@ -7254,9 +7237,9 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B3" s="59">
         <v>1</v>
@@ -7272,9 +7255,9 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B4" s="59">
         <v>1</v>
@@ -7290,9 +7273,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B5" s="59">
         <v>1</v>
@@ -7308,9 +7291,9 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="60" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" s="59">
         <v>1</v>
@@ -7326,9 +7309,9 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B7" s="59">
         <v>0.93</v>
@@ -7344,9 +7327,9 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="60" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B8" s="59">
         <v>0.5</v>
@@ -7362,9 +7345,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B9" s="59">
         <v>0.5</v>
@@ -7380,9 +7363,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B10" s="59">
         <v>0.98</v>
@@ -7398,7 +7381,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="57"/>
     </row>
   </sheetData>
@@ -7409,7 +7392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -7419,14 +7402,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.85546875" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
@@ -7452,13 +7435,13 @@
         <v>125</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J1" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7494,7 +7477,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="2">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7530,7 +7513,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -7566,7 +7549,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -7602,7 +7585,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <f t="shared" si="2"/>
         <v>2021</v>
@@ -7638,7 +7621,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <f t="shared" si="2"/>
         <v>2022</v>
@@ -7674,7 +7657,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <f t="shared" si="2"/>
         <v>2023</v>
@@ -7710,7 +7693,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <f t="shared" si="2"/>
         <v>2024</v>
@@ -7746,7 +7729,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <f t="shared" si="2"/>
         <v>2025</v>
@@ -7782,7 +7765,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <f t="shared" si="2"/>
         <v>2026</v>
@@ -7818,7 +7801,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <f t="shared" si="2"/>
         <v>2027</v>
@@ -7854,7 +7837,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <f t="shared" si="2"/>
         <v>2028</v>
@@ -7890,7 +7873,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <f t="shared" si="2"/>
         <v>2029</v>
@@ -7926,7 +7909,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <f t="shared" si="2"/>
         <v>2030</v>
@@ -7962,7 +7945,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -7986,7 +7969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8010,7 +7993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8034,7 +8017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8058,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8082,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8106,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8130,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8154,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8178,7 +8161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8202,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8226,7 +8209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8250,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8274,7 +8257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8298,7 +8281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8322,7 +8305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8346,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8370,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8394,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8418,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8442,7 +8425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8466,7 +8449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8490,7 +8473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8514,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8538,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8574,25 +8557,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
-        <v>126</v>
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="str">
+        <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
+        <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
@@ -8613,7 +8597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>74</v>
       </c>
@@ -8636,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8659,7 +8643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8682,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8705,7 +8689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8728,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8751,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8774,7 +8758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8797,7 +8781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>72</v>
       </c>
@@ -8820,7 +8804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8843,7 +8827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8866,7 +8850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8889,7 +8873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8912,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8935,7 +8919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8958,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8981,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -9004,7 +8988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -9027,7 +9011,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -9050,7 +9034,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -9073,7 +9057,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -9096,7 +9080,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -9119,7 +9103,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -9142,7 +9126,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -9165,7 +9149,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -9188,7 +9172,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -9219,25 +9203,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="38" t="s">
-        <v>150</v>
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="str">
+        <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
+        <v>Percentage of population in each category in baseline year (2017)</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -9258,12 +9243,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="C2" s="49">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9286,36 +9271,36 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="39">
         <v>8.7000000000000008E-2</v>
@@ -9333,10 +9318,10 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="39">
         <v>4.5999999999999999E-2</v>
@@ -9354,7 +9339,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -9362,7 +9347,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -9370,12 +9355,12 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="49">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9398,34 +9383,34 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="49">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="39">
         <v>5.3999999999999999E-2</v>
@@ -9443,9 +9428,9 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="39">
         <v>0.04</v>
@@ -9463,7 +9448,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9477,7 +9462,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
@@ -9521,9 +9506,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C14" s="50">
         <v>0.1</v>
@@ -9565,7 +9550,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>69</v>
       </c>
@@ -9622,14 +9607,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9644,25 +9629,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="38" t="s">
-        <v>127</v>
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="str">
+        <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
+        <v>Percentage of children in each category in baseline year (2017)</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -9683,12 +9669,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C2" s="39">
         <v>0.84</v>
@@ -9706,9 +9692,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="65" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C3" s="39">
         <v>9.1999999999999998E-2</v>
@@ -9726,9 +9712,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="65" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C4" s="39">
         <v>5.8000000000000003E-2</v>
@@ -9746,9 +9732,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="65" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C5" s="49">
         <f>1-SUM(C2:C4)</f>
@@ -9777,7 +9763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9787,18 +9773,18 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9828,12 +9814,12 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>163</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9845,15 +9831,15 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9865,15 +9851,15 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9885,7 +9871,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9899,9 +9885,9 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9913,12 +9899,12 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9930,9 +9916,9 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="53" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9944,12 +9930,12 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9961,9 +9947,9 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9982,38 +9968,39 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="15"/>
+    <col min="1" max="1" width="37.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="44" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="44" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>180</v>
+      </c>
+      <c r="C1" s="43" t="str">
+        <f>"Percentage of births in category in baseline year ("&amp;start_year&amp;")"</f>
+        <v>Percentage of births in category in baseline year (2017)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>76</v>
@@ -10022,7 +10009,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="41" t="s">
         <v>77</v>
       </c>
@@ -10030,7 +10017,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="41" t="s">
         <v>78</v>
       </c>
@@ -10038,7 +10025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="41" t="s">
         <v>79</v>
       </c>
@@ -10046,7 +10033,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
         <v>80</v>
       </c>
@@ -10054,7 +10041,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="41" t="s">
         <v>81</v>
       </c>
@@ -10062,7 +10049,7 @@
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="41" t="s">
         <v>82</v>
       </c>
@@ -10070,7 +10057,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
         <v>83</v>
       </c>
@@ -10078,7 +10065,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="41" t="s">
         <v>84</v>
       </c>
@@ -10086,20 +10073,20 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" s="47">
         <f>SUM(C2:C10)</f>
         <v>1.0010000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>85</v>
       </c>
@@ -10110,7 +10097,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="41" t="s">
         <v>87</v>
       </c>
@@ -10118,7 +10105,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="41" t="s">
         <v>88</v>
       </c>
@@ -10126,7 +10113,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="41" t="s">
         <v>89</v>
       </c>
@@ -10134,9 +10121,9 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C17" s="47">
         <f>SUM(C13:C16)</f>
@@ -10150,7 +10137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10160,34 +10147,34 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="56" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="56" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="56"/>
+    <col min="2" max="2" width="19.140625" style="56" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="56" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="72" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="71" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B2" s="68" t="s">
         <v>32</v>
@@ -10199,66 +10186,66 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="68" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="70"/>
       <c r="D3" s="70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E3" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="69"/>
       <c r="B4" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="70"/>
       <c r="D4" s="70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E4" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
       <c r="B5" s="68" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="70"/>
       <c r="D5" s="70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E5" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="69"/>
       <c r="B6" s="68" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="70"/>
       <c r="D6" s="70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E6" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="69"/>
       <c r="B7" s="68" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C7" s="67"/>
       <c r="D7" s="66"/>
@@ -10271,7 +10258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10281,29 +10268,29 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="94" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B1" s="73" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="95" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" s="95" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="95" t="s">
         <v>70</v>
       </c>
@@ -10311,24 +10298,24 @@
         <v>67</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="95" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D3" s="70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed way quartic and quadratics solved, improved inheritance in population & age group classes, fixed minor bug in calculating future stunting prob
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3AE053F1-2590-CC41-A740-BD07F23DAE35}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BF2BA707-3ED1-7940-9FC5-0E6FE9E2CE84}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4191,8 +4191,8 @@
   </sheetPr>
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4604,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5552,7 +5552,7 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7466,7 +7466,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9277,7 +9277,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Uniform family planning spelling
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FD2F4D14-E386-2A45-AD47-BDEAE6B7B8D9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98A9ADAE-31DD-AF43-A379-0E8D600CF42D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -390,9 +390,6 @@
     <t>Treatment of SAM</t>
   </si>
   <si>
-    <t>Family Planning</t>
-  </si>
-  <si>
     <t>Prevalence of iron deficiency anaemia</t>
   </si>
   <si>
@@ -802,6 +799,9 @@
   </si>
   <si>
     <t>Birth spacing</t>
+  </si>
+  <si>
+    <t>Family planning</t>
   </si>
 </sst>
 </file>
@@ -4145,8 +4145,8 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4158,18 +4158,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>168</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -4177,7 +4177,7 @@
     <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="92">
         <v>2017</v>
@@ -4186,7 +4186,7 @@
     <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="93">
         <v>2030</v>
@@ -4204,7 +4204,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="24">
         <v>0.28199999999999997</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="23">
         <v>0.23</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="24">
         <v>0.51</v>
@@ -4236,7 +4236,7 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="24">
         <v>0.37</v>
@@ -4244,7 +4244,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="24">
         <v>0.221</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="23">
         <v>0.3</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="23">
         <v>0</v>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="23">
         <v>0</v>
@@ -4286,7 +4286,7 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="23">
         <v>0.8</v>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="26">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
@@ -4306,12 +4306,12 @@
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="23">
         <v>0.127</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="23">
         <v>0.45200000000000001</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="23">
         <v>0.33400000000000002</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" s="23">
         <v>8.6999999999999994E-2</v>
@@ -4347,14 +4347,14 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="42">
         <v>0.20799999999999999</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="42">
         <v>3.5999999999999997E-2</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="42">
         <v>0.11899999999999999</v>
@@ -4378,7 +4378,7 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="42">
         <v>0.63700000000000001</v>
@@ -4386,7 +4386,7 @@
     </row>
     <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="44">
         <f>SUM(C28:C31)</f>
@@ -4396,19 +4396,19 @@
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="25">
         <v>25</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="25">
         <v>43</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="25">
         <v>67</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="25">
         <v>4.01</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="23">
         <v>0.13</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="25">
         <v>22.4</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
@@ -4511,13 +4511,13 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C50" s="7">
         <v>1.66</v>
@@ -4526,7 +4526,7 @@
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C51" s="7">
         <v>1.66</v>
@@ -4534,7 +4534,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" s="7">
         <v>5.64</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C53" s="7">
         <v>5.43</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C54" s="7">
         <v>1.91</v>
@@ -4558,12 +4558,12 @@
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" s="24">
         <v>0.2</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C58" s="24">
         <v>0.42</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59" s="24">
         <v>1</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C60" s="24">
         <v>1</v>
@@ -4621,24 +4621,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="82" t="s">
         <v>32</v>
@@ -4751,18 +4751,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="66" t="s">
         <v>59</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>59</v>
@@ -4783,16 +4783,16 @@
         <v>58</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="66"/>
     </row>
@@ -4834,8 +4834,8 @@
   </sheetPr>
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4846,12 +4846,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
@@ -4866,27 +4866,27 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
@@ -4960,7 +4960,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="37">
         <f>'Baseline year population inputs'!C50</f>
@@ -5047,7 +5047,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5067,7 +5067,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -5162,7 +5162,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="51">
         <v>1</v>
@@ -5206,7 +5206,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="51">
         <v>0</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="51">
         <v>0</v>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="51">
         <v>1</v>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="51">
         <v>1</v>
@@ -5668,7 +5668,7 @@
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="52">
         <v>0</v>
@@ -5713,7 +5713,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="52">
         <v>0</v>
@@ -5762,7 +5762,7 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="52">
         <v>0</v>
@@ -5858,7 +5858,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="52">
         <v>0</v>
@@ -5902,7 +5902,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="52">
         <v>0</v>
@@ -6000,7 +6000,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="89" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C24" s="52">
         <v>0</v>
@@ -6092,7 +6092,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C25" s="52">
         <v>0</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C26" s="52">
         <v>0</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="52">
         <v>0</v>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="51">
         <v>1</v>
@@ -6557,7 +6557,7 @@
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="51">
         <v>1</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="51">
         <v>1</v>
@@ -6645,7 +6645,7 @@
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="51">
         <v>1</v>
@@ -6689,7 +6689,7 @@
     </row>
     <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="51">
         <v>1</v>
@@ -6765,24 +6765,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="56">
         <v>0.9</v>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
@@ -6818,7 +6818,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="56">
         <v>1</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="56">
         <v>1</v>
@@ -6854,7 +6854,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="56">
         <v>1</v>
@@ -6872,7 +6872,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="56">
         <v>0.93</v>
@@ -6890,7 +6890,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="56">
         <v>0.5</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" s="56">
         <v>0.5</v>
@@ -6926,7 +6926,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="56">
         <v>0.98</v>
@@ -6975,10 +6975,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>113</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>114</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>49</v>
@@ -6993,10 +6993,10 @@
         <v>52</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J1" s="31" t="s">
         <v>36</v>
@@ -8160,7 +8160,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="33">
         <v>2.7000000000000001E-3</v>
@@ -8344,7 +8344,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="34">
         <v>0</v>
@@ -8806,10 +8806,10 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -8835,7 +8835,7 @@
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
@@ -8861,7 +8861,7 @@
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="39">
         <v>8.7000000000000008E-2</v>
@@ -8882,7 +8882,7 @@
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="39">
         <v>4.5999999999999999E-2</v>
@@ -8918,10 +8918,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -8946,7 +8946,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
@@ -8971,7 +8971,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="39">
         <v>5.3999999999999999E-2</v>
@@ -8991,7 +8991,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="39">
         <v>0.04</v>
@@ -9025,7 +9025,7 @@
     </row>
     <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>1</v>
@@ -9069,7 +9069,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="47">
         <v>0.1</v>
@@ -9113,7 +9113,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="46">
         <f t="shared" ref="C15:O15" si="0">iron_deficiency_anaemia*C14</f>
@@ -9235,7 +9235,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="39">
         <v>0.84</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="39">
         <v>9.1999999999999998E-2</v>
@@ -9275,7 +9275,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="39">
         <v>5.8000000000000003E-2</v>
@@ -9295,7 +9295,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="46">
         <f>1-SUM(C2:C4)</f>
@@ -9342,10 +9342,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9377,10 +9377,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9397,10 +9397,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9417,10 +9417,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9448,7 +9448,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9462,10 +9462,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9479,7 +9479,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9493,10 +9493,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9510,7 +9510,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9549,24 +9549,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E1" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="64" t="s">
         <v>32</v>
@@ -9585,7 +9585,7 @@
       </c>
       <c r="C3" s="66"/>
       <c r="D3" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="C4" s="66"/>
       <c r="D4" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="C5" s="66"/>
       <c r="D5" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E5" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9627,7 +9627,7 @@
       </c>
       <c r="C6" s="66"/>
       <c r="D6" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9637,7 +9637,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="62"/>
@@ -9670,44 +9670,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="91" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="91" t="s">
-        <v>187</v>
-      </c>
       <c r="D1" s="91" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="64" t="s">
         <v>67</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="91" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -9723,7 +9723,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9737,17 +9737,17 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="94" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9766,7 +9766,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="71">
         <v>0</v>
@@ -9797,7 +9797,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="B5" s="71">
         <v>0</v>
@@ -9828,7 +9828,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="71">
         <v>0</v>
@@ -9842,7 +9842,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="71">
         <v>0</v>
@@ -9856,7 +9856,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="71">
         <v>0</v>
@@ -9870,7 +9870,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -9884,7 +9884,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -9898,7 +9898,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -9942,7 +9942,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="71">
         <v>0</v>
@@ -9957,7 +9957,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="71">
         <v>0</v>
@@ -9971,7 +9971,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="71">
         <v>0</v>
@@ -10001,7 +10001,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="71">
         <v>0</v>
@@ -10016,7 +10016,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="71">
         <v>0</v>
@@ -10031,7 +10031,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="71">
         <v>0.1</v>
@@ -10061,7 +10061,7 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="71">
         <v>0</v>
@@ -10118,7 +10118,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="71">
         <v>0.80700000000000005</v>
@@ -10132,7 +10132,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="71">
         <v>0.73199999999999998</v>
@@ -10146,7 +10146,7 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="71">
         <v>0.316</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="71">
         <v>0.59699999999999998</v>
@@ -10174,7 +10174,7 @@
     </row>
     <row r="31" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="71">
         <v>0.19900000000000001</v>
@@ -10189,7 +10189,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="71">
         <v>0.13400000000000001</v>

</xml_diff>

<commit_message>
Getting OR for optimal birth spacing, changed location of birth spacing distribution
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98A9ADAE-31DD-AF43-A379-0E8D600CF42D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF94204-A036-3B44-A2CC-D39F7A091D22}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37040" yWindow="-20700" windowWidth="38400" windowHeight="21140" tabRatio="961" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4146,7 +4146,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4365,7 +4365,7 @@
         <v>76</v>
       </c>
       <c r="C29" s="42">
-        <v>3.5999999999999997E-2</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -4381,7 +4381,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="42">
-        <v>0.63700000000000001</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -4834,7 +4834,7 @@
   </sheetPr>
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -6751,7 +6751,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6960,7 +6960,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="O40" sqref="O40:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7030,7 +7030,7 @@
         <v>13370081</v>
       </c>
       <c r="I2" s="30">
-        <f t="shared" ref="I2:I40" si="1">(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
+        <f>(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>2480858.588708919</v>
       </c>
       <c r="J2" s="30">
@@ -7040,7 +7040,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
-        <f t="shared" ref="A3:A40" si="2">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
+        <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
       </c>
       <c r="B3" s="8">
@@ -7066,7 +7066,7 @@
         <v>13842766</v>
       </c>
       <c r="I3" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I2:I40" si="2">(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
         <v>2527889.0832815999</v>
       </c>
       <c r="J3" s="30">
@@ -7076,7 +7076,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2019</v>
       </c>
       <c r="B4" s="8">
@@ -7102,7 +7102,7 @@
         <v>14328740</v>
       </c>
       <c r="I4" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2586677.2014974509</v>
       </c>
       <c r="J4" s="30">
@@ -7112,7 +7112,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2020</v>
       </c>
       <c r="B5" s="8">
@@ -7138,7 +7138,7 @@
         <v>14821716</v>
       </c>
       <c r="I5" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2633707.6960701318</v>
       </c>
       <c r="J5" s="30">
@@ -7148,7 +7148,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2021</v>
       </c>
       <c r="B6" s="8">
@@ -7174,7 +7174,7 @@
         <v>15326652</v>
       </c>
       <c r="I6" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2680738.1906428128</v>
       </c>
       <c r="J6" s="30">
@@ -7184,7 +7184,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
       <c r="B7" s="8">
@@ -7210,7 +7210,7 @@
         <v>15838161</v>
       </c>
       <c r="I7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2739526.3088586638</v>
       </c>
       <c r="J7" s="30">
@@ -7220,7 +7220,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2023</v>
       </c>
       <c r="B8" s="8">
@@ -7246,7 +7246,7 @@
         <v>16358958</v>
       </c>
       <c r="I8" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2798314.4270745148</v>
       </c>
       <c r="J8" s="30">
@@ -7256,7 +7256,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2024</v>
       </c>
       <c r="B9" s="8">
@@ -7282,7 +7282,7 @@
         <v>16894224</v>
       </c>
       <c r="I9" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2845344.9216471957</v>
       </c>
       <c r="J9" s="30">
@@ -7292,7 +7292,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
       <c r="B10" s="8">
@@ -7318,7 +7318,7 @@
         <v>17446245</v>
       </c>
       <c r="I10" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2915890.6635062173</v>
       </c>
       <c r="J10" s="30">
@@ -7328,7 +7328,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
       <c r="B11" s="8">
@@ -7354,7 +7354,7 @@
         <v>18006944</v>
       </c>
       <c r="I11" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2974678.7817220683</v>
       </c>
       <c r="J11" s="30">
@@ -7364,7 +7364,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2027</v>
       </c>
       <c r="B12" s="8">
@@ -7390,7 +7390,7 @@
         <v>18583669</v>
       </c>
       <c r="I12" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3033466.8999379198</v>
       </c>
       <c r="J12" s="30">
@@ -7400,7 +7400,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
       <c r="B13" s="8">
@@ -7426,7 +7426,7 @@
         <v>19174580</v>
       </c>
       <c r="I13" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3092255.0181537713</v>
       </c>
       <c r="J13" s="30">
@@ -7436,7 +7436,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
       <c r="B14" s="8">
@@ -7462,7 +7462,7 @@
         <v>19776256</v>
       </c>
       <c r="I14" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3162800.7600127924</v>
       </c>
       <c r="J14" s="30">
@@ -7472,7 +7472,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2030</v>
       </c>
       <c r="B15" s="8">
@@ -7498,7 +7498,7 @@
         <v>20386728</v>
       </c>
       <c r="I15" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3221588.8782286434</v>
       </c>
       <c r="J15" s="30">
@@ -7508,7 +7508,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B16" s="8"/>
@@ -7522,7 +7522,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J16" s="30">
@@ -7532,7 +7532,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B17" s="8"/>
@@ -7546,7 +7546,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J17" s="30">
@@ -7556,7 +7556,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B18" s="8"/>
@@ -7570,7 +7570,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="30">
@@ -7580,7 +7580,7 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B19" s="8"/>
@@ -7594,7 +7594,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="30">
@@ -7604,7 +7604,7 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B20" s="8"/>
@@ -7618,7 +7618,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J20" s="30">
@@ -7628,7 +7628,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B21" s="8"/>
@@ -7642,7 +7642,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="30">
@@ -7652,7 +7652,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B22" s="8"/>
@@ -7666,7 +7666,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J22" s="30">
@@ -7676,7 +7676,7 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B23" s="8"/>
@@ -7690,7 +7690,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J23" s="30">
@@ -7700,7 +7700,7 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B24" s="8"/>
@@ -7714,7 +7714,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J24" s="30">
@@ -7724,7 +7724,7 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B25" s="8"/>
@@ -7738,7 +7738,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J25" s="30">
@@ -7748,7 +7748,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B26" s="8"/>
@@ -7762,7 +7762,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J26" s="30">
@@ -7772,7 +7772,7 @@
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B27" s="8"/>
@@ -7786,7 +7786,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27" s="30">
@@ -7796,7 +7796,7 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B28" s="8"/>
@@ -7810,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J28" s="30">
@@ -7820,7 +7820,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B29" s="8"/>
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J29" s="30">
@@ -7844,7 +7844,7 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B30" s="8"/>
@@ -7858,7 +7858,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J30" s="30">
@@ -7868,7 +7868,7 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B31" s="8"/>
@@ -7882,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J31" s="30">
@@ -7892,7 +7892,7 @@
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B32" s="8"/>
@@ -7906,7 +7906,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J32" s="30">
@@ -7916,7 +7916,7 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B33" s="8"/>
@@ -7930,7 +7930,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J33" s="30">
@@ -7940,7 +7940,7 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B34" s="8"/>
@@ -7954,7 +7954,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J34" s="30">
@@ -7964,7 +7964,7 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B35" s="8"/>
@@ -7978,7 +7978,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J35" s="30">
@@ -7988,7 +7988,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B36" s="8"/>
@@ -8002,7 +8002,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J36" s="30">
@@ -8012,7 +8012,7 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B37" s="8"/>
@@ -8026,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J37" s="30">
@@ -8036,7 +8036,7 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B38" s="8"/>
@@ -8050,7 +8050,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J38" s="30">
@@ -8060,7 +8060,7 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B39" s="8"/>
@@ -8074,7 +8074,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J39" s="30">
@@ -8084,7 +8084,7 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B40" s="8"/>
@@ -8098,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J40" s="30">
@@ -9722,8 +9722,8 @@
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9800,7 +9800,7 @@
         <v>205</v>
       </c>
       <c r="B5" s="71">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="71">
         <v>0.95</v>

</xml_diff>

<commit_message>
Fix for odict not having keyerror
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C7A75CD-DE6B-EF4B-8E4F-4FDACC701C17}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D0B208E-0740-3F44-8234-35B8360083B8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37040" yWindow="-20700" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -4145,7 +4145,7 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -4737,8 +4737,8 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5440,19 +5440,19 @@
       </c>
       <c r="D9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="E9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="F9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="G9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="H9" s="52">
         <v>0</v>
@@ -7066,7 +7066,7 @@
         <v>13842766</v>
       </c>
       <c r="I3" s="30">
-        <f t="shared" ref="I2:I40" si="2">(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" ref="I3:I40" si="2">(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
         <v>2527889.0832815999</v>
       </c>
       <c r="J3" s="30">
@@ -8771,7 +8771,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9656,8 +9656,8 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9692,9 +9692,7 @@
       <c r="C2" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="66" t="s">
-        <v>200</v>
-      </c>
+      <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="91" t="s">
@@ -9706,9 +9704,7 @@
       <c r="C3" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="D3" s="66" t="s">
-        <v>200</v>
-      </c>
+      <c r="D3" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10099,7 +10095,7 @@
       </c>
       <c r="D25" s="73">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
-        <v>10.015195269175592</v>
+        <v>5.2956558655829511</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Removed fracs mam to sam
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A29370E1-7464-5448-8D90-579A066D3D05}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B9EF170-96B5-6E47-93D4-ED102020E987}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35700" yWindow="-19120" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="IYCF cost" sheetId="57" r:id="rId10"/>
     <sheet name="Program dependencies" sheetId="58" r:id="rId11"/>
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
-    <sheet name="Incidence of conditions" sheetId="7" state="hidden" r:id="rId13"/>
+    <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" state="hidden" r:id="rId14"/>
     <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
   </sheets>
@@ -45,7 +45,7 @@
     <definedName name="frac_mam_1month">'Nutritional status distribution'!$C$10</definedName>
     <definedName name="frac_mam_24_59months">'Nutritional status distribution'!$G$10</definedName>
     <definedName name="frac_mam_6_11months">'Nutritional status distribution'!$E$10</definedName>
-    <definedName name="frac_MAMtoSAM">'Baseline year population inputs'!$C$59</definedName>
+    <definedName name="frac_MAMtoSAM">'Baseline year population inputs'!#REF!</definedName>
     <definedName name="frac_other_staples">'Baseline year population inputs'!$C$19</definedName>
     <definedName name="frac_PW_health_facility">'Baseline year population inputs'!$C$10</definedName>
     <definedName name="frac_rice">'Baseline year population inputs'!$C$16</definedName>
@@ -54,7 +54,7 @@
     <definedName name="frac_sam_1month">'Nutritional status distribution'!$C$11</definedName>
     <definedName name="frac_sam_24_59months">'Nutritional status distribution'!$G$11</definedName>
     <definedName name="frac_sam_6_11months">'Nutritional status distribution'!$E$11</definedName>
-    <definedName name="frac_SAMtoMAM">'Baseline year population inputs'!$C$60</definedName>
+    <definedName name="frac_SAMtoMAM">'Baseline year population inputs'!#REF!</definedName>
     <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$15</definedName>
     <definedName name="frac_wheat">'Baseline year population inputs'!$C$17</definedName>
     <definedName name="infant_mortality">'Baseline year population inputs'!$C$37</definedName>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -594,12 +594,6 @@
     <t>Other risks</t>
   </si>
   <si>
-    <t>Percentage of SAM cases that develop from MAM</t>
-  </si>
-  <si>
-    <t>Percentage of SAM cases that only recover to MAM</t>
-  </si>
-  <si>
     <t>Baseline year mortality and risk factors</t>
   </si>
   <si>
@@ -802,6 +796,9 @@
   </si>
   <si>
     <t>Family planning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           </t>
   </si>
 </sst>
 </file>
@@ -4143,10 +4140,10 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4161,15 +4158,15 @@
         <v>100</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -4177,7 +4174,7 @@
     <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="92">
         <v>2017</v>
@@ -4186,7 +4183,7 @@
     <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="93">
         <v>2030</v>
@@ -4347,7 +4344,7 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -4396,7 +4393,7 @@
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4436,7 +4433,7 @@
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C39" s="25">
         <v>4.01</v>
@@ -4577,24 +4574,8 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C59" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B60" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="C60" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="4"/>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4621,24 +4602,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D1" s="84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="83" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B2" s="82" t="s">
         <v>32</v>
@@ -4754,15 +4735,15 @@
         <v>69</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="66" t="s">
         <v>59</v>
@@ -4771,7 +4752,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>59</v>
@@ -4783,16 +4764,16 @@
         <v>58</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="66"/>
     </row>
@@ -4851,7 +4832,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
@@ -4933,7 +4914,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5162,7 +5143,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="51">
         <v>1</v>
@@ -5206,7 +5187,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5250,7 +5231,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="51">
         <v>0</v>
@@ -5296,7 +5277,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="51">
         <v>0</v>
@@ -5713,7 +5694,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C16" s="52">
         <v>0</v>
@@ -5762,7 +5743,7 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" s="52">
         <v>0</v>
@@ -6000,7 +5981,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="89" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6044,7 +6025,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C24" s="52">
         <v>0</v>
@@ -6092,7 +6073,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="89" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C25" s="52">
         <v>0</v>
@@ -6140,7 +6121,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="89" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C26" s="52">
         <v>0</v>
@@ -6188,7 +6169,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C27" s="52">
         <v>0</v>
@@ -6765,24 +6746,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="56">
         <v>0.9</v>
@@ -6800,7 +6781,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
@@ -6818,7 +6799,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="56">
         <v>1</v>
@@ -6836,7 +6817,7 @@
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" s="56">
         <v>1</v>
@@ -6854,7 +6835,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" s="56">
         <v>1</v>
@@ -6872,7 +6853,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B7" s="56">
         <v>0.93</v>
@@ -6890,7 +6871,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" s="56">
         <v>0.5</v>
@@ -6908,7 +6889,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" s="56">
         <v>0.5</v>
@@ -6926,7 +6907,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B10" s="56">
         <v>0.98</v>
@@ -9235,7 +9216,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" s="39">
         <v>0.84</v>
@@ -9255,7 +9236,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" s="39">
         <v>9.1999999999999998E-2</v>
@@ -9275,7 +9256,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="39">
         <v>5.8000000000000003E-2</v>
@@ -9295,7 +9276,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" s="46">
         <f>1-SUM(C2:C4)</f>
@@ -9342,10 +9323,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9377,10 +9358,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9397,10 +9378,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9417,10 +9398,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9448,7 +9429,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9462,10 +9443,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9479,7 +9460,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9496,7 +9477,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9510,7 +9491,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9549,24 +9530,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" s="69" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" s="64" t="s">
         <v>32</v>
@@ -9585,7 +9566,7 @@
       </c>
       <c r="C3" s="66"/>
       <c r="D3" s="66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E3" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9599,7 +9580,7 @@
       </c>
       <c r="C4" s="66"/>
       <c r="D4" s="66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E4" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9613,7 +9594,7 @@
       </c>
       <c r="C5" s="66"/>
       <c r="D5" s="66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E5" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9627,7 +9608,7 @@
       </c>
       <c r="C6" s="66"/>
       <c r="D6" s="66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E6" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9637,7 +9618,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="62"/>
@@ -9657,7 +9638,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9670,16 +9651,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="90" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C1" s="91" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -9690,24 +9671,22 @@
         <v>67</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>200</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="91" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" s="66" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -9722,7 +9701,7 @@
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -9744,10 +9723,10 @@
         <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="78" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9796,7 +9775,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" s="71">
         <v>0</v>
@@ -9827,7 +9806,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B7" s="71">
         <v>0</v>
@@ -9841,7 +9820,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="89" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B8" s="71">
         <v>0</v>
@@ -9855,7 +9834,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="89" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" s="71">
         <v>0</v>
@@ -9869,7 +9848,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -9883,7 +9862,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -9897,7 +9876,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -9941,7 +9920,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B15" s="71">
         <v>0</v>
@@ -9956,7 +9935,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B16" s="71">
         <v>0</v>
@@ -9970,7 +9949,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="71">
         <v>0</v>
@@ -10030,7 +10009,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B21" s="71">
         <v>0.1</v>
@@ -10098,7 +10077,7 @@
       </c>
       <c r="D25" s="73">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
-        <v>10.015195269175592</v>
+        <v>5.2956558655829511</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Turned on auto calculate
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B9EF170-96B5-6E47-93D4-ED102020E987}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B88E5EA4-F48C-B549-A620-6095E58A0EBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35700" yWindow="-19120" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="204">
   <si>
     <t>year</t>
   </si>
@@ -796,9 +796,6 @@
   </si>
   <si>
     <t>Family planning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           </t>
   </si>
 </sst>
 </file>
@@ -4142,8 +4139,8 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5421,19 +5418,19 @@
       </c>
       <c r="D9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="E9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="F9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="G9" s="51">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="H9" s="52">
         <v>0</v>
@@ -6941,7 +6938,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40:P40"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9638,7 +9635,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9685,9 +9682,7 @@
       <c r="C3" s="64" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="66" t="s">
-        <v>204</v>
-      </c>
+      <c r="D3" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New user exercises, include IYCF in spreadsheet.
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B88E5EA4-F48C-B549-A620-6095E58A0EBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3B6500C-E43F-6B44-ABBD-58AA190A6FC3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Program dependencies" sheetId="58" r:id="rId11"/>
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
-    <sheet name="Programs target population" sheetId="21" state="hidden" r:id="rId14"/>
+    <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
     <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
@@ -73,7 +73,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -796,6 +796,12 @@
   </si>
   <si>
     <t>Family planning</t>
+  </si>
+  <si>
+    <t>IYCF 2</t>
+  </si>
+  <si>
+    <t>IYCF 3</t>
   </si>
 </sst>
 </file>
@@ -4139,8 +4145,8 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4716,7 +4722,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5025,7 +5031,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6938,7 +6944,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9511,10 +9517,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9561,10 +9567,10 @@
       <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66" t="s">
+      <c r="C3" s="66" t="s">
         <v>198</v>
       </c>
+      <c r="D3" s="66"/>
       <c r="E3" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -9575,10 +9581,10 @@
       <c r="B4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66" t="s">
+      <c r="C4" s="66" t="s">
         <v>198</v>
       </c>
+      <c r="D4" s="66"/>
       <c r="E4" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -9589,10 +9595,10 @@
       <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66" t="s">
+      <c r="C5" s="66" t="s">
         <v>198</v>
       </c>
+      <c r="D5" s="66"/>
       <c r="E5" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -9603,10 +9609,10 @@
       <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66" t="s">
+      <c r="C6" s="66" t="s">
         <v>198</v>
       </c>
+      <c r="D6" s="66"/>
       <c r="E6" s="86" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -9620,6 +9626,160 @@
       <c r="C7" s="63"/>
       <c r="D7" s="62"/>
       <c r="E7" s="66"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="65"/>
+      <c r="B10" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="65"/>
+      <c r="B11" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="65"/>
+      <c r="B12" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="65"/>
+      <c r="B13" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="65"/>
+      <c r="B14" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="63"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="66"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="65"/>
+      <c r="B17" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="65"/>
+      <c r="B18" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="65"/>
+      <c r="B19" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="65"/>
+      <c r="B20" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="86" t="str">
+        <f>IF(E$7="","",E$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="65"/>
+      <c r="B21" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9694,10 +9854,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9913,7 +10073,7 @@
       </c>
       <c r="E14" s="61"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
         <v>174</v>
       </c>
@@ -9925,12 +10085,12 @@
       </c>
       <c r="D15" s="88">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
-        <v>10.49</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B16" s="71">
         <v>0</v>
@@ -9938,13 +10098,14 @@
       <c r="C16" s="71">
         <v>0.95</v>
       </c>
-      <c r="D16" s="72">
-        <v>8.84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D16" s="88">
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="B17" s="71">
         <v>0</v>
@@ -9952,29 +10113,28 @@
       <c r="C17" s="71">
         <v>0.95</v>
       </c>
-      <c r="D17" s="72">
-        <v>50</v>
-      </c>
-      <c r="E17" s="61"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D17" s="88">
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
+        <v>14.270000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="B18" s="71">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C18" s="71">
         <v>0.95</v>
       </c>
       <c r="D18" s="72">
-        <v>2.61</v>
-      </c>
-      <c r="E18" s="61"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="B19" s="71">
         <v>0</v>
@@ -9983,86 +10143,88 @@
         <v>0.95</v>
       </c>
       <c r="D19" s="72">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E19" s="61"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="B20" s="71">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
       </c>
       <c r="D20" s="72">
-        <v>1</v>
-      </c>
-      <c r="E20" s="74"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2.61</v>
+      </c>
+      <c r="E20" s="61"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B21" s="71">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="71">
         <v>0.95</v>
       </c>
       <c r="D21" s="72">
-        <v>4.6500000000000004</v>
+        <v>1</v>
       </c>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B22" s="71">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="C22" s="71">
         <v>0.95</v>
       </c>
       <c r="D22" s="72">
-        <v>3.78</v>
-      </c>
-      <c r="E22" s="61"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="E22" s="74"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="B23" s="71">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
       </c>
       <c r="D23" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E23" s="61"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" s="71">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
       </c>
       <c r="D24" s="72">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3.78</v>
+      </c>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B25" s="71">
         <v>0</v>
@@ -10070,130 +10232,158 @@
       <c r="C25" s="71">
         <v>0.95</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="71">
+        <v>0</v>
+      </c>
+      <c r="C26" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D26" s="72">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="71">
+        <v>0</v>
+      </c>
+      <c r="C27" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D27" s="73">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="70" t="s">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="71">
+      <c r="B28" s="71">
         <v>0.89970000000000006</v>
-      </c>
-      <c r="C26" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D26" s="72">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="71">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="C27" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D27" s="72">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="71">
-        <v>0.73199999999999998</v>
       </c>
       <c r="C28" s="71">
         <v>0.95</v>
       </c>
       <c r="D28" s="72">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="70" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B29" s="71">
-        <v>0.316</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C29" s="71">
         <v>0.95</v>
       </c>
       <c r="D29" s="72">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="70" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B30" s="71">
-        <v>0.59699999999999998</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
       </c>
       <c r="D30" s="72">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31" s="71">
-        <v>0.19900000000000001</v>
+        <v>0.316</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
       </c>
       <c r="D31" s="72">
-        <v>102</v>
-      </c>
-      <c r="F31" s="53"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B32" s="71">
-        <v>0.13400000000000001</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
       </c>
       <c r="D32" s="72">
-        <v>5.53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B33" s="71">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
       </c>
       <c r="D33" s="72">
-        <v>1</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F33" s="53"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F34" s="54"/>
+      <c r="A34" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="71">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C34" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D34" s="72">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="71">
+        <v>0</v>
+      </c>
+      <c r="C35" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D35" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F36" s="54"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D33">
-    <sortCondition ref="A2:A33"/>
+  <sortState ref="A2:D35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
maybe finally making some progress
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -2752,7 +2752,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2809,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2866,7 +2866,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2923,7 +2923,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +2980,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3037,7 +3037,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3094,7 +3094,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3151,7 +3151,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3208,7 +3208,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,7 +3265,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3322,7 +3322,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3379,7 +3379,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3436,7 +3436,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3493,7 +3493,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3550,7 +3550,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3607,7 +3607,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3664,7 +3664,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3721,7 +3721,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3770,7 +3770,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9789,7 +9789,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9801,7 +9801,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="90"/>
+      <c r="A1" s="90" t="s">
+        <v>165</v>
+      </c>
       <c r="B1" s="69" t="s">
         <v>182</v>
       </c>

</xml_diff>

<commit_message>
Updating ORS/Zn+ORS target populations
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\national\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21135" windowWidth="28920" windowHeight="16320" tabRatio="961" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="-21132" windowWidth="28920" windowHeight="16320" tabRatio="961"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -27,6 +32,11 @@
     <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
     <definedName name="abortion">'Baseline year population inputs'!$C$40</definedName>
     <definedName name="comm_deliv">'Treatment of SAM'!$D$3</definedName>
+    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$51</definedName>
+    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$53</definedName>
+    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$50</definedName>
+    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$54</definedName>
+    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$52</definedName>
     <definedName name="end_year">'Baseline year population inputs'!$C$4</definedName>
     <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$12</definedName>
     <definedName name="food_insecure">'Baseline year population inputs'!$C$7</definedName>
@@ -67,7 +77,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -82,7 +92,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +150,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -801,12 +811,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -1065,7 +1075,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1827,8 +1837,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1844,8 +1854,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1864,20 +1874,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1889,11 +1899,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1923,7 +1933,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1951,7 +1961,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2752,7 +2762,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2819,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2866,7 +2876,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2923,7 +2933,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +2990,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3037,7 +3047,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3094,7 +3104,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3151,7 +3161,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3208,7 +3218,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,7 +3275,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3322,7 +3332,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3379,7 +3389,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3436,7 +3446,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3493,7 +3503,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3550,7 +3560,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3607,7 +3617,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3664,7 +3674,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3721,7 +3731,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3770,7 +3780,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4139,18 +4149,18 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4161,14 +4171,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
@@ -4177,7 +4187,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
@@ -4186,17 +4196,17 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4204,7 +4214,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4212,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4220,7 +4230,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4228,7 +4238,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4236,7 +4246,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4244,17 +4254,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4262,7 +4272,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4278,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4286,7 +4296,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4295,15 +4305,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4311,7 +4321,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4319,7 +4329,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4327,7 +4337,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4335,18 +4345,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>200</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4354,7 +4364,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4362,7 +4372,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4370,7 +4380,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4378,7 +4388,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4387,20 +4397,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4408,7 +4418,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4418,7 +4428,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4428,7 +4438,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4436,7 +4446,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4444,7 +4454,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4452,16 +4462,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4470,7 +4480,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4479,7 +4489,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4489,7 +4499,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4500,16 +4510,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4518,7 +4528,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4526,7 +4536,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4534,7 +4544,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4542,7 +4552,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4550,12 +4560,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4563,7 +4573,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4571,7 +4581,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4591,13 +4601,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="80" customWidth="1"/>
-    <col min="2" max="16384" width="10.85546875" style="80"/>
+    <col min="1" max="1" width="18.6640625" style="80" customWidth="1"/>
+    <col min="2" max="16384" width="10.88671875" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
         <v>198</v>
       </c>
@@ -4614,7 +4624,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
         <v>165</v>
       </c>
@@ -4632,7 +4642,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="82"/>
       <c r="B3" s="82" t="s">
         <v>1</v>
@@ -4649,7 +4659,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="82"/>
       <c r="B4" s="82" t="s">
         <v>2</v>
@@ -4666,7 +4676,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="82"/>
       <c r="B5" s="82" t="s">
         <v>3</v>
@@ -4683,7 +4693,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="82"/>
       <c r="B6" s="82" t="s">
         <v>4</v>
@@ -4700,7 +4710,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" s="81"/>
     </row>
   </sheetData>
@@ -4719,15 +4729,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="2" max="2" width="47.88671875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4738,7 +4748,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -4747,7 +4757,7 @@
       </c>
       <c r="C2" s="66"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
@@ -4756,7 +4766,7 @@
       </c>
       <c r="C3" s="66"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>58</v>
       </c>
@@ -4765,7 +4775,7 @@
       </c>
       <c r="C4" s="66"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
         <v>138</v>
       </c>
@@ -4774,28 +4784,28 @@
       </c>
       <c r="C5" s="66"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4816,85 +4826,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="30.109375" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="66"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="66"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="66"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="66"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="66"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="66"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="66"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="66"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="66"/>
     </row>
   </sheetData>
@@ -4914,9 +4924,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4936,7 +4946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4961,7 +4971,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4986,7 +4996,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5025,22 +5035,22 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C11" sqref="C11:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5087,7 +5097,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5138,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5182,7 +5192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>199</v>
       </c>
@@ -5226,7 +5236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5272,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5319,24 +5329,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="51">
-        <v>1</v>
+        <f>diarrhoea_1mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="D7" s="51">
-        <v>1</v>
+        <f>diarrhoea_1_5mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="E7" s="51">
-        <v>1</v>
+        <f>diarrhoea_6_11mo/26</f>
+        <v>0.21692307692307691</v>
       </c>
       <c r="F7" s="51">
-        <v>1</v>
+        <f>diarrhoea_12_23mo/26</f>
+        <v>0.20884615384615385</v>
       </c>
       <c r="G7" s="51">
-        <v>1</v>
+        <f>diarrhoea_24_59mo/26</f>
+        <v>7.3461538461538453E-2</v>
       </c>
       <c r="H7" s="52">
         <v>0</v>
@@ -5363,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5409,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5457,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5501,24 +5516,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="51">
-        <v>1</v>
+        <f>diarrhoea_1mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="D11" s="51">
-        <v>1</v>
+        <f>diarrhoea_1_5mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="E11" s="51">
-        <v>1</v>
+        <f>diarrhoea_6_11mo/26</f>
+        <v>0.21692307692307691</v>
       </c>
       <c r="F11" s="51">
-        <v>1</v>
+        <f>diarrhoea_12_23mo/26</f>
+        <v>0.20884615384615385</v>
       </c>
       <c r="G11" s="51">
-        <v>1</v>
+        <f>diarrhoea_24_59mo/26</f>
+        <v>7.3461538461538453E-2</v>
       </c>
       <c r="H11" s="52">
         <v>0</v>
@@ -5545,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5589,10 +5609,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5643,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5688,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5737,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5786,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5834,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5878,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5922,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5970,10 +5990,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="87" t="s">
         <v>37</v>
       </c>
@@ -6020,7 +6040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="89" t="s">
         <v>189</v>
       </c>
@@ -6068,7 +6088,7 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="89" t="s">
         <v>190</v>
       </c>
@@ -6116,7 +6136,7 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="89" t="s">
         <v>191</v>
       </c>
@@ -6164,7 +6184,7 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="89" t="s">
         <v>192</v>
       </c>
@@ -6209,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6219,7 +6239,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6277,7 +6297,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6332,7 +6352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6387,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6431,7 +6451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6488,7 +6508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6532,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6577,7 +6597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6621,7 +6641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6665,7 +6685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6709,7 +6729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6732,16 +6752,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="53"/>
-    <col min="5" max="5" width="17.42578125" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="53"/>
+    <col min="5" max="5" width="17.44140625" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6758,7 +6778,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6776,7 +6796,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6794,7 +6814,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6812,7 +6832,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6830,7 +6850,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6848,7 +6868,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6866,7 +6886,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6884,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6902,7 +6922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6920,7 +6940,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6941,14 +6961,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.85546875" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="8.44140625" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.88671875" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6980,7 +7000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7016,7 +7036,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7052,7 +7072,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7088,7 +7108,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7124,7 +7144,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7160,7 +7180,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7196,7 +7216,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7232,7 +7252,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7268,7 +7288,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7304,7 +7324,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7340,7 +7360,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7376,7 +7396,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7412,7 +7432,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7448,7 +7468,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7484,7 +7504,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7508,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7532,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7556,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7580,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7604,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7628,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7652,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7676,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7700,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7724,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7748,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7772,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7796,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7820,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7844,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7868,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7892,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7916,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7940,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7964,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7988,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8012,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8036,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8060,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8106,13 +8126,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8136,7 +8156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8159,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8182,7 +8202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8205,7 +8225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8228,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8251,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8274,7 +8294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8297,7 +8317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8320,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8343,7 +8363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8366,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8389,7 +8409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8412,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8435,7 +8455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8458,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8481,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8504,7 +8524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8527,7 +8547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8550,7 +8570,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8573,7 +8593,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8596,7 +8616,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8619,7 +8639,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8642,7 +8662,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8665,7 +8685,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8688,7 +8708,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8711,7 +8731,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8752,13 +8772,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8782,7 +8802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8810,33 +8830,33 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8857,7 +8877,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8878,7 +8898,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8886,7 +8906,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8894,7 +8914,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8922,32 +8942,32 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -8967,7 +8987,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -8987,7 +9007,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9001,7 +9021,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9045,7 +9065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9089,7 +9109,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9146,14 +9166,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9178,13 +9198,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9208,7 +9228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9231,7 +9251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9251,7 +9271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9271,7 +9291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9312,13 +9332,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9353,7 +9373,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9370,10 +9390,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9390,10 +9410,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9410,7 +9430,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9424,7 +9444,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9438,7 +9458,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9455,7 +9475,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9469,7 +9489,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9486,7 +9506,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9517,15 +9537,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="2" max="2" width="19.109375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>179</v>
       </c>
@@ -9542,7 +9562,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>174</v>
       </c>
@@ -9556,7 +9576,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="65"/>
       <c r="B3" s="64" t="s">
         <v>1</v>
@@ -9570,7 +9590,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="65"/>
       <c r="B4" s="64" t="s">
         <v>2</v>
@@ -9584,7 +9604,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="65"/>
       <c r="B5" s="64" t="s">
         <v>3</v>
@@ -9598,7 +9618,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="65"/>
       <c r="B6" s="64" t="s">
         <v>4</v>
@@ -9612,7 +9632,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
         <v>173</v>
@@ -9621,7 +9641,7 @@
       <c r="D7" s="62"/>
       <c r="E7" s="66"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>202</v>
       </c>
@@ -9637,7 +9657,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="65"/>
       <c r="B10" s="64" t="s">
         <v>1</v>
@@ -9649,7 +9669,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="65"/>
       <c r="B11" s="64" t="s">
         <v>2</v>
@@ -9661,7 +9681,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="65"/>
       <c r="B12" s="64" t="s">
         <v>3</v>
@@ -9673,7 +9693,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="65"/>
       <c r="B13" s="64" t="s">
         <v>4</v>
@@ -9685,7 +9705,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
         <v>173</v>
@@ -9694,7 +9714,7 @@
       <c r="D14" s="62"/>
       <c r="E14" s="66"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
         <v>203</v>
       </c>
@@ -9710,7 +9730,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="65"/>
       <c r="B17" s="64" t="s">
         <v>1</v>
@@ -9724,7 +9744,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="65"/>
       <c r="B18" s="64" t="s">
         <v>2</v>
@@ -9738,7 +9758,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="65"/>
       <c r="B19" s="64" t="s">
         <v>3</v>
@@ -9752,7 +9772,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="65"/>
       <c r="B20" s="64" t="s">
         <v>4</v>
@@ -9766,7 +9786,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
         <v>173</v>
@@ -9788,19 +9808,19 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="90" t="s">
         <v>165</v>
       </c>
@@ -9814,7 +9834,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="91" t="s">
         <v>69</v>
       </c>
@@ -9826,7 +9846,7 @@
       </c>
       <c r="D2" s="66"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="91" t="s">
         <v>186</v>
       </c>
@@ -9854,16 +9874,16 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="70" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.42578125" style="53"/>
+    <col min="3" max="3" width="20.44140625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="53" customWidth="1"/>
+    <col min="5" max="16384" width="14.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
         <v>69</v>
       </c>
@@ -9878,7 +9898,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>29</v>
       </c>
@@ -9892,7 +9912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
         <v>86</v>
       </c>
@@ -9907,7 +9927,7 @@
       </c>
       <c r="E3" s="61"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>61</v>
       </c>
@@ -9922,7 +9942,7 @@
       </c>
       <c r="E4" s="61"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
         <v>201</v>
       </c>
@@ -9938,7 +9958,7 @@
       </c>
       <c r="E5" s="76"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>63</v>
       </c>
@@ -9953,7 +9973,7 @@
       </c>
       <c r="E6" s="75"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>189</v>
       </c>
@@ -9967,7 +9987,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89" t="s">
         <v>190</v>
       </c>
@@ -9981,7 +10001,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
         <v>191</v>
       </c>
@@ -9995,7 +10015,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89" t="s">
         <v>192</v>
       </c>
@@ -10009,7 +10029,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>188</v>
       </c>
@@ -10023,7 +10043,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>193</v>
       </c>
@@ -10037,7 +10057,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="70" t="s">
         <v>57</v>
       </c>
@@ -10052,7 +10072,7 @@
       </c>
       <c r="E13" s="61"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="70" t="s">
         <v>47</v>
       </c>
@@ -10067,7 +10087,7 @@
       </c>
       <c r="E14" s="61"/>
     </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="70" t="s">
         <v>174</v>
       </c>
@@ -10082,7 +10102,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
         <v>202</v>
       </c>
@@ -10097,7 +10117,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
         <v>203</v>
       </c>
@@ -10112,7 +10132,7 @@
         <v>14.270000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70" t="s">
         <v>199</v>
       </c>
@@ -10126,7 +10146,7 @@
         <v>8.84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>137</v>
       </c>
@@ -10141,7 +10161,7 @@
       </c>
       <c r="E19" s="61"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70" t="s">
         <v>34</v>
       </c>
@@ -10156,7 +10176,7 @@
       </c>
       <c r="E20" s="61"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>88</v>
       </c>
@@ -10171,7 +10191,7 @@
       </c>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>87</v>
       </c>
@@ -10186,7 +10206,7 @@
       </c>
       <c r="E22" s="74"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
         <v>138</v>
       </c>
@@ -10201,7 +10221,7 @@
       </c>
       <c r="E23" s="61"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
         <v>59</v>
       </c>
@@ -10216,7 +10236,7 @@
       </c>
       <c r="E24" s="61"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
         <v>84</v>
       </c>
@@ -10230,7 +10250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
         <v>58</v>
       </c>
@@ -10244,7 +10264,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70" t="s">
         <v>67</v>
       </c>
@@ -10259,7 +10279,7 @@
         <v>5.2956558655829511</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70" t="s">
         <v>28</v>
       </c>
@@ -10273,7 +10293,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="70" t="s">
         <v>83</v>
       </c>
@@ -10287,7 +10307,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="70" t="s">
         <v>82</v>
       </c>
@@ -10301,7 +10321,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="70" t="s">
         <v>81</v>
       </c>
@@ -10315,7 +10335,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="70" t="s">
         <v>79</v>
       </c>
@@ -10329,7 +10349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="70" t="s">
         <v>80</v>
       </c>
@@ -10344,7 +10364,7 @@
       </c>
       <c r="F33" s="53"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70" t="s">
         <v>85</v>
       </c>
@@ -10358,7 +10378,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="70" t="s">
         <v>60</v>
       </c>
@@ -10372,7 +10392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F36" s="54"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reconciled demo and template books
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\national\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3238136D-D270-8B4C-AEA6-E1F786808966}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21132" windowWidth="28920" windowHeight="16320" tabRatio="961"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -87,12 +88,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -116,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -145,12 +146,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -811,12 +812,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -1075,7 +1076,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1837,8 +1838,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1854,8 +1855,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1874,20 +1875,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1899,11 +1900,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1933,7 +1934,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1961,7 +1962,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2702,8 +2703,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -4143,24 +4144,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.44140625" style="15"/>
+    <col min="3" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4171,14 +4170,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
@@ -4187,7 +4186,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
@@ -4196,17 +4195,17 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4222,7 +4221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4230,7 +4229,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4238,7 +4237,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4254,17 +4253,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4272,7 +4271,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4280,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4288,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4296,7 +4295,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4305,15 +4304,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4321,7 +4320,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4345,18 +4344,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>200</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4372,7 +4371,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4388,7 +4387,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4397,20 +4396,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4428,7 +4427,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4438,7 +4437,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4462,16 +4461,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4480,7 +4479,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4489,7 +4488,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4499,7 +4498,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4510,16 +4509,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4528,7 +4527,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4544,7 +4543,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4552,7 +4551,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4560,12 +4559,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4573,7 +4572,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4591,7 +4590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4601,13 +4600,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="80" customWidth="1"/>
-    <col min="2" max="16384" width="10.88671875" style="80"/>
+    <col min="2" max="16384" width="10.83203125" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
         <v>198</v>
       </c>
@@ -4624,7 +4623,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="83" t="s">
         <v>165</v>
       </c>
@@ -4642,7 +4641,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="82"/>
       <c r="B3" s="82" t="s">
         <v>1</v>
@@ -4659,7 +4658,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="82"/>
       <c r="B4" s="82" t="s">
         <v>2</v>
@@ -4676,7 +4675,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="82"/>
       <c r="B5" s="82" t="s">
         <v>3</v>
@@ -4693,7 +4692,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="82"/>
       <c r="B6" s="82" t="s">
         <v>4</v>
@@ -4710,7 +4709,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="81"/>
     </row>
   </sheetData>
@@ -4719,7 +4718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4729,15 +4728,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.88671875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -4757,7 +4756,7 @@
       </c>
       <c r="C2" s="66"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
@@ -4766,7 +4765,7 @@
       </c>
       <c r="C3" s="66"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>58</v>
       </c>
@@ -4775,7 +4774,7 @@
       </c>
       <c r="C4" s="66"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>138</v>
       </c>
@@ -4784,28 +4783,28 @@
       </c>
       <c r="C5" s="66"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4816,7 +4815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4826,85 +4825,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="53"/>
+    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="66" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="66"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="66"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="66"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="66"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="66"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="66"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="66"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="66"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="66"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="66"/>
     </row>
   </sheetData>
@@ -4914,7 +4913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -4924,9 +4923,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4946,7 +4945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4996,7 +4995,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5028,29 +5027,29 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:G11"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.88671875" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5097,7 +5096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5192,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
         <v>199</v>
       </c>
@@ -5236,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5282,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5329,7 +5328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
@@ -5378,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5472,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5516,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
@@ -5565,7 +5564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5609,10 +5608,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5663,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5708,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5757,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5806,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5854,7 +5853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5898,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5942,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5990,10 +5989,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="87" t="s">
         <v>37</v>
       </c>
@@ -6040,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="89" t="s">
         <v>189</v>
       </c>
@@ -6088,7 +6087,7 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="89" t="s">
         <v>190</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="89" t="s">
         <v>191</v>
       </c>
@@ -6184,7 +6183,7 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="89" t="s">
         <v>192</v>
       </c>
@@ -6229,7 +6228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6239,7 +6238,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6297,7 +6296,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6352,7 +6351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6552,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6597,7 +6596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6641,7 +6640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6685,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6729,7 +6728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6742,7 +6741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6752,16 +6751,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" style="53"/>
-    <col min="5" max="5" width="17.44140625" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="53"/>
+    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6778,7 +6777,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6796,7 +6795,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6814,7 +6813,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6832,7 +6831,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6850,7 +6849,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6886,7 +6885,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6904,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6940,7 +6939,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6951,7 +6950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -6961,14 +6960,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.88671875" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="15"/>
+    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7036,7 +7035,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7072,7 +7071,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7108,7 +7107,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7144,7 +7143,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7180,7 +7179,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7216,7 +7215,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7252,7 +7251,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7288,7 +7287,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7324,7 +7323,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7360,7 +7359,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7396,7 +7395,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7432,7 +7431,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7468,7 +7467,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7504,7 +7503,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7528,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7552,7 +7551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7576,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7600,7 +7599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7624,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7648,7 +7647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7672,7 +7671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7696,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7720,7 +7719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7744,7 +7743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7768,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7792,7 +7791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7816,7 +7815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7840,7 +7839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7864,7 +7863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7888,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7912,7 +7911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7936,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7960,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7984,7 +7983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8008,7 +8007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8032,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8056,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8080,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8116,7 +8115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8126,13 +8125,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8156,7 +8155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8179,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8202,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8225,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8248,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8271,7 +8270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8294,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8317,7 +8316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8363,7 +8362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8386,7 +8385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8432,7 +8431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8455,7 +8454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8478,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8501,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8524,7 +8523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8547,7 +8546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8570,7 +8569,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8593,7 +8592,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8616,7 +8615,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8639,7 +8638,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8662,7 +8661,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8685,7 +8684,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8708,7 +8707,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8731,7 +8730,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8762,7 +8761,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8772,13 +8771,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8802,7 +8801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8830,7 +8829,7 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
@@ -8856,7 +8855,7 @@
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8877,7 +8876,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8898,7 +8897,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8906,7 +8905,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8914,7 +8913,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8942,7 +8941,7 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
@@ -8967,7 +8966,7 @@
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -8987,7 +8986,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -9007,7 +9006,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9021,7 +9020,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9065,7 +9064,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9109,7 +9108,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9166,14 +9165,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9188,7 +9187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9198,13 +9197,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9228,7 +9227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9271,7 +9270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9291,7 +9290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9322,7 +9321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9332,13 +9331,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9373,7 +9372,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9390,10 +9389,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9410,10 +9409,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9430,7 +9429,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9444,7 +9443,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9458,7 +9457,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9475,7 +9474,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9489,7 +9488,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9506,7 +9505,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9527,7 +9526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9537,15 +9536,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
         <v>179</v>
       </c>
@@ -9562,7 +9561,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
         <v>174</v>
       </c>
@@ -9576,7 +9575,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="65"/>
       <c r="B3" s="64" t="s">
         <v>1</v>
@@ -9590,7 +9589,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="65"/>
       <c r="B4" s="64" t="s">
         <v>2</v>
@@ -9604,7 +9603,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="65"/>
       <c r="B5" s="64" t="s">
         <v>3</v>
@@ -9618,7 +9617,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="65"/>
       <c r="B6" s="64" t="s">
         <v>4</v>
@@ -9632,7 +9631,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
         <v>173</v>
@@ -9641,7 +9640,7 @@
       <c r="D7" s="62"/>
       <c r="E7" s="66"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="67" t="s">
         <v>202</v>
       </c>
@@ -9657,7 +9656,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="65"/>
       <c r="B10" s="64" t="s">
         <v>1</v>
@@ -9669,7 +9668,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="65"/>
       <c r="B11" s="64" t="s">
         <v>2</v>
@@ -9681,7 +9680,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="65"/>
       <c r="B12" s="64" t="s">
         <v>3</v>
@@ -9693,7 +9692,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="65"/>
       <c r="B13" s="64" t="s">
         <v>4</v>
@@ -9705,7 +9704,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
         <v>173</v>
@@ -9714,7 +9713,7 @@
       <c r="D14" s="62"/>
       <c r="E14" s="66"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="67" t="s">
         <v>203</v>
       </c>
@@ -9730,7 +9729,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="65"/>
       <c r="B17" s="64" t="s">
         <v>1</v>
@@ -9744,7 +9743,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="65"/>
       <c r="B18" s="64" t="s">
         <v>2</v>
@@ -9758,7 +9757,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="65"/>
       <c r="B19" s="64" t="s">
         <v>3</v>
@@ -9772,7 +9771,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="65"/>
       <c r="B20" s="64" t="s">
         <v>4</v>
@@ -9786,7 +9785,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
         <v>173</v>
@@ -9802,7 +9801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9812,15 +9811,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="90" t="s">
         <v>165</v>
       </c>
@@ -9834,7 +9833,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="91" t="s">
         <v>69</v>
       </c>
@@ -9846,7 +9845,7 @@
       </c>
       <c r="D2" s="66"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="91" t="s">
         <v>186</v>
       </c>
@@ -9864,26 +9863,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" style="70" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.44140625" style="53"/>
+    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
+    <col min="5" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="79" t="s">
         <v>69</v>
       </c>
@@ -9898,7 +9897,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
         <v>29</v>
       </c>
@@ -9912,7 +9911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>86</v>
       </c>
@@ -9927,7 +9926,7 @@
       </c>
       <c r="E3" s="61"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>61</v>
       </c>
@@ -9942,7 +9941,7 @@
       </c>
       <c r="E4" s="61"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>201</v>
       </c>
@@ -9958,7 +9957,7 @@
       </c>
       <c r="E5" s="76"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70" t="s">
         <v>63</v>
       </c>
@@ -9973,9 +9972,9 @@
       </c>
       <c r="E6" s="75"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="89" t="s">
-        <v>189</v>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="70" t="s">
+        <v>64</v>
       </c>
       <c r="B7" s="71">
         <v>0</v>
@@ -9984,12 +9983,13 @@
         <v>0.95</v>
       </c>
       <c r="D7" s="72">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="89" t="s">
-        <v>190</v>
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="75"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="70" t="s">
+        <v>62</v>
       </c>
       <c r="B8" s="71">
         <v>0</v>
@@ -9998,12 +9998,13 @@
         <v>0.95</v>
       </c>
       <c r="D8" s="72">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.19</v>
+      </c>
+      <c r="E8" s="75"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="89" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" s="71">
         <v>0</v>
@@ -10012,12 +10013,12 @@
         <v>0.95</v>
       </c>
       <c r="D9" s="72">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -10026,12 +10027,12 @@
         <v>0.95</v>
       </c>
       <c r="D10" s="72">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>188</v>
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="89" t="s">
+        <v>191</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -10040,12 +10041,12 @@
         <v>0.95</v>
       </c>
       <c r="D11" s="72">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>193</v>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="89" t="s">
+        <v>192</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -10054,131 +10055,129 @@
         <v>0.95</v>
       </c>
       <c r="D12" s="72">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
-        <v>57</v>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="B13" s="71">
-        <v>0.34599999999999997</v>
+        <v>0</v>
       </c>
       <c r="C13" s="71">
         <v>0.95</v>
       </c>
       <c r="D13" s="72">
-        <v>2.06</v>
-      </c>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="70" t="s">
-        <v>47</v>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="B14" s="71">
-        <v>0.80800000000000005</v>
+        <v>0</v>
       </c>
       <c r="C14" s="71">
         <v>0.95</v>
       </c>
       <c r="D14" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="61"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="B15" s="71">
-        <v>0</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C15" s="71">
         <v>0.95</v>
       </c>
-      <c r="D15" s="88">
+      <c r="D15" s="72">
+        <v>2.06</v>
+      </c>
+      <c r="E15" s="61"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="71">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="C16" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D16" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="E16" s="61"/>
+    </row>
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="71">
+        <v>0</v>
+      </c>
+      <c r="C17" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D17" s="88">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="71">
-        <v>0</v>
-      </c>
-      <c r="C16" s="71">
+      <c r="B18" s="71">
+        <v>0</v>
+      </c>
+      <c r="C18" s="71">
         <v>0.95</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D18" s="88">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>3.78</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="71">
-        <v>0</v>
-      </c>
-      <c r="C17" s="71">
+      <c r="B19" s="71">
+        <v>0</v>
+      </c>
+      <c r="C19" s="71">
         <v>0.95</v>
       </c>
-      <c r="D17" s="88">
+      <c r="D19" s="88">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>14.270000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="71">
-        <v>0</v>
-      </c>
-      <c r="C18" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D18" s="72">
-        <v>8.84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="71">
-        <v>0</v>
-      </c>
-      <c r="C19" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D19" s="72">
-        <v>50</v>
-      </c>
-      <c r="E19" s="61"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
-        <v>34</v>
-      </c>
       <c r="B20" s="71">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
       </c>
       <c r="D20" s="72">
-        <v>2.61</v>
-      </c>
-      <c r="E20" s="61"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="B21" s="71">
         <v>0</v>
@@ -10187,86 +10186,88 @@
         <v>0.95</v>
       </c>
       <c r="D21" s="72">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="B22" s="71">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C22" s="71">
         <v>0.95</v>
       </c>
       <c r="D22" s="72">
-        <v>1</v>
-      </c>
-      <c r="E22" s="74"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.61</v>
+      </c>
+      <c r="E22" s="61"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B23" s="71">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
       </c>
       <c r="D23" s="72">
-        <v>4.6500000000000004</v>
+        <v>1</v>
       </c>
       <c r="E23" s="61"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B24" s="71">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
       </c>
       <c r="D24" s="72">
-        <v>3.78</v>
-      </c>
-      <c r="E24" s="61"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E24" s="74"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="B25" s="71">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C25" s="71">
         <v>0.95</v>
       </c>
       <c r="D25" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E25" s="61"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="71">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C26" s="71">
         <v>0.95</v>
       </c>
       <c r="D26" s="72">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.78</v>
+      </c>
+      <c r="E26" s="61"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="70" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B27" s="71">
         <v>0</v>
@@ -10274,130 +10275,158 @@
       <c r="C27" s="71">
         <v>0.95</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="71">
+        <v>0</v>
+      </c>
+      <c r="C28" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D28" s="72">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="71">
+        <v>0</v>
+      </c>
+      <c r="C29" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D29" s="73">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70" t="s">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="71">
+      <c r="B30" s="71">
         <v>0.89970000000000006</v>
-      </c>
-      <c r="C28" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D28" s="72">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="71">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="C29" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D29" s="72">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="71">
-        <v>0.73199999999999998</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
       </c>
       <c r="D30" s="72">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B31" s="71">
-        <v>0.316</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
       </c>
       <c r="D31" s="72">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B32" s="71">
-        <v>0.59699999999999998</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
       </c>
       <c r="D32" s="72">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="71">
-        <v>0.19900000000000001</v>
+        <v>0.316</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
       </c>
       <c r="D33" s="72">
-        <v>102</v>
-      </c>
-      <c r="F33" s="53"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B34" s="71">
-        <v>0.13400000000000001</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>
       </c>
       <c r="D34" s="72">
-        <v>5.53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B35" s="71">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C35" s="71">
         <v>0.95</v>
       </c>
       <c r="D35" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F36" s="54"/>
+        <v>102</v>
+      </c>
+      <c r="F35" s="53"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="71">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C36" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D36" s="72">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="71">
+        <v>0</v>
+      </c>
+      <c r="C37" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D37" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F38" s="54"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D35">
-    <sortCondition ref="A2:A35"/>
+  <sortState ref="A2:D37">
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
manually reverse ill-advised sleep-deprived merge
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3238136D-D270-8B4C-AEA6-E1F786808966}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21135" windowWidth="28920" windowHeight="16320" tabRatio="961" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -78,7 +72,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -88,12 +82,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,12 +140,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -780,9 +774,6 @@
   </si>
   <si>
     <t>Baseline year (projection start year)</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Unit costs (US$) by delivery modality and target population</t>
@@ -812,7 +803,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1795,7 +1786,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1930,8 +1921,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1962,7 +1951,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1977,6 +1965,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -2703,8 +2698,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 2" xfId="725"/>
+    <cellStyle name="Normal 3" xfId="726"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -2763,7 +2758,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2820,7 +2815,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2877,7 +2872,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2934,7 +2929,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2991,7 +2986,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3048,7 +3043,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3105,7 +3100,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3162,7 +3157,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3219,7 +3214,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3276,7 +3271,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3333,7 +3328,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3390,7 +3385,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3447,7 +3442,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3504,7 +3499,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3561,7 +3556,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3618,7 +3613,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3675,7 +3670,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3732,7 +3727,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3781,7 +3776,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4144,22 +4139,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4170,42 +4167,42 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="92">
+      <c r="C3" s="89">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="90">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4213,7 +4210,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4221,7 +4218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4229,7 +4226,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4237,7 +4234,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4245,7 +4242,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4253,17 +4250,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4271,7 +4268,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4279,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4287,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4295,7 +4292,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4304,15 +4301,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4320,7 +4317,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4328,7 +4325,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4336,7 +4333,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4344,18 +4341,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4363,7 +4360,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4371,7 +4368,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4379,7 +4376,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4387,7 +4384,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4396,20 +4393,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4417,7 +4414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4427,7 +4424,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4437,7 +4434,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4445,7 +4442,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4453,7 +4450,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4461,16 +4458,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4479,7 +4476,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4488,7 +4485,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4498,7 +4495,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4509,16 +4506,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4527,7 +4524,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4535,7 +4532,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4543,7 +4540,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4551,7 +4548,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4559,12 +4556,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4572,7 +4569,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4580,7 +4577,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4590,7 +4587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4600,117 +4597,117 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="80" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="80"/>
+    <col min="1" max="1" width="18.7109375" style="78" customWidth="1"/>
+    <col min="2" max="16384" width="10.85546875" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="84" t="s">
+    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="82" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="82" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="82" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="70">
         <v>3.78</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="82"/>
-      <c r="B3" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="72">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="80"/>
+      <c r="B3" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="70">
         <f t="shared" ref="D3:D6" si="0">10.49/4</f>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="82"/>
-      <c r="B4" s="82" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="80"/>
+      <c r="B4" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="80"/>
+      <c r="B6" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="81"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="79"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4718,7 +4715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4728,15 +4725,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="53"/>
+    <col min="1" max="1" width="53" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4747,64 +4744,64 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="66"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C2" s="64"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="66"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="70" t="s">
+      <c r="C3" s="64"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="66"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="70" t="s">
+      <c r="C4" s="64"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="66"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C5" s="64"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4815,7 +4812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4825,86 +4822,86 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="53"/>
+    <col min="1" max="1" width="30.140625" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="66" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="66" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="66" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="66" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="64" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="66" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="64" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="66"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="66"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="66"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="66"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="66"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="66"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="66"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="66"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="66"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="64"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="64"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="64"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="64"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="64"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="64"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="64"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="64"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="64"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4913,7 +4910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -4923,9 +4920,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4945,7 +4942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4970,7 +4967,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4995,7 +4992,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5027,29 +5024,29 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C11" sqref="C11:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5096,7 +5093,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5147,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5191,9 +5188,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5235,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5281,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5328,7 +5325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
@@ -5377,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5423,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5471,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5515,7 +5512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
@@ -5564,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5608,10 +5605,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5662,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5707,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5756,7 +5753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5805,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5853,7 +5850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5897,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5941,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5989,15 +5986,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="87" t="s">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="89" t="s">
-        <v>201</v>
+      <c r="B23" s="86" t="s">
+        <v>200</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6039,8 +6036,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="89" t="s">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="86" t="s">
         <v>189</v>
       </c>
       <c r="C24" s="52">
@@ -6087,8 +6084,8 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="89" t="s">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="86" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="52">
@@ -6135,8 +6132,8 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="89" t="s">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="86" t="s">
         <v>191</v>
       </c>
       <c r="C26" s="52">
@@ -6183,8 +6180,8 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="89" t="s">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="86" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="52">
@@ -6228,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6238,7 +6235,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6296,7 +6293,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6351,7 +6348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6406,7 +6403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6450,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6507,7 +6504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6551,7 +6548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6596,7 +6593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6640,7 +6637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6684,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6728,7 +6725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6741,7 +6738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6751,16 +6748,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="53"/>
-    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="53"/>
+    <col min="1" max="1" width="33.7109375" style="53" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="53"/>
+    <col min="5" max="5" width="17.42578125" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6777,7 +6774,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6795,7 +6792,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6813,7 +6810,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6831,7 +6828,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6849,7 +6846,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6867,7 +6864,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6885,7 +6882,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6903,7 +6900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6921,7 +6918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6939,7 +6936,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6950,7 +6947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -6960,14 +6957,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.85546875" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6999,7 +6996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7035,7 +7032,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7071,7 +7068,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7107,7 +7104,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7143,7 +7140,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7179,7 +7176,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7215,7 +7212,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7251,7 +7248,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7287,7 +7284,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7323,7 +7320,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7359,7 +7356,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7395,7 +7392,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7431,7 +7428,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7467,7 +7464,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7503,7 +7500,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7527,7 +7524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7551,7 +7548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7575,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7599,7 +7596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7623,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7647,7 +7644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7671,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7695,7 +7692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7719,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7743,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7767,7 +7764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7791,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7815,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7839,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7863,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7887,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7911,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7935,7 +7932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7959,7 +7956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7983,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8007,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8031,7 +8028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8055,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8079,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8115,7 +8112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8125,13 +8122,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8155,7 +8152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8178,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8201,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8224,7 +8221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8247,7 +8244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8270,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8293,7 +8290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8316,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8339,7 +8336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8362,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8385,7 +8382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8408,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8431,7 +8428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8454,7 +8451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8477,7 +8474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8500,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8523,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8546,7 +8543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8569,7 +8566,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8592,7 +8589,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8615,7 +8612,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8638,7 +8635,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8661,7 +8658,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8684,7 +8681,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8707,7 +8704,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8730,7 +8727,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8761,7 +8758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8771,13 +8768,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8801,7 +8798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8829,33 +8826,33 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8876,7 +8873,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8897,7 +8894,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8905,7 +8902,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8913,7 +8910,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8941,32 +8938,32 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -8986,7 +8983,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -9006,7 +9003,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9020,7 +9017,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9064,7 +9061,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9108,7 +9105,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9165,14 +9162,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9187,23 +9184,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9227,7 +9224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9250,7 +9247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9270,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9290,7 +9287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9321,7 +9318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9331,13 +9328,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9372,7 +9369,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9389,10 +9386,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9409,10 +9406,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9429,7 +9426,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9443,7 +9440,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9457,7 +9454,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9474,7 +9471,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9488,7 +9485,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9505,7 +9502,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9526,273 +9523,283 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="53"/>
+    <col min="2" max="2" width="19.140625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="86" t="str">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="65"/>
-      <c r="B3" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="86" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="63"/>
+      <c r="B3" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="65"/>
-      <c r="B4" s="64" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="63"/>
+      <c r="B4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="86" t="str">
+      <c r="C4" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="65"/>
-      <c r="B5" s="64" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="63"/>
+      <c r="B5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="86" t="str">
+      <c r="C5" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="92"/>
+      <c r="E5" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="65"/>
-      <c r="B6" s="64" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="63"/>
+      <c r="B6" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="86" t="str">
+      <c r="C6" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="65"/>
-      <c r="B7" s="64" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="63"/>
+      <c r="B7" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="66"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="67" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="64" t="s">
+      <c r="C7" s="94"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="92"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="86" t="str">
+      <c r="C9" s="92"/>
+      <c r="D9" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="65"/>
-      <c r="B10" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="86" t="str">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="63"/>
+      <c r="B10" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="65"/>
-      <c r="B11" s="64" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="63"/>
+      <c r="B11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="86" t="str">
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="65"/>
-      <c r="B12" s="64" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="63"/>
+      <c r="B12" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="86" t="str">
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="65"/>
-      <c r="B13" s="64" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="63"/>
+      <c r="B13" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="86" t="str">
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="65"/>
-      <c r="B14" s="64" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="63"/>
+      <c r="B14" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="66"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" s="64" t="s">
+      <c r="C14" s="94"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="92"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="86" t="str">
+      <c r="C16" s="92"/>
+      <c r="D16" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="65"/>
-      <c r="B17" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="86" t="str">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="63"/>
+      <c r="B17" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="65"/>
-      <c r="B18" s="64" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="63"/>
+      <c r="B18" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" s="86" t="str">
+      <c r="C18" s="92"/>
+      <c r="D18" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="65"/>
-      <c r="B19" s="64" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="63"/>
+      <c r="B19" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="86" t="str">
+      <c r="C19" s="92"/>
+      <c r="D19" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="65"/>
-      <c r="B20" s="64" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="63"/>
+      <c r="B20" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E20" s="86" t="str">
+      <c r="C20" s="92"/>
+      <c r="D20" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="93" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="65"/>
-      <c r="B21" s="64" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="63"/>
+      <c r="B21" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="66"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9801,61 +9808,61 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="88" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="91" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="66"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="91" t="s">
+      <c r="D2" s="92"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="66"/>
+      <c r="D3" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9863,570 +9870,540 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56" style="70" customWidth="1"/>
+    <col min="1" max="1" width="56" style="68" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="53"/>
+    <col min="3" max="3" width="20.42578125" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="53" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="94" t="str">
+      <c r="B1" s="91" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="77" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="70" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="71">
-        <v>0</v>
-      </c>
-      <c r="C2" s="71">
+      <c r="B2" s="69">
+        <v>0</v>
+      </c>
+      <c r="C2" s="69">
         <v>0.95</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="70">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="70" t="s">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="71">
-        <v>0</v>
-      </c>
-      <c r="C3" s="71">
+      <c r="B3" s="69">
+        <v>0</v>
+      </c>
+      <c r="C3" s="69">
         <v>0.95</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="70">
         <v>1</v>
       </c>
       <c r="E3" s="61"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="70" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="71">
-        <v>0</v>
-      </c>
-      <c r="C4" s="71">
+      <c r="B4" s="69">
+        <v>0</v>
+      </c>
+      <c r="C4" s="69">
         <v>0.95</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="70">
         <v>90</v>
       </c>
       <c r="E4" s="61"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="71">
-        <v>0</v>
-      </c>
-      <c r="C5" s="71">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="69">
+        <v>0</v>
+      </c>
+      <c r="C5" s="69">
         <v>0.95</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="71">
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E5" s="76"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="70" t="s">
+      <c r="E5" s="74"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="69">
         <v>0.36</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="69">
         <v>0.95</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="70">
         <v>0.25</v>
       </c>
-      <c r="E6" s="75"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="70" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="71">
-        <v>0</v>
-      </c>
-      <c r="C7" s="71">
+      <c r="E6" s="73"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="86" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="69">
+        <v>0</v>
+      </c>
+      <c r="C7" s="69">
         <v>0.95</v>
       </c>
-      <c r="D7" s="72">
-        <v>0.75</v>
-      </c>
-      <c r="E7" s="75"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="71">
-        <v>0</v>
-      </c>
-      <c r="C8" s="71">
+      <c r="D7" s="70">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="86" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="69">
+        <v>0</v>
+      </c>
+      <c r="C8" s="69">
         <v>0.95</v>
       </c>
-      <c r="D8" s="72">
-        <v>0.19</v>
-      </c>
-      <c r="E8" s="75"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="89" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="71">
-        <v>0</v>
-      </c>
-      <c r="C9" s="71">
+      <c r="D8" s="70">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="86" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="69">
+        <v>0</v>
+      </c>
+      <c r="C9" s="69">
         <v>0.95</v>
       </c>
-      <c r="D9" s="72">
+      <c r="D9" s="70">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="69">
+        <v>0</v>
+      </c>
+      <c r="C10" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D10" s="70">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="69">
+        <v>0</v>
+      </c>
+      <c r="C11" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D11" s="70">
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="89" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" s="71">
-        <v>0</v>
-      </c>
-      <c r="C10" s="71">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="69">
+        <v>0</v>
+      </c>
+      <c r="C12" s="69">
         <v>0.95</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D12" s="70">
         <v>1.78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="89" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="71">
-        <v>0</v>
-      </c>
-      <c r="C11" s="71">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="69">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="C13" s="69">
         <v>0.95</v>
       </c>
-      <c r="D11" s="72">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="89" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" s="71">
-        <v>0</v>
-      </c>
-      <c r="C12" s="71">
+      <c r="D13" s="70">
+        <v>2.06</v>
+      </c>
+      <c r="E13" s="61"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="69">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="C14" s="69">
         <v>0.95</v>
       </c>
-      <c r="D12" s="72">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="71">
-        <v>0</v>
-      </c>
-      <c r="C13" s="71">
+      <c r="D14" s="70">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="61"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="69">
+        <v>0</v>
+      </c>
+      <c r="C15" s="69">
         <v>0.95</v>
       </c>
-      <c r="D13" s="72">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" s="71">
-        <v>0</v>
-      </c>
-      <c r="C14" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D14" s="72">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="71">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="C15" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D15" s="72">
-        <v>2.06</v>
-      </c>
-      <c r="E15" s="61"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="71">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="C16" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D16" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="E16" s="61"/>
-    </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="71">
-        <v>0</v>
-      </c>
-      <c r="C17" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D17" s="88">
+      <c r="D15" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="70" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="71">
-        <v>0</v>
-      </c>
-      <c r="C18" s="71">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="68" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="69">
+        <v>0</v>
+      </c>
+      <c r="C16" s="69">
         <v>0.95</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D16" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>3.78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="B19" s="71">
-        <v>0</v>
-      </c>
-      <c r="C19" s="71">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="68" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="69">
+        <v>0</v>
+      </c>
+      <c r="C17" s="69">
         <v>0.95</v>
       </c>
-      <c r="D19" s="88">
+      <c r="D17" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>14.270000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="71">
-        <v>0</v>
-      </c>
-      <c r="C20" s="71">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="69">
+        <v>0</v>
+      </c>
+      <c r="C18" s="69">
         <v>0.95</v>
       </c>
-      <c r="D20" s="72">
+      <c r="D18" s="70">
         <v>8.84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="70" t="s">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="71">
-        <v>0</v>
-      </c>
-      <c r="C21" s="71">
+      <c r="B19" s="69">
+        <v>0</v>
+      </c>
+      <c r="C19" s="69">
         <v>0.95</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D19" s="70">
         <v>50</v>
       </c>
+      <c r="E19" s="61"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="69">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="C20" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D20" s="70">
+        <v>2.61</v>
+      </c>
+      <c r="E20" s="61"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="69">
+        <v>0</v>
+      </c>
+      <c r="C21" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D21" s="70">
+        <v>1</v>
+      </c>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="71">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="C22" s="71">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="69">
+        <v>0</v>
+      </c>
+      <c r="C22" s="69">
         <v>0.95</v>
       </c>
-      <c r="D22" s="72">
-        <v>2.61</v>
-      </c>
-      <c r="E22" s="61"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="71">
-        <v>0</v>
-      </c>
-      <c r="C23" s="71">
+      <c r="D22" s="70">
+        <v>1</v>
+      </c>
+      <c r="E22" s="72"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="69">
         <v>0.95</v>
       </c>
-      <c r="D23" s="72">
-        <v>1</v>
+      <c r="D23" s="70">
+        <v>4.6500000000000004</v>
       </c>
       <c r="E23" s="61"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="71">
-        <v>0</v>
-      </c>
-      <c r="C24" s="71">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="69">
+        <v>0.3538</v>
+      </c>
+      <c r="C24" s="69">
         <v>0.95</v>
       </c>
-      <c r="D24" s="72">
-        <v>1</v>
-      </c>
-      <c r="E24" s="74"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="C25" s="71">
+      <c r="D24" s="70">
+        <v>3.78</v>
+      </c>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="69">
+        <v>0</v>
+      </c>
+      <c r="C25" s="69">
         <v>0.95</v>
       </c>
-      <c r="D25" s="72">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="E25" s="61"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="70" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="71">
-        <v>0.3538</v>
-      </c>
-      <c r="C26" s="71">
+      <c r="D25" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="69">
+        <v>0</v>
+      </c>
+      <c r="C26" s="69">
         <v>0.95</v>
       </c>
-      <c r="D26" s="72">
-        <v>3.78</v>
-      </c>
-      <c r="E26" s="61"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="71">
-        <v>0</v>
-      </c>
-      <c r="C27" s="71">
+      <c r="D26" s="70">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="69">
+        <v>0</v>
+      </c>
+      <c r="C27" s="69">
         <v>0.95</v>
       </c>
-      <c r="D27" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="70" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="71">
-        <v>0</v>
-      </c>
-      <c r="C28" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D28" s="72">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="71">
-        <v>0</v>
-      </c>
-      <c r="C29" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D29" s="73">
+      <c r="D27" s="71">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="70" t="s">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="71">
+      <c r="B28" s="69">
         <v>0.89970000000000006</v>
       </c>
-      <c r="C30" s="71">
+      <c r="C28" s="69">
         <v>0.95</v>
       </c>
-      <c r="D30" s="72">
+      <c r="D28" s="70">
         <v>0.41</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="70" t="s">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="71">
+      <c r="B29" s="69">
         <v>0.80700000000000005</v>
       </c>
-      <c r="C31" s="71">
+      <c r="C29" s="69">
         <v>0.95</v>
       </c>
-      <c r="D31" s="72">
+      <c r="D29" s="70">
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="70" t="s">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="71">
+      <c r="B30" s="69">
         <v>0.73199999999999998</v>
       </c>
-      <c r="C32" s="71">
+      <c r="C30" s="69">
         <v>0.95</v>
       </c>
-      <c r="D32" s="72">
+      <c r="D30" s="70">
         <v>0.9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="70" t="s">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="71">
+      <c r="B31" s="69">
         <v>0.316</v>
       </c>
-      <c r="C33" s="71">
+      <c r="C31" s="69">
         <v>0.95</v>
       </c>
-      <c r="D33" s="72">
+      <c r="D31" s="70">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="70" t="s">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="71">
+      <c r="B32" s="69">
         <v>0.59699999999999998</v>
       </c>
-      <c r="C34" s="71">
+      <c r="C32" s="69">
         <v>0.95</v>
       </c>
-      <c r="D34" s="72">
+      <c r="D32" s="70">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="70" t="s">
+    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="71">
+      <c r="B33" s="69">
         <v>0.19900000000000001</v>
       </c>
-      <c r="C35" s="71">
+      <c r="C33" s="69">
         <v>0.95</v>
       </c>
-      <c r="D35" s="72">
+      <c r="D33" s="70">
         <v>102</v>
       </c>
-      <c r="F35" s="53"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="70" t="s">
+      <c r="F33" s="53"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="71">
+      <c r="B34" s="69">
         <v>0.13400000000000001</v>
       </c>
-      <c r="C36" s="71">
+      <c r="C34" s="69">
         <v>0.95</v>
       </c>
-      <c r="D36" s="72">
+      <c r="D34" s="70">
         <v>5.53</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="70" t="s">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="71">
-        <v>0</v>
-      </c>
-      <c r="C37" s="71">
+      <c r="B35" s="69">
+        <v>0</v>
+      </c>
+      <c r="C35" s="69">
         <v>0.95</v>
       </c>
-      <c r="D37" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F38" s="54"/>
+      <c r="D35" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="54"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:D35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Ability to read in cost curve type
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0314992-9840-4246-863D-8F203EB7D4A6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21135" windowWidth="28920" windowHeight="16320" tabRatio="961" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,8 @@
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
-    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
+    <sheet name="Cost curve options" sheetId="61" r:id="rId15"/>
+    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
@@ -72,7 +79,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -82,12 +89,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -140,12 +147,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="210">
   <si>
     <t>year</t>
   </si>
@@ -798,19 +805,34 @@
   </si>
   <si>
     <t>Unit cost (US$)</t>
+  </si>
+  <si>
+    <t>Decreasing</t>
+  </si>
+  <si>
+    <t>Increasing</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Constant (default)</t>
+  </si>
+  <si>
+    <t>Marginal cost to coverage relationship</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -938,12 +960,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Arial"/>
@@ -1786,7 +1802,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1935,9 +1951,6 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="3" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1956,7 +1969,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1968,7 +1981,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2698,8 +2711,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -2758,7 +2771,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2815,7 +2828,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2872,7 +2885,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2929,7 +2942,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2986,7 +2999,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3043,7 +3056,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3100,7 +3113,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3157,7 +3170,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3214,7 +3227,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3271,7 +3284,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3328,7 +3341,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3385,7 +3398,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3442,7 +3455,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3499,7 +3512,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3556,7 +3569,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3613,7 +3626,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3670,7 +3683,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3727,7 +3740,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3776,7 +3789,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4139,24 +4152,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4167,42 +4180,42 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="89">
+      <c r="C3" s="86">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="87">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4210,7 +4223,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4218,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4226,7 +4239,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4234,7 +4247,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4242,7 +4255,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4250,17 +4263,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4268,7 +4281,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4276,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4284,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4292,7 +4305,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4301,15 +4314,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4317,7 +4330,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4325,7 +4338,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4333,7 +4346,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4341,18 +4354,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>199</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4360,7 +4373,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4368,7 +4381,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4376,7 +4389,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4384,7 +4397,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4393,20 +4406,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4414,7 +4427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4424,7 +4437,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4434,7 +4447,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4442,7 +4455,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4450,7 +4463,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4458,16 +4471,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4476,7 +4489,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4485,7 +4498,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4495,7 +4508,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4506,16 +4519,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4524,7 +4537,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4532,7 +4545,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4540,7 +4553,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4548,7 +4561,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4556,12 +4569,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4569,7 +4582,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4577,7 +4590,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4587,7 +4600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4597,34 +4610,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="78" customWidth="1"/>
-    <col min="2" max="16384" width="10.85546875" style="78"/>
+    <col min="1" max="1" width="18.6640625" style="75" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="79" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="79" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="77" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="70">
@@ -4638,9 +4651,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="70">
@@ -4655,9 +4668,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
-      <c r="B4" s="80" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="77"/>
+      <c r="B4" s="77" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="70">
@@ -4672,9 +4685,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="77"/>
+      <c r="B5" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="70">
@@ -4689,9 +4702,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="77"/>
+      <c r="B6" s="77" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="70">
@@ -4706,8 +4719,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="79"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4715,7 +4728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4725,15 +4738,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4744,7 +4757,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -4753,7 +4766,7 @@
       </c>
       <c r="C2" s="64"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
@@ -4762,7 +4775,7 @@
       </c>
       <c r="C3" s="64"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="68" t="s">
         <v>58</v>
       </c>
@@ -4771,7 +4784,7 @@
       </c>
       <c r="C4" s="64"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="68" t="s">
         <v>138</v>
       </c>
@@ -4780,28 +4793,28 @@
       </c>
       <c r="C5" s="64"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4812,7 +4825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4822,85 +4835,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="64" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="64" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="64" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="64"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="64"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="64"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="64"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="64"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="64"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="64"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="64"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="64"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="64"/>
     </row>
   </sheetData>
@@ -4910,7 +4923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -4920,9 +4933,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4942,7 +4955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4967,7 +4980,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4992,7 +5005,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5024,29 +5037,29 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5093,7 +5106,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5144,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5188,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
         <v>198</v>
       </c>
@@ -5232,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5278,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5325,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
@@ -5374,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5420,7 +5433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5468,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5512,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
@@ -5561,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5605,10 +5618,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5659,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5704,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5753,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5802,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5850,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5894,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5938,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5986,14 +5999,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="84" t="s">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="83" t="s">
         <v>200</v>
       </c>
       <c r="C23" s="52">
@@ -6036,8 +6049,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="86" t="s">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="83" t="s">
         <v>189</v>
       </c>
       <c r="C24" s="52">
@@ -6084,8 +6097,8 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="86" t="s">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="83" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="52">
@@ -6132,8 +6145,8 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="86" t="s">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="83" t="s">
         <v>191</v>
       </c>
       <c r="C26" s="52">
@@ -6180,8 +6193,8 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="86" t="s">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="83" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="52">
@@ -6225,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6235,7 +6248,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6293,7 +6306,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6348,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6403,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6447,7 +6460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6504,7 +6517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6548,7 +6561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6593,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6637,7 +6650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6681,7 +6694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6725,7 +6738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6738,7 +6751,45 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA98797-1B50-1C46-868B-824E5FEAF95C}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6748,16 +6799,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="53"/>
-    <col min="5" max="5" width="17.42578125" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="53"/>
+    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6774,7 +6825,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6792,7 +6843,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6810,7 +6861,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6828,7 +6879,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6846,7 +6897,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6864,7 +6915,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6882,7 +6933,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6900,7 +6951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6918,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6936,7 +6987,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6947,24 +6998,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.85546875" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6996,7 +7047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7032,7 +7083,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7068,7 +7119,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7104,7 +7155,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7140,7 +7191,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7176,7 +7227,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7212,7 +7263,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7248,7 +7299,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7284,7 +7335,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7320,7 +7371,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7356,7 +7407,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7392,7 +7443,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7428,7 +7479,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7464,7 +7515,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7500,7 +7551,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7524,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7547,8 +7598,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L17" s="20"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7572,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7596,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7620,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7644,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7668,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7692,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7716,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7740,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7764,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7788,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7812,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7836,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7860,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7884,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7908,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7932,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7956,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7980,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8004,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8028,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8052,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8076,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8112,7 +8164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8122,13 +8174,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8152,7 +8204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8175,7 +8227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8198,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8221,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8244,7 +8296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8267,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8290,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8313,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8336,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8359,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8382,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8405,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8428,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8451,7 +8503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8474,7 +8526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8497,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8520,7 +8572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8543,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8566,7 +8618,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8589,7 +8641,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8612,7 +8664,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8635,7 +8687,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8658,7 +8710,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8681,7 +8733,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8704,7 +8756,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8727,7 +8779,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8758,7 +8810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8768,13 +8820,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8798,7 +8850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8826,33 +8878,33 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8873,7 +8925,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8894,7 +8946,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8902,7 +8954,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8910,7 +8962,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8938,32 +8990,32 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -8983,7 +9035,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -9003,7 +9055,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9017,7 +9069,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9061,7 +9113,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9105,7 +9157,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9162,14 +9214,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9184,23 +9236,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9224,7 +9276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9247,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9267,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9287,7 +9339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9318,7 +9370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9328,13 +9380,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9369,7 +9421,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9386,10 +9438,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9406,10 +9458,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9426,7 +9478,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9440,7 +9492,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9454,7 +9506,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9471,7 +9523,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9485,7 +9537,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9502,7 +9554,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9523,25 +9575,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="66" t="s">
         <v>179</v>
       </c>
@@ -9558,248 +9610,252 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="65" t="s">
         <v>174</v>
       </c>
       <c r="B2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93" t="str">
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="63"/>
       <c r="B3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93" t="str">
+      <c r="C3" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="63"/>
       <c r="B4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93" t="str">
+      <c r="C4" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="63"/>
       <c r="B5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="92"/>
-      <c r="E5" s="93" t="str">
+      <c r="C5" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="63"/>
       <c r="B6" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93" t="str">
+      <c r="C6" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="89"/>
+      <c r="E6" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="63"/>
       <c r="B7" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="92"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="91"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="89"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="65" t="s">
         <v>201</v>
       </c>
       <c r="B9" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="93" t="str">
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="63"/>
       <c r="B10" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="93" t="str">
+      <c r="C10" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="63"/>
       <c r="B11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="93" t="str">
+      <c r="C11" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="89"/>
+      <c r="E11" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="63"/>
       <c r="B12" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="93" t="str">
+      <c r="C12" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="89"/>
+      <c r="E12" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="63"/>
       <c r="B13" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="93" t="str">
+      <c r="C13" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="63"/>
       <c r="B14" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="94"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="92"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="91"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="89"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="65" t="s">
         <v>202</v>
       </c>
       <c r="B16" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="93" t="str">
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="63"/>
       <c r="B17" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="93" t="str">
+      <c r="C17" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="63"/>
       <c r="B18" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="93" t="str">
+      <c r="C18" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="63"/>
       <c r="B19" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="93" t="str">
+      <c r="C19" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="63"/>
       <c r="B20" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="93" t="str">
+      <c r="C20" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="89"/>
+      <c r="E20" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="63"/>
       <c r="B21" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="92"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9808,7 +9864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9818,30 +9874,30 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="84" t="s">
         <v>165</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="85" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="85" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="85" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -9850,10 +9906,10 @@
       <c r="C2" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="92"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="88" t="s">
+      <c r="D2" s="89"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="85" t="s">
         <v>186</v>
       </c>
       <c r="B3" s="62" t="s">
@@ -9862,7 +9918,7 @@
       <c r="C3" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9870,41 +9926,45 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" style="68" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.42578125" style="53"/>
+    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+      <c r="A1" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="91" t="str">
+      <c r="B1" s="88" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="72" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="68" t="s">
         <v>29</v>
       </c>
@@ -9917,8 +9977,11 @@
       <c r="D2" s="70">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="70" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="68" t="s">
         <v>86</v>
       </c>
@@ -9931,9 +9994,11 @@
       <c r="D3" s="70">
         <v>1</v>
       </c>
-      <c r="E3" s="61"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="68" t="s">
         <v>61</v>
       </c>
@@ -9946,9 +10011,11 @@
       <c r="D4" s="70">
         <v>90</v>
       </c>
-      <c r="E4" s="61"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="68" t="s">
         <v>200</v>
       </c>
@@ -9962,9 +10029,11 @@
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E5" s="74"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="68" t="s">
         <v>63</v>
       </c>
@@ -9977,10 +10046,12 @@
       <c r="D6" s="70">
         <v>0.25</v>
       </c>
-      <c r="E6" s="73"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="86" t="s">
+      <c r="E6" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="83" t="s">
         <v>189</v>
       </c>
       <c r="B7" s="69">
@@ -9992,9 +10063,12 @@
       <c r="D7" s="70">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="86" t="s">
+      <c r="E7" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="83" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="69">
@@ -10006,9 +10080,12 @@
       <c r="D8" s="70">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86" t="s">
+      <c r="E8" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="83" t="s">
         <v>191</v>
       </c>
       <c r="B9" s="69">
@@ -10020,9 +10097,12 @@
       <c r="D9" s="70">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="86" t="s">
+      <c r="E9" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="83" t="s">
         <v>192</v>
       </c>
       <c r="B10" s="69">
@@ -10034,8 +10114,11 @@
       <c r="D10" s="70">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>188</v>
       </c>
@@ -10048,8 +10131,11 @@
       <c r="D11" s="70">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
         <v>193</v>
       </c>
@@ -10062,8 +10148,11 @@
       <c r="D12" s="70">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="68" t="s">
         <v>57</v>
       </c>
@@ -10076,9 +10165,11 @@
       <c r="D13" s="70">
         <v>2.06</v>
       </c>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="68" t="s">
         <v>47</v>
       </c>
@@ -10091,9 +10182,11 @@
       <c r="D14" s="70">
         <v>0.05</v>
       </c>
-      <c r="E14" s="61"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="68" t="s">
         <v>174</v>
       </c>
@@ -10103,12 +10196,15 @@
       <c r="C15" s="69">
         <v>0.95</v>
       </c>
-      <c r="D15" s="85">
+      <c r="D15" s="82">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="68" t="s">
         <v>201</v>
       </c>
@@ -10118,12 +10214,15 @@
       <c r="C16" s="69">
         <v>0.95</v>
       </c>
-      <c r="D16" s="85">
+      <c r="D16" s="82">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.66</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="68" t="s">
         <v>202</v>
       </c>
@@ -10133,12 +10232,15 @@
       <c r="C17" s="69">
         <v>0.95</v>
       </c>
-      <c r="D17" s="85">
+      <c r="D17" s="82">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
-        <v>14.270000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.66</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="68" t="s">
         <v>198</v>
       </c>
@@ -10151,8 +10253,11 @@
       <c r="D18" s="70">
         <v>8.84</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="68" t="s">
         <v>137</v>
       </c>
@@ -10165,9 +10270,11 @@
       <c r="D19" s="70">
         <v>50</v>
       </c>
-      <c r="E19" s="61"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="68" t="s">
         <v>34</v>
       </c>
@@ -10180,9 +10287,11 @@
       <c r="D20" s="70">
         <v>2.61</v>
       </c>
-      <c r="E20" s="61"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="68" t="s">
         <v>88</v>
       </c>
@@ -10195,9 +10304,11 @@
       <c r="D21" s="70">
         <v>1</v>
       </c>
-      <c r="E21" s="61"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="68" t="s">
         <v>87</v>
       </c>
@@ -10210,9 +10321,11 @@
       <c r="D22" s="70">
         <v>1</v>
       </c>
-      <c r="E22" s="72"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="68" t="s">
         <v>138</v>
       </c>
@@ -10225,9 +10338,11 @@
       <c r="D23" s="70">
         <v>4.6500000000000004</v>
       </c>
-      <c r="E23" s="61"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="68" t="s">
         <v>59</v>
       </c>
@@ -10240,9 +10355,11 @@
       <c r="D24" s="70">
         <v>3.78</v>
       </c>
-      <c r="E24" s="61"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="68" t="s">
         <v>84</v>
       </c>
@@ -10255,8 +10372,11 @@
       <c r="D25" s="70">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="68" t="s">
         <v>58</v>
       </c>
@@ -10269,8 +10389,11 @@
       <c r="D26" s="70">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="68" t="s">
         <v>67</v>
       </c>
@@ -10284,8 +10407,11 @@
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="68" t="s">
         <v>28</v>
       </c>
@@ -10298,8 +10424,11 @@
       <c r="D28" s="70">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="68" t="s">
         <v>83</v>
       </c>
@@ -10312,8 +10441,11 @@
       <c r="D29" s="70">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="68" t="s">
         <v>82</v>
       </c>
@@ -10326,8 +10458,11 @@
       <c r="D30" s="70">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="68" t="s">
         <v>81</v>
       </c>
@@ -10340,8 +10475,11 @@
       <c r="D31" s="70">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="68" t="s">
         <v>79</v>
       </c>
@@ -10354,8 +10492,11 @@
       <c r="D32" s="70">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="68" t="s">
         <v>80</v>
       </c>
@@ -10368,9 +10509,12 @@
       <c r="D33" s="70">
         <v>102</v>
       </c>
+      <c r="E33" s="70" t="s">
+        <v>208</v>
+      </c>
       <c r="F33" s="53"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="68" t="s">
         <v>85</v>
       </c>
@@ -10383,8 +10527,11 @@
       <c r="D34" s="70">
         <v>5.53</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="70" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="68" t="s">
         <v>60</v>
       </c>
@@ -10397,8 +10544,11 @@
       <c r="D35" s="70">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F36" s="54"/>
     </row>
   </sheetData>
@@ -10407,5 +10557,17 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E3893C6-1CD6-D045-8057-77412F55397B}">
+          <x14:formula1>
+            <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E35</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hid tab, set all to constant by default
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0314992-9840-4246-863D-8F203EB7D4A6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0064327A-C7AE-F14C-953C-BBBAFF95EA77}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
-    <sheet name="Cost curve options" sheetId="61" r:id="rId15"/>
+    <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
     <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -6758,7 +6758,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6770,12 +6770,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
@@ -9933,7 +9933,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9995,7 +9995,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10012,7 +10012,7 @@
         <v>90</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10030,7 +10030,7 @@
         <v>0.82100000000000006</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10047,7 +10047,7 @@
         <v>0.25</v>
       </c>
       <c r="E6" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10064,7 +10064,7 @@
         <v>0.73</v>
       </c>
       <c r="E7" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10081,7 +10081,7 @@
         <v>1.78</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10166,7 +10166,7 @@
         <v>2.06</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10201,7 +10201,7 @@
         <v>3.66</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10219,7 +10219,7 @@
         <v>3.66</v>
       </c>
       <c r="E16" s="70" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10237,7 +10237,7 @@
         <v>3.66</v>
       </c>
       <c r="E17" s="70" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10425,7 +10425,7 @@
         <v>0.41</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10528,7 +10528,7 @@
         <v>5.53</v>
       </c>
       <c r="E34" s="70" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated demo and template to contain flexible cost curves
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3238136D-D270-8B4C-AEA6-E1F786808966}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{364FF543-F739-8D4B-A508-18C935E44CDC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
-    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
+    <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
+    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
   <si>
     <t>year</t>
   </si>
@@ -807,6 +808,21 @@
   </si>
   <si>
     <t>Unit cost (US$)</t>
+  </si>
+  <si>
+    <t>Constant (default)</t>
+  </si>
+  <si>
+    <t>Increasing</t>
+  </si>
+  <si>
+    <t>Decreasing</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Marginal cost to coverage relationship</t>
   </si>
 </sst>
 </file>
@@ -819,7 +835,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -947,12 +963,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Arial"/>
@@ -1795,7 +1805,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1946,9 +1956,6 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="3" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1962,13 +1969,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4182,7 +4189,7 @@
       <c r="B3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="92">
+      <c r="C3" s="89">
         <v>2017</v>
       </c>
     </row>
@@ -4191,7 +4198,7 @@
       <c r="B4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="90">
         <v>2030</v>
       </c>
     </row>
@@ -4602,32 +4609,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="80" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="80"/>
+    <col min="1" max="1" width="18.6640625" style="77" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="82" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="81" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="81" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="81" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="79" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="72">
@@ -4642,8 +4649,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="82"/>
-      <c r="B3" s="82" t="s">
+      <c r="A3" s="79"/>
+      <c r="B3" s="79" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="72">
@@ -4659,8 +4666,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="82"/>
-      <c r="B4" s="82" t="s">
+      <c r="A4" s="79"/>
+      <c r="B4" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="72">
@@ -4676,8 +4683,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82" t="s">
+      <c r="A5" s="79"/>
+      <c r="B5" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="72">
@@ -4693,8 +4700,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="79"/>
+      <c r="B6" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="72">
@@ -4710,7 +4717,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="81"/>
+      <c r="C9" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5993,10 +6000,10 @@
       <c r="B22" s="49"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="86" t="s">
         <v>201</v>
       </c>
       <c r="C23" s="52">
@@ -6040,7 +6047,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="86" t="s">
         <v>189</v>
       </c>
       <c r="C24" s="52">
@@ -6088,7 +6095,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="86" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="52">
@@ -6136,7 +6143,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="86" t="s">
         <v>191</v>
       </c>
       <c r="C26" s="52">
@@ -6184,7 +6191,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="86" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="52">
@@ -6741,6 +6748,41 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D421F3D-2276-E54C-B883-DD4D8338F3A2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -9570,7 +9612,7 @@
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
-      <c r="E2" s="86" t="str">
+      <c r="E2" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9584,7 +9626,7 @@
         <v>197</v>
       </c>
       <c r="D3" s="66"/>
-      <c r="E3" s="86" t="str">
+      <c r="E3" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9598,7 +9640,7 @@
         <v>197</v>
       </c>
       <c r="D4" s="66"/>
-      <c r="E4" s="86" t="str">
+      <c r="E4" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9612,7 +9654,7 @@
         <v>197</v>
       </c>
       <c r="D5" s="66"/>
-      <c r="E5" s="86" t="str">
+      <c r="E5" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9626,7 +9668,7 @@
         <v>197</v>
       </c>
       <c r="D6" s="66"/>
-      <c r="E6" s="86" t="str">
+      <c r="E6" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9651,7 +9693,7 @@
       <c r="D9" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="86" t="str">
+      <c r="E9" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9663,7 +9705,7 @@
       </c>
       <c r="C10" s="66"/>
       <c r="D10" s="66"/>
-      <c r="E10" s="86" t="str">
+      <c r="E10" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9675,7 +9717,7 @@
       </c>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
-      <c r="E11" s="86" t="str">
+      <c r="E11" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9687,7 +9729,7 @@
       </c>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
-      <c r="E12" s="86" t="str">
+      <c r="E12" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9699,7 +9741,7 @@
       </c>
       <c r="C13" s="66"/>
       <c r="D13" s="66"/>
-      <c r="E13" s="86" t="str">
+      <c r="E13" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9724,7 +9766,7 @@
       <c r="D16" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E16" s="86" t="str">
+      <c r="E16" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9738,7 +9780,7 @@
       <c r="D17" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E17" s="86" t="str">
+      <c r="E17" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9752,7 +9794,7 @@
       <c r="D18" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E18" s="86" t="str">
+      <c r="E18" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9766,7 +9808,7 @@
       <c r="D19" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="86" t="str">
+      <c r="E19" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9780,7 +9822,7 @@
       <c r="D20" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E20" s="86" t="str">
+      <c r="E20" s="83" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
@@ -9820,21 +9862,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="87" t="s">
         <v>165</v>
       </c>
       <c r="B1" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="88" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="88" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="64" t="s">
@@ -9846,7 +9888,7 @@
       <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="88" t="s">
         <v>186</v>
       </c>
       <c r="B3" s="64" t="s">
@@ -9870,7 +9912,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9879,22 +9921,26 @@
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="53"/>
+    <col min="5" max="5" width="18.6640625" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+      <c r="A1" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="94" t="str">
+      <c r="B1" s="91" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="74" t="s">
         <v>205</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9910,6 +9956,9 @@
       <c r="D2" s="72">
         <v>25</v>
       </c>
+      <c r="E2" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
@@ -9924,7 +9973,9 @@
       <c r="D3" s="72">
         <v>1</v>
       </c>
-      <c r="E3" s="61"/>
+      <c r="E3" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
@@ -9939,7 +9990,9 @@
       <c r="D4" s="72">
         <v>90</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
@@ -9955,7 +10008,9 @@
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70" t="s">
@@ -9970,7 +10025,9 @@
       <c r="D6" s="72">
         <v>0.25</v>
       </c>
-      <c r="E6" s="75"/>
+      <c r="E6" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
@@ -9985,7 +10042,9 @@
       <c r="D7" s="72">
         <v>0.75</v>
       </c>
-      <c r="E7" s="75"/>
+      <c r="E7" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
@@ -10000,10 +10059,12 @@
       <c r="D8" s="72">
         <v>0.19</v>
       </c>
-      <c r="E8" s="75"/>
+      <c r="E8" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="86" t="s">
         <v>189</v>
       </c>
       <c r="B9" s="71">
@@ -10015,9 +10076,12 @@
       <c r="D9" s="72">
         <v>0.73</v>
       </c>
+      <c r="E9" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="86" t="s">
         <v>190</v>
       </c>
       <c r="B10" s="71">
@@ -10029,9 +10093,12 @@
       <c r="D10" s="72">
         <v>1.78</v>
       </c>
+      <c r="E10" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="86" t="s">
         <v>191</v>
       </c>
       <c r="B11" s="71">
@@ -10043,9 +10110,12 @@
       <c r="D11" s="72">
         <v>0.24</v>
       </c>
+      <c r="E11" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="86" t="s">
         <v>192</v>
       </c>
       <c r="B12" s="71">
@@ -10056,6 +10126,9 @@
       </c>
       <c r="D12" s="72">
         <v>0.55000000000000004</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10071,6 +10144,9 @@
       <c r="D13" s="72">
         <v>0.73</v>
       </c>
+      <c r="E13" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
@@ -10085,6 +10161,9 @@
       <c r="D14" s="72">
         <v>1.78</v>
       </c>
+      <c r="E14" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
@@ -10099,7 +10178,9 @@
       <c r="D15" s="72">
         <v>2.06</v>
       </c>
-      <c r="E15" s="61"/>
+      <c r="E15" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
@@ -10114,7 +10195,9 @@
       <c r="D16" s="72">
         <v>0.05</v>
       </c>
-      <c r="E16" s="61"/>
+      <c r="E16" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
@@ -10126,9 +10209,12 @@
       <c r="C17" s="71">
         <v>0.95</v>
       </c>
-      <c r="D17" s="88">
+      <c r="D17" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10141,9 +10227,12 @@
       <c r="C18" s="71">
         <v>0.95</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>3.78</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10156,9 +10245,12 @@
       <c r="C19" s="71">
         <v>0.95</v>
       </c>
-      <c r="D19" s="88">
+      <c r="D19" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>14.270000000000001</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10174,6 +10266,9 @@
       <c r="D20" s="72">
         <v>8.84</v>
       </c>
+      <c r="E20" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
@@ -10188,7 +10283,9 @@
       <c r="D21" s="72">
         <v>50</v>
       </c>
-      <c r="E21" s="61"/>
+      <c r="E21" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
@@ -10203,7 +10300,9 @@
       <c r="D22" s="72">
         <v>2.61</v>
       </c>
-      <c r="E22" s="61"/>
+      <c r="E22" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
@@ -10218,7 +10317,9 @@
       <c r="D23" s="72">
         <v>1</v>
       </c>
-      <c r="E23" s="61"/>
+      <c r="E23" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
@@ -10233,7 +10334,9 @@
       <c r="D24" s="72">
         <v>1</v>
       </c>
-      <c r="E24" s="74"/>
+      <c r="E24" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
@@ -10248,7 +10351,9 @@
       <c r="D25" s="72">
         <v>4.6500000000000004</v>
       </c>
-      <c r="E25" s="61"/>
+      <c r="E25" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
@@ -10263,7 +10368,9 @@
       <c r="D26" s="72">
         <v>3.78</v>
       </c>
-      <c r="E26" s="61"/>
+      <c r="E26" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="70" t="s">
@@ -10278,6 +10385,9 @@
       <c r="D27" s="72">
         <v>1</v>
       </c>
+      <c r="E27" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="70" t="s">
@@ -10292,6 +10402,9 @@
       <c r="D28" s="72">
         <v>48</v>
       </c>
+      <c r="E28" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="70" t="s">
@@ -10307,6 +10420,9 @@
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
+      <c r="E29" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="70" t="s">
@@ -10321,6 +10437,9 @@
       <c r="D30" s="72">
         <v>0.41</v>
       </c>
+      <c r="E30" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
@@ -10335,6 +10454,9 @@
       <c r="D31" s="72">
         <v>0.9</v>
       </c>
+      <c r="E31" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
@@ -10349,6 +10471,9 @@
       <c r="D32" s="72">
         <v>0.9</v>
       </c>
+      <c r="E32" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
@@ -10363,6 +10488,9 @@
       <c r="D33" s="72">
         <v>79</v>
       </c>
+      <c r="E33" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
@@ -10377,6 +10505,9 @@
       <c r="D34" s="72">
         <v>31</v>
       </c>
+      <c r="E34" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="35" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
@@ -10391,6 +10522,9 @@
       <c r="D35" s="72">
         <v>102</v>
       </c>
+      <c r="E35" s="72" t="s">
+        <v>206</v>
+      </c>
       <c r="F35" s="53"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10406,6 +10540,9 @@
       <c r="D36" s="72">
         <v>5.53</v>
       </c>
+      <c r="E36" s="72" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
@@ -10419,6 +10556,9 @@
       </c>
       <c r="D37" s="72">
         <v>1</v>
+      </c>
+      <c r="E37" s="72" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10430,5 +10570,17 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4A8EF9C-69C5-FA47-B4F0-310AA7683106}">
+          <x14:formula1>
+            <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E37</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delayed cord clamping in cost and coverages tab
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A813F76-0C1B-FF4B-865D-DB1C574DB473}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8EA6519C-9000-5848-956E-B5C84169DE75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="211">
   <si>
     <t>year</t>
   </si>
@@ -5041,7 +5041,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9909,7 +9909,7 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9994,7 +9994,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B5" s="71">
         <v>0</v>
@@ -10002,43 +10002,43 @@
       <c r="C5" s="71">
         <v>0.95</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="72">
+        <v>1</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="71">
+        <v>0</v>
+      </c>
+      <c r="C6" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="73">
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E5" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="71">
-        <v>0.36</v>
-      </c>
-      <c r="C6" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D6" s="72">
-        <v>0.25</v>
-      </c>
       <c r="E6" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="71">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C7" s="71">
         <v>0.95</v>
       </c>
       <c r="D7" s="72">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="E7" s="72" t="s">
         <v>206</v>
@@ -10046,7 +10046,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8" s="71">
         <v>0</v>
@@ -10055,15 +10055,15 @@
         <v>0.95</v>
       </c>
       <c r="D8" s="72">
-        <v>0.19</v>
+        <v>0.75</v>
       </c>
       <c r="E8" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="86" t="s">
-        <v>189</v>
+      <c r="A9" s="70" t="s">
+        <v>62</v>
       </c>
       <c r="B9" s="71">
         <v>0</v>
@@ -10072,7 +10072,7 @@
         <v>0.95</v>
       </c>
       <c r="D9" s="72">
-        <v>0.73</v>
+        <v>0.19</v>
       </c>
       <c r="E9" s="72" t="s">
         <v>206</v>
@@ -10080,7 +10080,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -10089,7 +10089,7 @@
         <v>0.95</v>
       </c>
       <c r="D10" s="72">
-        <v>1.78</v>
+        <v>0.73</v>
       </c>
       <c r="E10" s="72" t="s">
         <v>206</v>
@@ -10097,7 +10097,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="86" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -10106,7 +10106,7 @@
         <v>0.95</v>
       </c>
       <c r="D11" s="72">
-        <v>0.24</v>
+        <v>1.78</v>
       </c>
       <c r="E11" s="72" t="s">
         <v>206</v>
@@ -10114,7 +10114,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -10123,15 +10123,15 @@
         <v>0.95</v>
       </c>
       <c r="D12" s="72">
-        <v>0.55000000000000004</v>
+        <v>0.24</v>
       </c>
       <c r="E12" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14" t="s">
-        <v>188</v>
+      <c r="A13" s="86" t="s">
+        <v>192</v>
       </c>
       <c r="B13" s="71">
         <v>0</v>
@@ -10140,7 +10140,7 @@
         <v>0.95</v>
       </c>
       <c r="D13" s="72">
-        <v>0.73</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="72" t="s">
         <v>206</v>
@@ -10148,7 +10148,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B14" s="71">
         <v>0</v>
@@ -10157,24 +10157,24 @@
         <v>0.95</v>
       </c>
       <c r="D14" s="72">
-        <v>1.78</v>
+        <v>0.73</v>
       </c>
       <c r="E14" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="70" t="s">
-        <v>57</v>
+      <c r="A15" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="B15" s="71">
-        <v>0.34599999999999997</v>
+        <v>0</v>
       </c>
       <c r="C15" s="71">
         <v>0.95</v>
       </c>
       <c r="D15" s="72">
-        <v>2.06</v>
+        <v>1.78</v>
       </c>
       <c r="E15" s="72" t="s">
         <v>206</v>
@@ -10182,95 +10182,95 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B16" s="71">
-        <v>0.80800000000000005</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C16" s="71">
         <v>0.95</v>
       </c>
       <c r="D16" s="72">
-        <v>0.05</v>
+        <v>2.06</v>
       </c>
       <c r="E16" s="72" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>174</v>
+        <v>47</v>
       </c>
       <c r="B17" s="71">
-        <v>0</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="C17" s="71">
         <v>0.95</v>
       </c>
-      <c r="D17" s="85">
+      <c r="D17" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="71">
+        <v>0</v>
+      </c>
+      <c r="C18" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D18" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
-      <c r="E17" s="72" t="s">
+      <c r="E18" s="72" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="70" t="s">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="71">
-        <v>0</v>
-      </c>
-      <c r="C18" s="71">
+      <c r="B19" s="71">
+        <v>0</v>
+      </c>
+      <c r="C19" s="71">
         <v>0.95</v>
       </c>
-      <c r="D18" s="85">
+      <c r="D19" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>3.78</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E19" s="72" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="70" t="s">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="B19" s="71">
-        <v>0</v>
-      </c>
-      <c r="C19" s="71">
+      <c r="B20" s="71">
+        <v>0</v>
+      </c>
+      <c r="C20" s="71">
         <v>0.95</v>
       </c>
-      <c r="D19" s="85">
+      <c r="D20" s="85">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>14.270000000000001</v>
       </c>
-      <c r="E19" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="71">
-        <v>0</v>
-      </c>
-      <c r="C20" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D20" s="72">
-        <v>8.84</v>
-      </c>
       <c r="E20" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="B21" s="71">
         <v>0</v>
@@ -10279,7 +10279,7 @@
         <v>0.95</v>
       </c>
       <c r="D21" s="72">
-        <v>50</v>
+        <v>8.84</v>
       </c>
       <c r="E21" s="72" t="s">
         <v>206</v>
@@ -10287,16 +10287,16 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="B22" s="71">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C22" s="71">
         <v>0.95</v>
       </c>
       <c r="D22" s="72">
-        <v>2.61</v>
+        <v>50</v>
       </c>
       <c r="E22" s="72" t="s">
         <v>206</v>
@@ -10304,16 +10304,16 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="B23" s="71">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
       </c>
       <c r="D23" s="72">
-        <v>1</v>
+        <v>2.61</v>
       </c>
       <c r="E23" s="72" t="s">
         <v>206</v>
@@ -10321,7 +10321,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B24" s="71">
         <v>0</v>
@@ -10338,16 +10338,16 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B25" s="71">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="71">
         <v>0.95</v>
       </c>
       <c r="D25" s="72">
-        <v>4.6500000000000004</v>
+        <v>1</v>
       </c>
       <c r="E25" s="72" t="s">
         <v>206</v>
@@ -10355,16 +10355,16 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="B26" s="71">
-        <v>0.3538</v>
+        <v>0.1</v>
       </c>
       <c r="C26" s="71">
         <v>0.95</v>
       </c>
       <c r="D26" s="72">
-        <v>3.78</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E26" s="72" t="s">
         <v>206</v>
@@ -10372,16 +10372,16 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="70" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B27" s="71">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C27" s="71">
         <v>0.95</v>
       </c>
       <c r="D27" s="72">
-        <v>1</v>
+        <v>3.78</v>
       </c>
       <c r="E27" s="72" t="s">
         <v>206</v>
@@ -10389,7 +10389,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="70" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B28" s="71">
         <v>0</v>
@@ -10398,7 +10398,7 @@
         <v>0.95</v>
       </c>
       <c r="D28" s="72">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E28" s="72" t="s">
         <v>206</v>
@@ -10406,7 +10406,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="70" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B29" s="71">
         <v>0</v>
@@ -10414,43 +10414,43 @@
       <c r="C29" s="71">
         <v>0.95</v>
       </c>
-      <c r="D29" s="73">
+      <c r="D29" s="72">
+        <v>48</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="71">
+        <v>0</v>
+      </c>
+      <c r="C30" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D30" s="73">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
-      <c r="E29" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="71">
-        <v>0.89970000000000006</v>
-      </c>
-      <c r="C30" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D30" s="72">
-        <v>0.41</v>
-      </c>
       <c r="E30" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B31" s="71">
-        <v>0.80700000000000005</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
       </c>
       <c r="D31" s="72">
-        <v>0.9</v>
+        <v>0.41</v>
       </c>
       <c r="E31" s="72" t="s">
         <v>206</v>
@@ -10458,10 +10458,10 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B32" s="71">
-        <v>0.73199999999999998</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
@@ -10475,16 +10475,16 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B33" s="71">
-        <v>0.316</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
       </c>
       <c r="D33" s="72">
-        <v>79</v>
+        <v>0.9</v>
       </c>
       <c r="E33" s="72" t="s">
         <v>206</v>
@@ -10492,79 +10492,96 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B34" s="71">
-        <v>0.59699999999999998</v>
+        <v>0.316</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>
       </c>
       <c r="D34" s="72">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E34" s="72" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="71">
-        <v>0.19900000000000001</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C35" s="71">
         <v>0.95</v>
       </c>
       <c r="D35" s="72">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="E35" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="F35" s="53"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B36" s="71">
-        <v>0.13400000000000001</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C36" s="71">
         <v>0.95</v>
       </c>
       <c r="D36" s="72">
-        <v>5.53</v>
+        <v>102</v>
       </c>
       <c r="E36" s="72" t="s">
         <v>206</v>
       </c>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B37" s="71">
-        <v>0</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="C37" s="71">
         <v>0.95</v>
       </c>
       <c r="D37" s="72">
-        <v>1</v>
+        <v>5.53</v>
       </c>
       <c r="E37" s="72" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F38" s="54"/>
+      <c r="A38" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="71">
+        <v>0</v>
+      </c>
+      <c r="C38" s="71">
+        <v>0.95</v>
+      </c>
+      <c r="D38" s="72">
+        <v>1</v>
+      </c>
+      <c r="E38" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F39" s="54"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D37">
-    <sortCondition ref="A2:A37"/>
+  <sortState ref="A2:D38">
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10575,7 +10592,7 @@
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E37</xm:sqref>
+          <xm:sqref>E2:E38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated curve names in sheets
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8EA6519C-9000-5848-956E-B5C84169DE75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{84F7FCCC-A3AC-B943-9D80-E69126E57DD5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,19 +810,19 @@
     <t>Unit cost (US$)</t>
   </si>
   <si>
-    <t>Constant (default)</t>
-  </si>
-  <si>
-    <t>Increasing</t>
-  </si>
-  <si>
-    <t>Decreasing</t>
-  </si>
-  <si>
-    <t>Mixed</t>
-  </si>
-  <si>
-    <t>Marginal costs</t>
+    <t>Linear (constant marginal cost) [default]</t>
+  </si>
+  <si>
+    <t>Curved with increasing marginal cost</t>
+  </si>
+  <si>
+    <t>Curved with decreasing marginal cost</t>
+  </si>
+  <si>
+    <t>S-shaped (decreasing then increasing marginal cost)</t>
+  </si>
+  <si>
+    <t>Cost-coverage relationship</t>
   </si>
 </sst>
 </file>
@@ -6751,9 +6751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D421F3D-2276-E54C-B883-DD4D8338F3A2}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -9911,7 +9909,9 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9919,7 +9919,7 @@
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="53" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="53" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Changed fractions eating to avoid 0 pop
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{84F7FCCC-A3AC-B943-9D80-E69126E57DD5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF585BFD-6A36-A846-BE93-4A42CEE302C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4157,7 +4157,9 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4283,7 +4285,7 @@
         <v>95</v>
       </c>
       <c r="C16" s="23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4291,7 +4293,7 @@
         <v>96</v>
       </c>
       <c r="C17" s="23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4308,7 +4310,7 @@
       </c>
       <c r="C19" s="26">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
-        <v>0.19999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6315,47 +6317,47 @@
       </c>
       <c r="E30" s="51">
         <f t="shared" ref="E30:O30" si="1">frac_rice</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="O30" s="51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6370,47 +6372,47 @@
       </c>
       <c r="E31" s="51">
         <f t="shared" ref="E31:O31" si="2">frac_wheat</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="O31" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Comments for program costs
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\national\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF585BFD-6A36-A846-BE93-4A42CEE302C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15540" tabRatio="961" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -89,12 +88,100 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nick Scott</author>
+  </authors>
+  <commentList>
+    <comment ref="D28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The cost per child per year can be estimated as 
+= (cost per treatment) * (annual diarrhoea incidence)
+Diarrhoea incidence is the average in children under 5.  See user guide for further information</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The cost per child per year can be estimated as 
+= (cost per treatment episode) * (SAM prevalence) * 2.6
+Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The cost per child per year can be estimated as 
+= (cost per treatment) * (annual diarrhoea incidence)
+Diarrhoea incidence is the average in children under 5.  See user guide for further information</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,13 +233,13 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -807,9 +894,6 @@
     <t>Saturation coverage of target population</t>
   </si>
   <si>
-    <t>Unit cost (US$)</t>
-  </si>
-  <si>
     <t>Linear (constant marginal cost) [default]</t>
   </si>
   <si>
@@ -823,19 +907,22 @@
   </si>
   <si>
     <t>Cost-coverage relationship</t>
+  </si>
+  <si>
+    <t>Unit cost (US$ per person per year)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -974,6 +1061,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1086,7 +1186,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1805,7 +1905,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1848,8 +1948,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1865,8 +1965,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1885,20 +1985,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1910,11 +2010,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1944,7 +2044,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1955,8 +2055,6 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1969,7 +2067,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2710,8 +2808,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 2" xfId="725"/>
+    <cellStyle name="Normal 3" xfId="726"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -4151,24 +4249,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="15"/>
+    <col min="3" max="16384" width="14.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4179,42 +4277,42 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="89">
+      <c r="C3" s="87">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="88">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4222,7 +4320,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4230,7 +4328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4238,7 +4336,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4246,7 +4344,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4254,7 +4352,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4262,17 +4360,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4280,7 +4378,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4288,7 +4386,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4296,7 +4394,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4304,7 +4402,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4313,15 +4411,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4329,7 +4427,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4337,7 +4435,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4345,7 +4443,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4353,18 +4451,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>200</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4372,7 +4470,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4380,7 +4478,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4388,7 +4486,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4396,7 +4494,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4405,20 +4503,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4426,7 +4524,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4436,7 +4534,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4446,7 +4544,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4454,7 +4552,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4462,7 +4560,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4470,16 +4568,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4488,7 +4586,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4497,7 +4595,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4507,7 +4605,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4518,16 +4616,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4536,7 +4634,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4544,7 +4642,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4552,7 +4650,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4560,7 +4658,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4568,12 +4666,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4581,7 +4679,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4589,7 +4687,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4599,7 +4697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4609,34 +4707,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="77" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="77"/>
+    <col min="1" max="1" width="18.6640625" style="75" customWidth="1"/>
+    <col min="2" max="16384" width="10.77734375" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="79" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="79" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="78" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="77" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="72">
@@ -4650,9 +4748,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="72">
@@ -4667,9 +4765,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="79"/>
-      <c r="B4" s="79" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="77"/>
+      <c r="B4" s="77" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="72">
@@ -4684,9 +4782,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="77"/>
+      <c r="B5" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="72">
@@ -4701,9 +4799,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="77"/>
+      <c r="B6" s="77" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="72">
@@ -4718,8 +4816,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="78"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4727,7 +4825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4737,15 +4835,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="53"/>
+    <col min="2" max="2" width="47.77734375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4756,7 +4854,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -4765,7 +4863,7 @@
       </c>
       <c r="C2" s="66"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
@@ -4774,7 +4872,7 @@
       </c>
       <c r="C3" s="66"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>58</v>
       </c>
@@ -4783,7 +4881,7 @@
       </c>
       <c r="C4" s="66"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
         <v>138</v>
       </c>
@@ -4792,28 +4890,28 @@
       </c>
       <c r="C5" s="66"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4824,7 +4922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4834,85 +4932,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="53"/>
+    <col min="1" max="1" width="30.109375" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="66"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="66"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="66"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="66"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="66"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="66"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="66"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="66"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="66"/>
     </row>
   </sheetData>
@@ -4922,7 +5020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -4932,9 +5030,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4954,7 +5052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4979,7 +5077,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -5004,7 +5102,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5036,7 +5134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5046,19 +5144,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5105,7 +5203,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5156,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5200,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>199</v>
       </c>
@@ -5244,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5290,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5337,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
@@ -5386,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5432,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5480,7 +5578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5524,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
@@ -5573,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5617,10 +5715,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5671,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5716,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5765,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5814,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5862,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5906,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5950,7 +6048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5998,14 +6096,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="84" t="s">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="84" t="s">
         <v>201</v>
       </c>
       <c r="C23" s="52">
@@ -6048,8 +6146,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="86" t="s">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="84" t="s">
         <v>189</v>
       </c>
       <c r="C24" s="52">
@@ -6096,8 +6194,8 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="86" t="s">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="84" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="52">
@@ -6144,8 +6242,8 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="86" t="s">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="84" t="s">
         <v>191</v>
       </c>
       <c r="C26" s="52">
@@ -6192,8 +6290,8 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="86" t="s">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="84" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="52">
@@ -6237,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6247,7 +6345,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6305,7 +6403,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6360,7 +6458,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6415,7 +6513,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6459,7 +6557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6516,7 +6614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6560,7 +6658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6605,7 +6703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6649,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6693,7 +6791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6737,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6750,31 +6848,31 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D421F3D-2276-E54C-B883-DD4D8338F3A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="15" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -6783,7 +6881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6793,16 +6891,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="53"/>
-    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="53"/>
+    <col min="2" max="2" width="12.44140625" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="53"/>
+    <col min="5" max="5" width="17.44140625" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6819,7 +6917,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6837,7 +6935,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6855,7 +6953,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6873,7 +6971,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6891,7 +6989,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6909,7 +7007,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6927,7 +7025,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6945,7 +7043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6963,7 +7061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6981,7 +7079,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6992,7 +7090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -7002,14 +7100,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="8.44140625" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.77734375" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -7041,7 +7139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7077,7 +7175,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7113,7 +7211,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7149,7 +7247,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7185,7 +7283,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7221,7 +7319,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7257,7 +7355,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7293,7 +7391,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7329,7 +7427,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7365,7 +7463,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7401,7 +7499,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7437,7 +7535,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7473,7 +7571,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7509,7 +7607,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7545,7 +7643,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7569,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7593,7 +7691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7617,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7641,7 +7739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7665,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7689,7 +7787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7713,7 +7811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7737,7 +7835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7761,7 +7859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7785,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7809,7 +7907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7833,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7857,7 +7955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7881,7 +7979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7905,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7929,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7953,7 +8051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7977,7 +8075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8001,7 +8099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8025,7 +8123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8049,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8073,7 +8171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8097,7 +8195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8121,7 +8219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8157,7 +8255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8167,13 +8265,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8197,7 +8295,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8220,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8243,7 +8341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8266,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8289,7 +8387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8312,7 +8410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8335,7 +8433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8358,7 +8456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8381,7 +8479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8404,7 +8502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8427,7 +8525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8450,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8473,7 +8571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8496,7 +8594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8519,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8542,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8565,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8588,7 +8686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8611,7 +8709,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8634,7 +8732,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8657,7 +8755,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8680,7 +8778,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8703,7 +8801,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8726,7 +8824,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8749,7 +8847,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8772,7 +8870,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8803,7 +8901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8813,13 +8911,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8843,7 +8941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8871,7 +8969,7 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
@@ -8897,7 +8995,7 @@
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8918,7 +9016,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8939,7 +9037,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8947,7 +9045,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8955,7 +9053,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8983,7 +9081,7 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
@@ -9008,7 +9106,7 @@
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -9028,7 +9126,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -9048,7 +9146,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9062,7 +9160,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9106,7 +9204,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9150,7 +9248,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9207,14 +9305,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9229,7 +9327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9239,13 +9337,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9269,7 +9367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9292,7 +9390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9312,7 +9410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9332,7 +9430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9363,7 +9461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9373,13 +9471,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9414,7 +9512,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9431,10 +9529,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9451,10 +9549,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9471,7 +9569,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9485,7 +9583,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9499,7 +9597,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9516,7 +9614,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9530,7 +9628,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9547,7 +9645,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9568,7 +9666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9578,15 +9676,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="53"/>
+    <col min="2" max="2" width="19.109375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>179</v>
       </c>
@@ -9603,7 +9701,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>174</v>
       </c>
@@ -9612,12 +9710,12 @@
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
-      <c r="E2" s="83" t="str">
+      <c r="E2" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="65"/>
       <c r="B3" s="64" t="s">
         <v>1</v>
@@ -9626,12 +9724,12 @@
         <v>197</v>
       </c>
       <c r="D3" s="66"/>
-      <c r="E3" s="83" t="str">
+      <c r="E3" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="65"/>
       <c r="B4" s="64" t="s">
         <v>2</v>
@@ -9640,12 +9738,12 @@
         <v>197</v>
       </c>
       <c r="D4" s="66"/>
-      <c r="E4" s="83" t="str">
+      <c r="E4" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="65"/>
       <c r="B5" s="64" t="s">
         <v>3</v>
@@ -9654,12 +9752,12 @@
         <v>197</v>
       </c>
       <c r="D5" s="66"/>
-      <c r="E5" s="83" t="str">
+      <c r="E5" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="65"/>
       <c r="B6" s="64" t="s">
         <v>4</v>
@@ -9668,12 +9766,12 @@
         <v>197</v>
       </c>
       <c r="D6" s="66"/>
-      <c r="E6" s="83" t="str">
+      <c r="E6" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
         <v>173</v>
@@ -9682,7 +9780,7 @@
       <c r="D7" s="62"/>
       <c r="E7" s="66"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>202</v>
       </c>
@@ -9693,60 +9791,60 @@
       <c r="D9" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="83" t="str">
+      <c r="E9" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="65"/>
       <c r="B10" s="64" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="66"/>
       <c r="D10" s="66"/>
-      <c r="E10" s="83" t="str">
+      <c r="E10" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="65"/>
       <c r="B11" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
-      <c r="E11" s="83" t="str">
+      <c r="E11" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="65"/>
       <c r="B12" s="64" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
-      <c r="E12" s="83" t="str">
+      <c r="E12" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="65"/>
       <c r="B13" s="64" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="66"/>
       <c r="D13" s="66"/>
-      <c r="E13" s="83" t="str">
+      <c r="E13" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
         <v>173</v>
@@ -9755,7 +9853,7 @@
       <c r="D14" s="62"/>
       <c r="E14" s="66"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
         <v>203</v>
       </c>
@@ -9766,12 +9864,12 @@
       <c r="D16" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E16" s="83" t="str">
+      <c r="E16" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="65"/>
       <c r="B17" s="64" t="s">
         <v>1</v>
@@ -9780,12 +9878,12 @@
       <c r="D17" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E17" s="83" t="str">
+      <c r="E17" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="65"/>
       <c r="B18" s="64" t="s">
         <v>2</v>
@@ -9794,12 +9892,12 @@
       <c r="D18" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E18" s="83" t="str">
+      <c r="E18" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="65"/>
       <c r="B19" s="64" t="s">
         <v>3</v>
@@ -9808,12 +9906,12 @@
       <c r="D19" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="83" t="str">
+      <c r="E19" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="65"/>
       <c r="B20" s="64" t="s">
         <v>4</v>
@@ -9822,12 +9920,12 @@
       <c r="D20" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E20" s="83" t="str">
+      <c r="E20" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
         <v>173</v>
@@ -9843,7 +9941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9853,30 +9951,30 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>165</v>
       </c>
       <c r="B1" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="86" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="64" t="s">
@@ -9887,8 +9985,8 @@
       </c>
       <c r="D2" s="66"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="88" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="86" t="s">
         <v>186</v>
       </c>
       <c r="B3" s="64" t="s">
@@ -9905,45 +10003,45 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="70" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="53" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" style="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="53"/>
+    <col min="6" max="16384" width="14.44140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="91" t="str">
+      <c r="B1" s="89" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="74" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" s="75" t="s">
+      <c r="D1" s="73" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E1" s="73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>29</v>
       </c>
@@ -9957,10 +10055,10 @@
         <v>25</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
         <v>86</v>
       </c>
@@ -9974,10 +10072,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>61</v>
       </c>
@@ -9991,10 +10089,10 @@
         <v>90</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
         <v>150</v>
       </c>
@@ -10008,10 +10106,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>201</v>
       </c>
@@ -10021,15 +10119,14 @@
       <c r="C6" s="71">
         <v>0.95</v>
       </c>
-      <c r="D6" s="73">
-        <f>SUM('Programs family planning'!E2:E10)</f>
-        <v>0.82100000000000006</v>
+      <c r="D6" s="72">
+        <v>0.82</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
         <v>63</v>
       </c>
@@ -10043,10 +10140,10 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
         <v>64</v>
       </c>
@@ -10060,10 +10157,10 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="70" t="s">
         <v>62</v>
       </c>
@@ -10077,11 +10174,11 @@
         <v>0.19</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="84" t="s">
         <v>189</v>
       </c>
       <c r="B10" s="71">
@@ -10094,11 +10191,11 @@
         <v>0.73</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="84" t="s">
         <v>190</v>
       </c>
       <c r="B11" s="71">
@@ -10111,11 +10208,11 @@
         <v>1.78</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="84" t="s">
         <v>191</v>
       </c>
       <c r="B12" s="71">
@@ -10128,11 +10225,11 @@
         <v>0.24</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="84" t="s">
         <v>192</v>
       </c>
       <c r="B13" s="71">
@@ -10145,10 +10242,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>188</v>
       </c>
@@ -10162,10 +10259,10 @@
         <v>0.73</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>193</v>
       </c>
@@ -10179,10 +10276,10 @@
         <v>1.78</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
         <v>57</v>
       </c>
@@ -10196,10 +10293,10 @@
         <v>2.06</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
         <v>47</v>
       </c>
@@ -10213,10 +10310,10 @@
         <v>0.05</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70" t="s">
         <v>174</v>
       </c>
@@ -10226,15 +10323,15 @@
       <c r="C18" s="71">
         <v>0.95</v>
       </c>
-      <c r="D18" s="85">
+      <c r="D18" s="83">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>202</v>
       </c>
@@ -10244,15 +10341,15 @@
       <c r="C19" s="71">
         <v>0.95</v>
       </c>
-      <c r="D19" s="85">
+      <c r="D19" s="83">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>3.78</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70" t="s">
         <v>203</v>
       </c>
@@ -10262,15 +10359,15 @@
       <c r="C20" s="71">
         <v>0.95</v>
       </c>
-      <c r="D20" s="85">
+      <c r="D20" s="83">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>14.270000000000001</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>199</v>
       </c>
@@ -10284,10 +10381,10 @@
         <v>8.84</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>137</v>
       </c>
@@ -10301,10 +10398,10 @@
         <v>50</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
         <v>34</v>
       </c>
@@ -10318,10 +10415,10 @@
         <v>2.61</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
         <v>88</v>
       </c>
@@ -10335,10 +10432,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
         <v>87</v>
       </c>
@@ -10352,10 +10449,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
         <v>138</v>
       </c>
@@ -10369,10 +10466,10 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70" t="s">
         <v>59</v>
       </c>
@@ -10386,10 +10483,10 @@
         <v>3.78</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70" t="s">
         <v>84</v>
       </c>
@@ -10403,10 +10500,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="70" t="s">
         <v>58</v>
       </c>
@@ -10420,10 +10517,10 @@
         <v>48</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="70" t="s">
         <v>67</v>
       </c>
@@ -10433,15 +10530,14 @@
       <c r="C30" s="71">
         <v>0.95</v>
       </c>
-      <c r="D30" s="73">
-        <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
-        <v>5.2956558655829511</v>
+      <c r="D30" s="72">
+        <v>5.3</v>
       </c>
       <c r="E30" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="70" t="s">
         <v>28</v>
       </c>
@@ -10455,10 +10551,10 @@
         <v>0.41</v>
       </c>
       <c r="E31" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="70" t="s">
         <v>83</v>
       </c>
@@ -10472,10 +10568,10 @@
         <v>0.9</v>
       </c>
       <c r="E32" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="70" t="s">
         <v>82</v>
       </c>
@@ -10489,10 +10585,10 @@
         <v>0.9</v>
       </c>
       <c r="E33" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70" t="s">
         <v>81</v>
       </c>
@@ -10506,10 +10602,10 @@
         <v>79</v>
       </c>
       <c r="E34" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="70" t="s">
         <v>79</v>
       </c>
@@ -10523,10 +10619,10 @@
         <v>31</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="70" t="s">
         <v>80</v>
       </c>
@@ -10540,11 +10636,11 @@
         <v>102</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F36" s="53"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="70" t="s">
         <v>85</v>
       </c>
@@ -10558,10 +10654,10 @@
         <v>5.53</v>
       </c>
       <c r="E37" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="70" t="s">
         <v>60</v>
       </c>
@@ -10575,10 +10671,10 @@
         <v>1</v>
       </c>
       <c r="E38" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F39" s="54"/>
     </row>
   </sheetData>
@@ -10587,10 +10683,11 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4A8EF9C-69C5-FA47-B4F0-310AA7683106}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Changed hospital to health facility
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\national\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B5FFAB85-380B-6C44-9A07-35BAE6437924}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15540" tabRatio="961" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -88,12 +89,75 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The cost per child per year can be estimated as 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">= (cost per treatment) * (annual diarrhoea incidence)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Diarrhoea incidence is the average in children under 5.  See user guide for further information</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nick Scott:</t>
         </r>
@@ -110,16 +174,16 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 The cost per child per year can be estimated as 
-= (cost per treatment) * (annual diarrhoea incidence)
-Diarrhoea incidence is the average in children under 5.  See user guide for further information</t>
+= (cost per treatment episode) * (SAM prevalence) * 2.6
+Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -127,7 +191,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nick Scott:</t>
         </r>
@@ -136,33 +200,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-The cost per child per year can be estimated as 
-= (cost per treatment episode) * (SAM prevalence) * 2.6
-Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 The cost per child per year can be estimated as 
@@ -176,12 +214,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -234,12 +272,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -849,18 +887,12 @@
     <t>IFAS (community)</t>
   </si>
   <si>
-    <t>IFAS (hospital)</t>
-  </si>
-  <si>
     <t>IFAS (retailer)</t>
   </si>
   <si>
     <t>IFAS (school)</t>
   </si>
   <si>
-    <t>IFAS for pregnant women (hospital)</t>
-  </si>
-  <si>
     <t>Projection years</t>
   </si>
   <si>
@@ -910,19 +942,25 @@
   </si>
   <si>
     <t>Unit cost (US$ per person per year)</t>
+  </si>
+  <si>
+    <t>IFAS (health facility)</t>
+  </si>
+  <si>
+    <t>IFAS for pregnant women (health facility)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1066,13 +1104,26 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1186,7 +1237,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1948,8 +1999,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1965,8 +2016,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1985,20 +2036,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2010,11 +2061,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2044,7 +2095,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2067,7 +2118,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2808,8 +2859,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -4249,24 +4300,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.44140625" style="15"/>
+    <col min="3" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4277,42 +4326,42 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C3" s="87">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="88">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4320,7 +4369,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4328,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4336,7 +4385,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4344,7 +4393,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4352,7 +4401,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4360,17 +4409,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4378,7 +4427,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4386,7 +4435,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4394,7 +4443,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4402,7 +4451,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4411,15 +4460,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4427,7 +4476,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4435,7 +4484,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4443,7 +4492,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4451,18 +4500,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4470,7 +4519,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4478,7 +4527,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4486,7 +4535,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4494,7 +4543,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4503,20 +4552,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4524,7 +4573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4534,7 +4583,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4544,7 +4593,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4552,7 +4601,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4560,7 +4609,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4568,16 +4617,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4586,7 +4635,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4595,7 +4644,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4605,7 +4654,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4616,16 +4665,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4634,7 +4683,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4642,7 +4691,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4650,7 +4699,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4658,7 +4707,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4666,12 +4715,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4679,7 +4728,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4687,7 +4736,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4697,7 +4746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4707,15 +4756,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="75" customWidth="1"/>
-    <col min="2" max="16384" width="10.77734375" style="75"/>
+    <col min="2" max="16384" width="10.83203125" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" s="79" t="s">
         <v>178</v>
@@ -4730,7 +4779,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
         <v>165</v>
       </c>
@@ -4748,7 +4797,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
       <c r="B3" s="77" t="s">
         <v>1</v>
@@ -4765,7 +4814,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="77"/>
       <c r="B4" s="77" t="s">
         <v>2</v>
@@ -4782,7 +4831,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="77"/>
       <c r="B5" s="77" t="s">
         <v>3</v>
@@ -4799,7 +4848,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="77"/>
       <c r="B6" s="77" t="s">
         <v>4</v>
@@ -4816,7 +4865,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="76"/>
     </row>
   </sheetData>
@@ -4825,25 +4874,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4854,7 +4903,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -4863,16 +4912,16 @@
       </c>
       <c r="C2" s="66"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="66"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>58</v>
       </c>
@@ -4881,7 +4930,7 @@
       </c>
       <c r="C4" s="66"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>138</v>
       </c>
@@ -4890,28 +4939,28 @@
       </c>
       <c r="C5" s="66"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4922,7 +4971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4932,85 +4981,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="53"/>
+    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="66" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="66"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="66"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="66"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="66"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="66"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="66"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="66"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="66"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="66"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="66"/>
     </row>
   </sheetData>
@@ -5020,7 +5069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5030,9 +5079,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5052,7 +5101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -5077,7 +5126,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -5102,7 +5151,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5134,29 +5183,29 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5203,7 +5252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5254,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5298,9 +5347,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5342,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5388,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5435,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
@@ -5484,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5530,7 +5579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5578,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5622,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
@@ -5671,7 +5720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5715,10 +5764,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5769,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5814,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5863,10 +5912,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="C17" s="52">
         <v>0</v>
@@ -5912,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5960,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -6004,7 +6053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -6048,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -6096,15 +6145,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="82" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6146,7 +6195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="84" t="s">
         <v>189</v>
       </c>
@@ -6194,9 +6243,9 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="84" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="C25" s="52">
         <v>0</v>
@@ -6242,9 +6291,9 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="52">
         <v>0</v>
@@ -6290,9 +6339,9 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27" s="52">
         <v>0</v>
@@ -6335,7 +6384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6345,7 +6394,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6403,7 +6452,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6458,7 +6507,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6513,7 +6562,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6557,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6614,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6658,7 +6707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6703,7 +6752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6747,7 +6796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6791,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6835,7 +6884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6848,31 +6897,31 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -6881,7 +6930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6891,16 +6940,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" style="53"/>
-    <col min="5" max="5" width="17.44140625" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="53"/>
+    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6917,7 +6966,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6935,7 +6984,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6953,7 +7002,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6971,7 +7020,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6989,7 +7038,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -7007,7 +7056,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -7025,7 +7074,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -7043,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -7061,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -7079,7 +7128,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -7090,7 +7139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -7100,14 +7149,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.77734375" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="15"/>
+    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -7139,7 +7188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7175,7 +7224,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7211,7 +7260,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7247,7 +7296,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7283,7 +7332,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7319,7 +7368,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7355,7 +7404,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7391,7 +7440,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7427,7 +7476,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7463,7 +7512,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7499,7 +7548,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7535,7 +7584,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7571,7 +7620,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7607,7 +7656,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7643,7 +7692,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7667,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7691,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7715,7 +7764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7739,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7763,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7787,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7811,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7835,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7859,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7883,7 +7932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7907,7 +7956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7931,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7955,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7979,7 +8028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8003,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8027,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8051,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8075,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8099,7 +8148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8123,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8147,7 +8196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8171,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8195,7 +8244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8219,7 +8268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8255,7 +8304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8265,13 +8314,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8295,7 +8344,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8318,7 +8367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8341,7 +8390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8364,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8387,7 +8436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8410,7 +8459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8433,7 +8482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8456,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8479,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8502,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8525,7 +8574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8548,7 +8597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8571,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8594,7 +8643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8617,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8640,7 +8689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8663,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8686,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8709,7 +8758,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8732,7 +8781,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8755,7 +8804,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8778,7 +8827,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8801,7 +8850,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8824,7 +8873,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8847,7 +8896,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8870,7 +8919,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8901,7 +8950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8911,13 +8960,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8941,7 +8990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8969,7 +9018,7 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
@@ -8995,7 +9044,7 @@
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -9016,7 +9065,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -9037,7 +9086,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -9045,7 +9094,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -9053,7 +9102,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -9081,7 +9130,7 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
@@ -9106,7 +9155,7 @@
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -9126,7 +9175,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -9146,7 +9195,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9160,7 +9209,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9204,7 +9253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9248,7 +9297,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9305,14 +9354,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9327,7 +9376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9337,13 +9386,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
-    <col min="2" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9367,7 +9416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9390,7 +9439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9410,7 +9459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9430,7 +9479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9461,7 +9510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9471,13 +9520,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9512,7 +9561,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9529,10 +9578,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9549,10 +9598,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9569,7 +9618,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9583,7 +9632,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9597,7 +9646,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9614,7 +9663,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9628,7 +9677,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9645,7 +9694,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9666,7 +9715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9676,15 +9725,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="53"/>
+    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
         <v>179</v>
       </c>
@@ -9701,7 +9750,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
         <v>174</v>
       </c>
@@ -9715,13 +9764,13 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="65"/>
       <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="81" t="str">
@@ -9729,13 +9778,13 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="65"/>
       <c r="B4" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="81" t="str">
@@ -9743,13 +9792,13 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="65"/>
       <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="81" t="str">
@@ -9757,13 +9806,13 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="65"/>
       <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="81" t="str">
@@ -9771,7 +9820,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
         <v>173</v>
@@ -9780,23 +9829,23 @@
       <c r="D7" s="62"/>
       <c r="E7" s="66"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="66"/>
       <c r="D9" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E9" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="65"/>
       <c r="B10" s="64" t="s">
         <v>1</v>
@@ -9808,7 +9857,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="65"/>
       <c r="B11" s="64" t="s">
         <v>2</v>
@@ -9820,7 +9869,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="65"/>
       <c r="B12" s="64" t="s">
         <v>3</v>
@@ -9832,7 +9881,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="65"/>
       <c r="B13" s="64" t="s">
         <v>4</v>
@@ -9844,7 +9893,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
         <v>173</v>
@@ -9853,79 +9902,79 @@
       <c r="D14" s="62"/>
       <c r="E14" s="66"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B16" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="66"/>
       <c r="D16" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E16" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="65"/>
       <c r="B17" s="64" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E17" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="65"/>
       <c r="B18" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E18" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="65"/>
       <c r="B19" s="64" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="66"/>
       <c r="D19" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E19" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="65"/>
       <c r="B20" s="64" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="66"/>
       <c r="D20" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E20" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
         <v>173</v>
@@ -9941,7 +9990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9951,15 +10000,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="85" t="s">
         <v>165</v>
       </c>
@@ -9973,7 +10022,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="86" t="s">
         <v>69</v>
       </c>
@@ -9985,7 +10034,7 @@
       </c>
       <c r="D2" s="66"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="86" t="s">
         <v>186</v>
       </c>
@@ -10003,27 +10052,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" style="70" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" style="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.44140625" style="53"/>
+    <col min="6" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="74" t="s">
         <v>69</v>
       </c>
@@ -10032,16 +10081,16 @@
         <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
         <v>29</v>
       </c>
@@ -10055,10 +10104,10 @@
         <v>25</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>86</v>
       </c>
@@ -10072,10 +10121,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>61</v>
       </c>
@@ -10089,10 +10138,10 @@
         <v>90</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>150</v>
       </c>
@@ -10106,12 +10155,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B6" s="71">
         <v>0</v>
@@ -10123,10 +10172,10 @@
         <v>0.82</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
         <v>63</v>
       </c>
@@ -10140,10 +10189,10 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
         <v>64</v>
       </c>
@@ -10157,10 +10206,10 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="70" t="s">
         <v>62</v>
       </c>
@@ -10174,10 +10223,10 @@
         <v>0.19</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="84" t="s">
         <v>189</v>
       </c>
@@ -10191,12 +10240,12 @@
         <v>0.73</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="84" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -10208,12 +10257,12 @@
         <v>1.78</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -10225,12 +10274,12 @@
         <v>0.24</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="71">
         <v>0</v>
@@ -10242,10 +10291,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
         <v>188</v>
       </c>
@@ -10259,12 +10308,12 @@
         <v>0.73</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B15" s="71">
         <v>0</v>
@@ -10276,10 +10325,10 @@
         <v>1.78</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
         <v>57</v>
       </c>
@@ -10293,10 +10342,10 @@
         <v>2.06</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
         <v>47</v>
       </c>
@@ -10310,10 +10359,10 @@
         <v>0.05</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
         <v>174</v>
       </c>
@@ -10328,12 +10377,12 @@
         <v>3.66</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B19" s="71">
         <v>0</v>
@@ -10346,12 +10395,12 @@
         <v>3.78</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B20" s="71">
         <v>0</v>
@@ -10364,12 +10413,12 @@
         <v>14.270000000000001</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B21" s="71">
         <v>0</v>
@@ -10381,10 +10430,10 @@
         <v>8.84</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
         <v>137</v>
       </c>
@@ -10398,10 +10447,10 @@
         <v>50</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
         <v>34</v>
       </c>
@@ -10415,10 +10464,10 @@
         <v>2.61</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
         <v>88</v>
       </c>
@@ -10432,10 +10481,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
         <v>87</v>
       </c>
@@ -10449,10 +10498,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
         <v>138</v>
       </c>
@@ -10466,10 +10515,10 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="70" t="s">
         <v>59</v>
       </c>
@@ -10483,10 +10532,10 @@
         <v>3.78</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="70" t="s">
         <v>84</v>
       </c>
@@ -10500,10 +10549,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="70" t="s">
         <v>58</v>
       </c>
@@ -10517,10 +10566,10 @@
         <v>48</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="70" t="s">
         <v>67</v>
       </c>
@@ -10534,10 +10583,10 @@
         <v>5.3</v>
       </c>
       <c r="E30" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="70" t="s">
         <v>28</v>
       </c>
@@ -10551,10 +10600,10 @@
         <v>0.41</v>
       </c>
       <c r="E31" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="70" t="s">
         <v>83</v>
       </c>
@@ -10568,10 +10617,10 @@
         <v>0.9</v>
       </c>
       <c r="E32" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
         <v>82</v>
       </c>
@@ -10585,10 +10634,10 @@
         <v>0.9</v>
       </c>
       <c r="E33" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
         <v>81</v>
       </c>
@@ -10602,10 +10651,10 @@
         <v>79</v>
       </c>
       <c r="E34" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
         <v>79</v>
       </c>
@@ -10619,10 +10668,10 @@
         <v>31</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
         <v>80</v>
       </c>
@@ -10636,11 +10685,11 @@
         <v>102</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F36" s="53"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
         <v>85</v>
       </c>
@@ -10654,10 +10703,10 @@
         <v>5.53</v>
       </c>
       <c r="E37" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
         <v>60</v>
       </c>
@@ -10671,10 +10720,10 @@
         <v>1</v>
       </c>
       <c r="E38" s="72" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F39" s="54"/>
     </row>
   </sheetData>
@@ -10687,7 +10736,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Moved under 5 pop to baseline, no projection
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B5FFAB85-380B-6C44-9A07-35BAE6437924}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05CFEDD8-7BE8-7247-972E-0A21069AAE0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Causes of death" sheetId="4" r:id="rId3"/>
     <sheet name="Nutritional status distribution" sheetId="5" r:id="rId4"/>
     <sheet name="Breastfeeding distribution" sheetId="50" r:id="rId5"/>
-    <sheet name="Time trends" sheetId="51" r:id="rId6"/>
+    <sheet name="Time trends" sheetId="51" state="hidden" r:id="rId6"/>
     <sheet name="IYCF packages" sheetId="55" r:id="rId7"/>
     <sheet name="Treatment of SAM" sheetId="60" r:id="rId8"/>
     <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
@@ -28,56 +28,56 @@
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
     <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
-    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
+    <sheet name="Programs family planning" sheetId="54" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
-    <definedName name="abortion">'Baseline year population inputs'!$C$40</definedName>
+    <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="abortion">'Baseline year population inputs'!$C$41</definedName>
     <definedName name="comm_deliv">'Treatment of SAM'!$D$3</definedName>
-    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$51</definedName>
-    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$53</definedName>
-    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$50</definedName>
-    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$54</definedName>
-    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$52</definedName>
+    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$52</definedName>
+    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$54</definedName>
+    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$51</definedName>
+    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$55</definedName>
+    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$53</definedName>
     <definedName name="end_year">'Baseline year population inputs'!$C$4</definedName>
-    <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$12</definedName>
-    <definedName name="food_insecure">'Baseline year population inputs'!$C$7</definedName>
-    <definedName name="frac_children_health_facility">'Baseline year population inputs'!$C$11</definedName>
-    <definedName name="frac_diarrhea_severe">'Baseline year population inputs'!$C$57</definedName>
-    <definedName name="frac_maize">'Baseline year population inputs'!$C$18</definedName>
-    <definedName name="frac_malaria_risk">'Baseline year population inputs'!$C$8</definedName>
+    <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$13</definedName>
+    <definedName name="food_insecure">'Baseline year population inputs'!$C$8</definedName>
+    <definedName name="frac_children_health_facility">'Baseline year population inputs'!$C$12</definedName>
+    <definedName name="frac_diarrhea_severe">'Baseline year population inputs'!$C$58</definedName>
+    <definedName name="frac_maize">'Baseline year population inputs'!$C$19</definedName>
+    <definedName name="frac_malaria_risk">'Baseline year population inputs'!$C$9</definedName>
     <definedName name="frac_mam_1_5months">'Nutritional status distribution'!$D$10</definedName>
     <definedName name="frac_mam_12_23months">'Nutritional status distribution'!$F$10</definedName>
     <definedName name="frac_mam_1month">'Nutritional status distribution'!$C$10</definedName>
     <definedName name="frac_mam_24_59months">'Nutritional status distribution'!$G$10</definedName>
     <definedName name="frac_mam_6_11months">'Nutritional status distribution'!$E$10</definedName>
     <definedName name="frac_MAMtoSAM">'Baseline year population inputs'!#REF!</definedName>
-    <definedName name="frac_other_staples">'Baseline year population inputs'!$C$19</definedName>
-    <definedName name="frac_PW_health_facility">'Baseline year population inputs'!$C$10</definedName>
-    <definedName name="frac_rice">'Baseline year population inputs'!$C$16</definedName>
+    <definedName name="frac_other_staples">'Baseline year population inputs'!$C$20</definedName>
+    <definedName name="frac_PW_health_facility">'Baseline year population inputs'!$C$11</definedName>
+    <definedName name="frac_rice">'Baseline year population inputs'!$C$17</definedName>
     <definedName name="frac_sam_1_5months">'Nutritional status distribution'!$D$11</definedName>
     <definedName name="frac_sam_12_23months">'Nutritional status distribution'!$F$11</definedName>
     <definedName name="frac_sam_1month">'Nutritional status distribution'!$C$11</definedName>
     <definedName name="frac_sam_24_59months">'Nutritional status distribution'!$G$11</definedName>
     <definedName name="frac_sam_6_11months">'Nutritional status distribution'!$E$11</definedName>
     <definedName name="frac_SAMtoMAM">'Baseline year population inputs'!#REF!</definedName>
-    <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$15</definedName>
-    <definedName name="frac_wheat">'Baseline year population inputs'!$C$17</definedName>
-    <definedName name="infant_mortality">'Baseline year population inputs'!$C$37</definedName>
-    <definedName name="iron_deficiency_anaemia">'Baseline year population inputs'!$C$58</definedName>
+    <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$16</definedName>
+    <definedName name="frac_wheat">'Baseline year population inputs'!$C$18</definedName>
+    <definedName name="infant_mortality">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="iron_deficiency_anaemia">'Baseline year population inputs'!$C$59</definedName>
     <definedName name="manage_mam">'Treatment of SAM'!$D$2</definedName>
-    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$39</definedName>
-    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$36</definedName>
-    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Baseline year population inputs'!$C$10</definedName>
-    <definedName name="preterm_AGA">'Baseline year population inputs'!$C$45</definedName>
-    <definedName name="preterm_SGA">'Baseline year population inputs'!$C$44</definedName>
-    <definedName name="school_attendance">'Baseline year population inputs'!$C$9</definedName>
+    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$40</definedName>
+    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$37</definedName>
+    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Baseline year population inputs'!$C$11</definedName>
+    <definedName name="preterm_AGA">'Baseline year population inputs'!$C$46</definedName>
+    <definedName name="preterm_SGA">'Baseline year population inputs'!$C$45</definedName>
+    <definedName name="school_attendance">'Baseline year population inputs'!$C$10</definedName>
     <definedName name="start_year">'Baseline year population inputs'!$C$3</definedName>
-    <definedName name="stillbirth" localSheetId="6">'Baseline year population inputs'!$C$38</definedName>
-    <definedName name="stillbirth">'Baseline year population inputs'!$C$41</definedName>
-    <definedName name="term_AGA">'Baseline year population inputs'!$C$47</definedName>
-    <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
-    <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="stillbirth" localSheetId="6">'Baseline year population inputs'!$C$39</definedName>
+    <definedName name="stillbirth">'Baseline year population inputs'!$C$42</definedName>
+    <definedName name="term_AGA">'Baseline year population inputs'!$C$48</definedName>
+    <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
+    <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -163,7 +163,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -172,14 +172,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The cost per child per year can be estimated as 
-= (cost per treatment episode) * (SAM prevalence) * 2.6
-Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The cost per child per year can be estimated as 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">= (cost per treatment episode) * (SAM prevalence) * 2.6
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
         </r>
       </text>
     </comment>
@@ -315,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
   <si>
     <t>year</t>
   </si>
@@ -656,9 +693,6 @@
     <t>Number of births</t>
   </si>
   <si>
-    <t>Children under 5</t>
-  </si>
-  <si>
     <t>Total WRA</t>
   </si>
   <si>
@@ -948,6 +982,9 @@
   </si>
   <si>
     <t>IFAS for pregnant women (health facility)</t>
+  </si>
+  <si>
+    <t>Children under 5 population</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1993,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2133,6 +2170,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -4304,9 +4342,11 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4320,15 +4360,15 @@
         <v>100</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>165</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -4336,7 +4376,7 @@
     <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="87">
         <v>2017</v>
@@ -4345,7 +4385,7 @@
     <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="88">
         <v>2030</v>
@@ -4362,82 +4402,82 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="90">
+        <v>9862402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C8" s="24">
         <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="23">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C10" s="23">
         <v>0.23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="24">
-        <v>0.51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="24">
-        <v>0.37</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="24">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C13" s="24">
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="15"/>
-    </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="23">
-        <v>0.3</v>
-      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="23">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="23">
         <v>0.1</v>
@@ -4445,299 +4485,307 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="23">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C20" s="26">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="15"/>
-    </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="15" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="23">
-        <v>0.127</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="23">
-        <v>0.45200000000000001</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="23">
-        <v>0.33400000000000002</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C26" s="23">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-    </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15" t="s">
-        <v>198</v>
-      </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="42">
-        <v>0.20799999999999999</v>
-      </c>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="42">
-        <v>0.63700000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="42">
-        <v>0.11899999999999999</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="42">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C32" s="42">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="B32" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="44">
-        <f>SUM(C28:C31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
+    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="B33" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="44">
+        <f>SUM(C29:C32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="16"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C37" s="25">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="25">
-        <v>43</v>
-      </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="25">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="C39" s="25">
-        <v>4.01</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="25">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C41" s="23">
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="60" t="s">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C42" s="25">
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D42" s="20"/>
-    </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15" t="s">
-        <v>134</v>
-      </c>
       <c r="D43" s="20"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="23">
-        <v>3.1E-2</v>
+      <c r="A44" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="D44" s="20"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45" s="23">
-        <v>0.109</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="23">
+        <v>0.109</v>
+      </c>
+      <c r="D46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C47" s="23">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="19" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C48" s="26">
         <f>1-term_SGA-preterm_AGA-preterm_SGA</f>
         <v>0.495</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="15" t="s">
+      <c r="D49" s="20"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="20"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="7">
-        <v>1.66</v>
-      </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="7">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D51" s="20"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C52" s="7">
-        <v>5.64</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C53" s="7">
-        <v>5.43</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C54" s="7">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="7">
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="9" t="s">
+      <c r="A57" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C58" s="24">
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="24">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="24">
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="4"/>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4764,24 +4812,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="79" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="77" t="s">
         <v>32</v>
@@ -4897,15 +4945,15 @@
         <v>69</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="66" t="s">
         <v>59</v>
@@ -4914,7 +4962,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>59</v>
@@ -4926,16 +4974,16 @@
         <v>58</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="66"/>
     </row>
@@ -4994,7 +5042,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
@@ -5076,7 +5124,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5106,23 +5154,23 @@
         <v>71</v>
       </c>
       <c r="B2" s="37">
-        <f>'Baseline year population inputs'!C50</f>
-        <v>1.66</v>
-      </c>
-      <c r="C2" s="37">
         <f>'Baseline year population inputs'!C51</f>
         <v>1.66</v>
       </c>
+      <c r="C2" s="37">
+        <f>'Baseline year population inputs'!C52</f>
+        <v>1.66</v>
+      </c>
       <c r="D2" s="37">
-        <f>'Baseline year population inputs'!C52</f>
+        <f>'Baseline year population inputs'!C53</f>
         <v>5.64</v>
       </c>
       <c r="E2" s="37">
-        <f>'Baseline year population inputs'!C53</f>
+        <f>'Baseline year population inputs'!C54</f>
         <v>5.43</v>
       </c>
       <c r="F2" s="37">
-        <f>'Baseline year population inputs'!C54</f>
+        <f>'Baseline year population inputs'!C55</f>
         <v>1.91</v>
       </c>
     </row>
@@ -5190,7 +5238,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5305,7 +5353,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="51">
         <v>1</v>
@@ -5349,7 +5397,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5393,7 +5441,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="51">
         <v>0</v>
@@ -5439,7 +5487,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="51">
         <v>0</v>
@@ -5866,7 +5914,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16" s="52">
         <v>0</v>
@@ -5915,7 +5963,7 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" s="52">
         <v>0</v>
@@ -6153,7 +6201,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6197,7 +6245,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="84" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="52">
         <v>0</v>
@@ -6245,7 +6293,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="52">
         <v>0</v>
@@ -6293,7 +6341,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="52">
         <v>0</v>
@@ -6341,7 +6389,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="52">
         <v>0</v>
@@ -6906,22 +6954,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -6937,7 +6985,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6951,24 +6999,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="56">
         <v>0.9</v>
@@ -6986,7 +7034,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
@@ -7004,7 +7052,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="56">
         <v>1</v>
@@ -7022,7 +7070,7 @@
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="56">
         <v>1</v>
@@ -7040,7 +7088,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="56">
         <v>1</v>
@@ -7058,7 +7106,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" s="56">
         <v>0.93</v>
@@ -7076,7 +7124,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="56">
         <v>0.5</v>
@@ -7094,7 +7142,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="56">
         <v>0.5</v>
@@ -7112,7 +7160,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="56">
         <v>0.98</v>
@@ -7143,20 +7191,20 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" style="15"/>
+    <col min="2" max="9" width="16.83203125" style="15" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -7164,31 +7212,28 @@
         <v>112</v>
       </c>
       <c r="C1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="31" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7197,34 +7242,31 @@
         <v>2110000</v>
       </c>
       <c r="C2" s="29">
-        <v>9862402</v>
+        <v>3032037</v>
       </c>
       <c r="D2" s="29">
-        <v>3032037</v>
+        <v>4756743</v>
       </c>
       <c r="E2" s="29">
-        <v>4756743</v>
+        <v>3406589</v>
       </c>
       <c r="F2" s="29">
-        <v>3406589</v>
-      </c>
-      <c r="G2" s="29">
         <v>2174712</v>
       </c>
+      <c r="G2" s="30">
+        <f t="shared" ref="G2:G40" si="0">C2+D2+E2+F2</f>
+        <v>13370081</v>
+      </c>
       <c r="H2" s="30">
-        <f t="shared" ref="H2:H40" si="0">D2+E2+F2+G2</f>
-        <v>13370081</v>
-      </c>
-      <c r="I2" s="30">
         <f>(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>2480858.588708919</v>
       </c>
-      <c r="J2" s="30">
-        <f>H2-I2</f>
+      <c r="I2" s="30">
+        <f>G2-H2</f>
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7233,34 +7275,31 @@
         <v>2150000</v>
       </c>
       <c r="C3" s="29">
-        <v>10050371</v>
+        <v>3164674</v>
       </c>
       <c r="D3" s="29">
-        <v>3164674</v>
+        <v>4882700</v>
       </c>
       <c r="E3" s="29">
-        <v>4882700</v>
+        <v>3520083</v>
       </c>
       <c r="F3" s="29">
-        <v>3520083</v>
-      </c>
-      <c r="G3" s="29">
         <v>2275309</v>
       </c>
-      <c r="H3" s="30">
+      <c r="G3" s="30">
         <f t="shared" si="0"/>
         <v>13842766</v>
       </c>
+      <c r="H3" s="30">
+        <f>(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
+        <v>2527889.0832815999</v>
+      </c>
       <c r="I3" s="30">
-        <f t="shared" ref="I3:I40" si="2">(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
-        <v>2527889.0832815999</v>
-      </c>
-      <c r="J3" s="30">
-        <f t="shared" ref="J3:J15" si="3">H3-I3</f>
+        <f t="shared" ref="I3:I15" si="2">G3-H3</f>
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7269,34 +7308,31 @@
         <v>2200000</v>
       </c>
       <c r="C4" s="29">
-        <v>10237786</v>
+        <v>3296354</v>
       </c>
       <c r="D4" s="29">
-        <v>3296354</v>
+        <v>5018666</v>
       </c>
       <c r="E4" s="29">
-        <v>5018666</v>
+        <v>3634703</v>
       </c>
       <c r="F4" s="29">
-        <v>3634703</v>
-      </c>
-      <c r="G4" s="29">
         <v>2379017</v>
       </c>
-      <c r="H4" s="30">
+      <c r="G4" s="30">
         <f t="shared" si="0"/>
         <v>14328740</v>
       </c>
+      <c r="H4" s="30">
+        <f>(B4 + stillbirth*B4/(1000-stillbirth))/(1-abortion)</f>
+        <v>2586677.2014974509</v>
+      </c>
       <c r="I4" s="30">
         <f t="shared" si="2"/>
-        <v>2586677.2014974509</v>
-      </c>
-      <c r="J4" s="30">
-        <f t="shared" si="3"/>
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7305,34 +7341,31 @@
         <v>2240000</v>
       </c>
       <c r="C5" s="29">
-        <v>10438537</v>
+        <v>3418969</v>
       </c>
       <c r="D5" s="29">
-        <v>3418969</v>
+        <v>5168014</v>
       </c>
       <c r="E5" s="29">
-        <v>5168014</v>
+        <v>3750324</v>
       </c>
       <c r="F5" s="29">
-        <v>3750324</v>
-      </c>
-      <c r="G5" s="29">
         <v>2484409</v>
       </c>
-      <c r="H5" s="30">
+      <c r="G5" s="30">
         <f t="shared" si="0"/>
         <v>14821716</v>
       </c>
+      <c r="H5" s="30">
+        <f>(B5 + stillbirth*B5/(1000-stillbirth))/(1-abortion)</f>
+        <v>2633707.6960701318</v>
+      </c>
       <c r="I5" s="30">
         <f t="shared" si="2"/>
-        <v>2633707.6960701318</v>
-      </c>
-      <c r="J5" s="30">
-        <f t="shared" si="3"/>
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7341,34 +7374,31 @@
         <v>2280000</v>
       </c>
       <c r="C6" s="29">
-        <v>10636534</v>
+        <v>3532758</v>
       </c>
       <c r="D6" s="29">
-        <v>3532758</v>
+        <v>5332455</v>
       </c>
       <c r="E6" s="29">
-        <v>5332455</v>
+        <v>3869436</v>
       </c>
       <c r="F6" s="29">
-        <v>3869436</v>
-      </c>
-      <c r="G6" s="29">
         <v>2592003</v>
       </c>
-      <c r="H6" s="30">
+      <c r="G6" s="30">
         <f t="shared" si="0"/>
         <v>15326652</v>
       </c>
+      <c r="H6" s="30">
+        <f>(B6 + stillbirth*B6/(1000-stillbirth))/(1-abortion)</f>
+        <v>2680738.1906428128</v>
+      </c>
       <c r="I6" s="30">
         <f t="shared" si="2"/>
-        <v>2680738.1906428128</v>
-      </c>
-      <c r="J6" s="30">
-        <f t="shared" si="3"/>
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7377,34 +7407,31 @@
         <v>2330000</v>
       </c>
       <c r="C7" s="29">
-        <v>10854967</v>
+        <v>3637390</v>
       </c>
       <c r="D7" s="29">
-        <v>3637390</v>
+        <v>5508952</v>
       </c>
       <c r="E7" s="29">
-        <v>5508952</v>
+        <v>3990560</v>
       </c>
       <c r="F7" s="29">
-        <v>3990560</v>
-      </c>
-      <c r="G7" s="29">
         <v>2701259</v>
       </c>
-      <c r="H7" s="30">
+      <c r="G7" s="30">
         <f t="shared" si="0"/>
         <v>15838161</v>
       </c>
+      <c r="H7" s="30">
+        <f>(B7 + stillbirth*B7/(1000-stillbirth))/(1-abortion)</f>
+        <v>2739526.3088586638</v>
+      </c>
       <c r="I7" s="30">
         <f t="shared" si="2"/>
-        <v>2739526.3088586638</v>
-      </c>
-      <c r="J7" s="30">
-        <f t="shared" si="3"/>
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7413,34 +7440,31 @@
         <v>2380000</v>
       </c>
       <c r="C8" s="29">
-        <v>11089897</v>
+        <v>3737403</v>
       </c>
       <c r="D8" s="29">
-        <v>3737403</v>
+        <v>5696990</v>
       </c>
       <c r="E8" s="29">
-        <v>5696990</v>
+        <v>4112898</v>
       </c>
       <c r="F8" s="29">
-        <v>4112898</v>
-      </c>
-      <c r="G8" s="29">
         <v>2811667</v>
       </c>
-      <c r="H8" s="30">
+      <c r="G8" s="30">
         <f t="shared" si="0"/>
         <v>16358958</v>
       </c>
+      <c r="H8" s="30">
+        <f>(B8 + stillbirth*B8/(1000-stillbirth))/(1-abortion)</f>
+        <v>2798314.4270745148</v>
+      </c>
       <c r="I8" s="30">
         <f t="shared" si="2"/>
-        <v>2798314.4270745148</v>
-      </c>
-      <c r="J8" s="30">
-        <f t="shared" si="3"/>
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7449,34 +7473,31 @@
         <v>2420000</v>
       </c>
       <c r="C9" s="29">
-        <v>11331595</v>
+        <v>3840674</v>
       </c>
       <c r="D9" s="29">
-        <v>3840674</v>
+        <v>5895615</v>
       </c>
       <c r="E9" s="29">
-        <v>5895615</v>
+        <v>4235117</v>
       </c>
       <c r="F9" s="29">
-        <v>4235117</v>
-      </c>
-      <c r="G9" s="29">
         <v>2922818</v>
       </c>
-      <c r="H9" s="30">
+      <c r="G9" s="30">
         <f t="shared" si="0"/>
         <v>16894224</v>
       </c>
+      <c r="H9" s="30">
+        <f>(B9 + stillbirth*B9/(1000-stillbirth))/(1-abortion)</f>
+        <v>2845344.9216471957</v>
+      </c>
       <c r="I9" s="30">
         <f t="shared" si="2"/>
-        <v>2845344.9216471957</v>
-      </c>
-      <c r="J9" s="30">
-        <f t="shared" si="3"/>
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7485,34 +7506,31 @@
         <v>2480000</v>
       </c>
       <c r="C10" s="29">
-        <v>11574198</v>
+        <v>3951644</v>
       </c>
       <c r="D10" s="29">
-        <v>3951644</v>
+        <v>6103745</v>
       </c>
       <c r="E10" s="29">
-        <v>6103745</v>
+        <v>4356516</v>
       </c>
       <c r="F10" s="29">
-        <v>4356516</v>
-      </c>
-      <c r="G10" s="29">
         <v>3034340</v>
       </c>
-      <c r="H10" s="30">
+      <c r="G10" s="30">
         <f t="shared" si="0"/>
         <v>17446245</v>
       </c>
+      <c r="H10" s="30">
+        <f>(B10 + stillbirth*B10/(1000-stillbirth))/(1-abortion)</f>
+        <v>2915890.6635062173</v>
+      </c>
       <c r="I10" s="30">
         <f t="shared" si="2"/>
-        <v>2915890.6635062173</v>
-      </c>
-      <c r="J10" s="30">
-        <f t="shared" si="3"/>
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7521,34 +7539,31 @@
         <v>2530000</v>
       </c>
       <c r="C11" s="29">
-        <v>11838769</v>
+        <v>4065313</v>
       </c>
       <c r="D11" s="29">
-        <v>4065313</v>
+        <v>6319831</v>
       </c>
       <c r="E11" s="29">
-        <v>6319831</v>
+        <v>4477188</v>
       </c>
       <c r="F11" s="29">
-        <v>4477188</v>
-      </c>
-      <c r="G11" s="29">
         <v>3144612</v>
       </c>
-      <c r="H11" s="30">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>18006944</v>
       </c>
+      <c r="H11" s="30">
+        <f>(B11 + stillbirth*B11/(1000-stillbirth))/(1-abortion)</f>
+        <v>2974678.7817220683</v>
+      </c>
       <c r="I11" s="30">
         <f t="shared" si="2"/>
-        <v>2974678.7817220683</v>
-      </c>
-      <c r="J11" s="30">
-        <f t="shared" si="3"/>
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7557,34 +7572,31 @@
         <v>2580000</v>
       </c>
       <c r="C12" s="29">
-        <v>12092177</v>
+        <v>4185562</v>
       </c>
       <c r="D12" s="29">
-        <v>4185562</v>
+        <v>6545116</v>
       </c>
       <c r="E12" s="29">
-        <v>6545116</v>
+        <v>4597739</v>
       </c>
       <c r="F12" s="29">
-        <v>4597739</v>
-      </c>
-      <c r="G12" s="29">
         <v>3255252</v>
       </c>
-      <c r="H12" s="30">
+      <c r="G12" s="30">
         <f t="shared" si="0"/>
         <v>18583669</v>
       </c>
+      <c r="H12" s="30">
+        <f>(B12 + stillbirth*B12/(1000-stillbirth))/(1-abortion)</f>
+        <v>3033466.8999379198</v>
+      </c>
       <c r="I12" s="30">
         <f t="shared" si="2"/>
-        <v>3033466.8999379198</v>
-      </c>
-      <c r="J12" s="30">
-        <f t="shared" si="3"/>
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7593,34 +7605,31 @@
         <v>2630000</v>
       </c>
       <c r="C13" s="29">
-        <v>12338218</v>
+        <v>4309237</v>
       </c>
       <c r="D13" s="29">
-        <v>4309237</v>
+        <v>6776307</v>
       </c>
       <c r="E13" s="29">
-        <v>6776307</v>
+        <v>4722286</v>
       </c>
       <c r="F13" s="29">
-        <v>4722286</v>
-      </c>
-      <c r="G13" s="29">
         <v>3366750</v>
       </c>
-      <c r="H13" s="30">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>19174580</v>
       </c>
+      <c r="H13" s="30">
+        <f>(B13 + stillbirth*B13/(1000-stillbirth))/(1-abortion)</f>
+        <v>3092255.0181537713</v>
+      </c>
       <c r="I13" s="30">
         <f t="shared" si="2"/>
-        <v>3092255.0181537713</v>
-      </c>
-      <c r="J13" s="30">
-        <f t="shared" si="3"/>
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7629,34 +7638,31 @@
         <v>2690000</v>
       </c>
       <c r="C14" s="29">
-        <v>12584924</v>
+        <v>4430738</v>
       </c>
       <c r="D14" s="29">
-        <v>4430738</v>
+        <v>7008703</v>
       </c>
       <c r="E14" s="29">
-        <v>7008703</v>
+        <v>4856898</v>
       </c>
       <c r="F14" s="29">
-        <v>4856898</v>
-      </c>
-      <c r="G14" s="29">
         <v>3479917</v>
       </c>
-      <c r="H14" s="30">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>19776256</v>
       </c>
+      <c r="H14" s="30">
+        <f>(B14 + stillbirth*B14/(1000-stillbirth))/(1-abortion)</f>
+        <v>3162800.7600127924</v>
+      </c>
       <c r="I14" s="30">
         <f t="shared" si="2"/>
-        <v>3162800.7600127924</v>
-      </c>
-      <c r="J14" s="30">
-        <f t="shared" si="3"/>
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7665,34 +7671,31 @@
         <v>2740000</v>
       </c>
       <c r="C15" s="29">
-        <v>12839335</v>
+        <v>4546624</v>
       </c>
       <c r="D15" s="29">
-        <v>4546624</v>
+        <v>7239465</v>
       </c>
       <c r="E15" s="29">
-        <v>7239465</v>
+        <v>5005361</v>
       </c>
       <c r="F15" s="29">
-        <v>5005361</v>
-      </c>
-      <c r="G15" s="29">
         <v>3595278</v>
       </c>
-      <c r="H15" s="30">
+      <c r="G15" s="30">
         <f t="shared" si="0"/>
         <v>20386728</v>
       </c>
+      <c r="H15" s="30">
+        <f>(B15 + stillbirth*B15/(1000-stillbirth))/(1-abortion)</f>
+        <v>3221588.8782286434</v>
+      </c>
       <c r="I15" s="30">
         <f t="shared" si="2"/>
-        <v>3221588.8782286434</v>
-      </c>
-      <c r="J15" s="30">
-        <f t="shared" si="3"/>
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7702,21 +7705,20 @@
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="G16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H16" s="30">
-        <f t="shared" si="0"/>
+        <f>(B16 + stillbirth*B16/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I16" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="30">
-        <f t="shared" ref="J16:J40" si="4">H16-I16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I16:I40" si="3">G16-H16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7726,21 +7728,20 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H17" s="30">
-        <f t="shared" si="0"/>
+        <f>(B17 + stillbirth*B17/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I17" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7750,21 +7751,20 @@
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="G18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H18" s="30">
-        <f t="shared" si="0"/>
+        <f>(B18 + stillbirth*B18/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I18" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7774,21 +7774,20 @@
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="G19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H19" s="30">
-        <f t="shared" si="0"/>
+        <f>(B19 + stillbirth*B19/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I19" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7798,21 +7797,20 @@
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
+      <c r="G20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H20" s="30">
-        <f t="shared" si="0"/>
+        <f>(B20 + stillbirth*B20/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I20" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7822,21 +7820,20 @@
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="G21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H21" s="30">
-        <f t="shared" si="0"/>
+        <f>(B21 + stillbirth*B21/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I21" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7846,21 +7843,20 @@
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H22" s="30">
-        <f t="shared" si="0"/>
+        <f>(B22 + stillbirth*B22/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I22" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7870,21 +7866,20 @@
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="G23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H23" s="30">
-        <f t="shared" si="0"/>
+        <f>(B23 + stillbirth*B23/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I23" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7894,21 +7889,20 @@
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
+      <c r="G24" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H24" s="30">
-        <f t="shared" si="0"/>
+        <f>(B24 + stillbirth*B24/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I24" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7918,21 +7912,20 @@
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="G25" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H25" s="30">
-        <f t="shared" si="0"/>
+        <f>(B25 + stillbirth*B25/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I25" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7942,21 +7935,20 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
+      <c r="G26" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H26" s="30">
-        <f t="shared" si="0"/>
+        <f>(B26 + stillbirth*B26/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I26" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7966,21 +7958,20 @@
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="G27" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H27" s="30">
-        <f t="shared" si="0"/>
+        <f>(B27 + stillbirth*B27/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I27" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7990,21 +7981,20 @@
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="G28" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H28" s="30">
-        <f t="shared" si="0"/>
+        <f>(B28 + stillbirth*B28/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I28" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8014,21 +8004,20 @@
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+      <c r="G29" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H29" s="30">
-        <f t="shared" si="0"/>
+        <f>(B29 + stillbirth*B29/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I29" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8038,21 +8027,20 @@
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
+      <c r="G30" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H30" s="30">
-        <f t="shared" si="0"/>
+        <f>(B30 + stillbirth*B30/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I30" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8062,21 +8050,20 @@
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="G31" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H31" s="30">
-        <f t="shared" si="0"/>
+        <f>(B31 + stillbirth*B31/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I31" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8086,21 +8073,20 @@
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+      <c r="G32" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H32" s="30">
-        <f t="shared" si="0"/>
+        <f>(B32 + stillbirth*B32/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I32" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8110,21 +8096,20 @@
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
+      <c r="G33" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H33" s="30">
-        <f t="shared" si="0"/>
+        <f>(B33 + stillbirth*B33/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I33" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8134,21 +8119,20 @@
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
+      <c r="G34" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H34" s="30">
-        <f t="shared" si="0"/>
+        <f>(B34 + stillbirth*B34/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I34" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8158,21 +8142,20 @@
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
+      <c r="G35" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H35" s="30">
-        <f t="shared" si="0"/>
+        <f>(B35 + stillbirth*B35/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I35" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8182,21 +8165,20 @@
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
+      <c r="G36" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H36" s="30">
-        <f t="shared" si="0"/>
+        <f>(B36 + stillbirth*B36/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I36" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8206,21 +8188,20 @@
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
       <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="G37" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H37" s="30">
-        <f t="shared" si="0"/>
+        <f>(B37 + stillbirth*B37/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I37" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8230,21 +8211,20 @@
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="G38" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H38" s="30">
-        <f t="shared" si="0"/>
+        <f>(B38 + stillbirth*B38/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I38" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8254,21 +8234,20 @@
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="G39" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H39" s="30">
-        <f t="shared" si="0"/>
+        <f>(B39 + stillbirth*B39/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I39" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8278,22 +8257,21 @@
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
+      <c r="G40" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H40" s="30">
-        <f t="shared" si="0"/>
+        <f>(B40 + stillbirth*B40/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I40" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:J40">
+  <conditionalFormatting sqref="B2:I40">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
     </cfRule>
@@ -8311,7 +8289,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8957,7 +8935,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8992,10 +8970,10 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9021,7 +8999,7 @@
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
@@ -9047,7 +9025,7 @@
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="39">
         <v>8.7000000000000008E-2</v>
@@ -9068,7 +9046,7 @@
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="39">
         <v>4.5999999999999999E-2</v>
@@ -9104,10 +9082,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9132,7 +9110,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
@@ -9157,7 +9135,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="39">
         <v>5.3999999999999999E-2</v>
@@ -9177,7 +9155,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="39">
         <v>0.04</v>
@@ -9255,7 +9233,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" s="47">
         <v>0.1</v>
@@ -9421,7 +9399,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="39">
         <v>0.84</v>
@@ -9441,7 +9419,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="39">
         <v>9.1999999999999998E-2</v>
@@ -9461,7 +9439,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="39">
         <v>5.8000000000000003E-2</v>
@@ -9481,7 +9459,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="46">
         <f>1-SUM(C2:C4)</f>
@@ -9528,10 +9506,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9563,10 +9541,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9583,10 +9561,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9603,10 +9581,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9634,7 +9612,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9648,10 +9626,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9665,7 +9643,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9682,7 +9660,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9696,7 +9674,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9722,7 +9700,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9735,24 +9713,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="64" t="s">
         <v>32</v>
@@ -9769,8 +9747,8 @@
       <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>195</v>
+      <c r="C3" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="81" t="str">
@@ -9783,8 +9761,8 @@
       <c r="B4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>195</v>
+      <c r="C4" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="81" t="str">
@@ -9797,8 +9775,8 @@
       <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>195</v>
+      <c r="C5" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="81" t="str">
@@ -9811,8 +9789,8 @@
       <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>195</v>
+      <c r="C6" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="81" t="str">
@@ -9823,7 +9801,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="62"/>
@@ -9831,14 +9809,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="66"/>
-      <c r="D9" s="66" t="s">
-        <v>195</v>
+      <c r="D9" s="66" t="b">
+        <v>0</v>
       </c>
       <c r="E9" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9896,7 +9874,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C14" s="63"/>
       <c r="D14" s="62"/>
@@ -9904,14 +9882,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="66"/>
       <c r="D16" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9925,7 +9903,7 @@
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9939,7 +9917,7 @@
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9953,7 +9931,7 @@
       </c>
       <c r="C19" s="66"/>
       <c r="D19" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9967,7 +9945,7 @@
       </c>
       <c r="C20" s="66"/>
       <c r="D20" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9977,7 +9955,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="62"/>
@@ -10010,16 +9988,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="85" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="86" t="s">
-        <v>183</v>
-      </c>
       <c r="D1" s="86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -10030,19 +10008,19 @@
         <v>67</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="66"/>
     </row>
@@ -10081,13 +10059,13 @@
         <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10104,7 +10082,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10121,7 +10099,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10138,12 +10116,12 @@
         <v>90</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="71">
         <v>0</v>
@@ -10155,12 +10133,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="71">
         <v>0</v>
@@ -10172,7 +10150,7 @@
         <v>0.82</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10189,7 +10167,7 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10206,7 +10184,7 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10223,12 +10201,12 @@
         <v>0.19</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="84" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -10240,12 +10218,12 @@
         <v>0.73</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -10257,12 +10235,12 @@
         <v>1.78</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -10274,12 +10252,12 @@
         <v>0.24</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="71">
         <v>0</v>
@@ -10291,12 +10269,12 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="71">
         <v>0</v>
@@ -10308,12 +10286,12 @@
         <v>0.73</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="71">
         <v>0</v>
@@ -10325,7 +10303,7 @@
         <v>1.78</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10342,7 +10320,7 @@
         <v>2.06</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10359,12 +10337,12 @@
         <v>0.05</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" s="71">
         <v>0</v>
@@ -10377,12 +10355,12 @@
         <v>3.66</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B19" s="71">
         <v>0</v>
@@ -10395,12 +10373,12 @@
         <v>3.78</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="71">
         <v>0</v>
@@ -10413,12 +10391,12 @@
         <v>14.270000000000001</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" s="71">
         <v>0</v>
@@ -10430,12 +10408,12 @@
         <v>8.84</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="71">
         <v>0</v>
@@ -10447,7 +10425,7 @@
         <v>50</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10464,7 +10442,7 @@
         <v>2.61</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10481,7 +10459,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10498,12 +10476,12 @@
         <v>1</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" s="71">
         <v>0.1</v>
@@ -10515,7 +10493,7 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10532,7 +10510,7 @@
         <v>3.78</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10549,7 +10527,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10566,7 +10544,7 @@
         <v>48</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10583,7 +10561,7 @@
         <v>5.3</v>
       </c>
       <c r="E30" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10600,7 +10578,7 @@
         <v>0.41</v>
       </c>
       <c r="E31" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10617,7 +10595,7 @@
         <v>0.9</v>
       </c>
       <c r="E32" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10634,7 +10612,7 @@
         <v>0.9</v>
       </c>
       <c r="E33" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10651,7 +10629,7 @@
         <v>79</v>
       </c>
       <c r="E34" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10668,7 +10646,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10685,7 +10663,7 @@
         <v>102</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F36" s="53"/>
     </row>
@@ -10703,7 +10681,7 @@
         <v>5.53</v>
       </c>
       <c r="E37" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10720,7 +10698,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Set max cov Fam plan
</commit_message>
<xml_diff>
--- a/applications/demo/data/national/demo_input.xlsx
+++ b/applications/demo/data/national/demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05CFEDD8-7BE8-7247-972E-0A21069AAE0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99BDCD51-4C4B-F64C-A6D1-64A2D6F36993}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="IYCF cost" sheetId="57" r:id="rId10"/>
     <sheet name="Program dependencies" sheetId="58" r:id="rId11"/>
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
-    <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
+    <sheet name="Incidence of conditions" sheetId="7" state="hidden" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
     <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
     <sheet name="Programs family planning" sheetId="54" r:id="rId16"/>
@@ -4344,8 +4344,8 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5124,7 +5124,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5237,8 +5237,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6231,16 +6231,20 @@
         <v>0</v>
       </c>
       <c r="L23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="M23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="N23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="O23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>